<commit_message>
RotS-Resources: Vale Exits updated.
</commit_message>
<xml_diff>
--- a/Vale Exits.xlsx
+++ b/Vale Exits.xlsx
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,11 +1660,11 @@
         <v>74</v>
       </c>
       <c r="F2" t="str">
-        <f>CONCATENATE(A2,"%0Exits are: ",C2)</f>
+        <f t="shared" ref="F2:F33" si="0">CONCATENATE(A2,"%0Exits are: ",C2)</f>
         <v>A Bald Boulder%0Exits are: N E</v>
       </c>
       <c r="G2" t="str">
-        <f>CONCATENATE(A2, " -  Room Exits: ", C2, "  Front: ", IF(D2="", "None", D2), "  Back: ", IF(E2="", "None", E2))</f>
+        <f t="shared" ref="G2:G33" si="1">CONCATENATE(A2, " -  Room Exits: ", C2, "  Front: ", IF(D2="", "None", D2), "  Back: ", IF(E2="", "None", E2))</f>
         <v>A Bald Boulder -  Room Exits: N E  Front: ensesw  Back: None</v>
       </c>
       <c r="H2" t="str">
@@ -1672,7 +1672,7 @@
         <v>#sub {A Bald Boulder%0Exits are: N E} {A Bald Boulder -  Room Exits: N E  Front: ensesw  Back: None}</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A2,"} {%0 %1- ",G2, "}")</f>
+        <f t="shared" ref="I2:I33" si="2">CONCATENATE("#sub {%0 %1- ",A2,"} {%0 %1- ",G2, "}")</f>
         <v>#sub {%0 %1- A Bald Boulder} {%0 %1- A Bald Boulder -  Room Exits: N E  Front: ensesw  Back: None}</v>
       </c>
     </row>
@@ -1693,11 +1693,11 @@
         <v>165</v>
       </c>
       <c r="F3" t="str">
-        <f>CONCATENATE(A3,"%0Exits are: ",C3)</f>
+        <f t="shared" si="0"/>
         <v>A Break in the Forest%0Exits are: N E S</v>
       </c>
       <c r="G3" t="str">
-        <f>CONCATENATE(A3, " -  Room Exits: ", C3, "  Front: ", IF(D3="", "None", D3), "  Back: ", IF(E3="", "None", E3))</f>
+        <f t="shared" si="1"/>
         <v>A Break in the Forest -  Room Exits: N E S  Front: nnnnww  Back: e</v>
       </c>
       <c r="H3" t="str">
@@ -1705,7 +1705,7 @@
         <v>#sub {A Break in the Forest%0Exits are: N E S} {A Break in the Forest -  Room Exits: N E S  Front: nnnnww  Back: e}</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A3,"} {%0 %1- ",G3, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Break in the Forest} {%0 %1- A Break in the Forest -  Room Exits: N E S  Front: nnnnww  Back: e}</v>
       </c>
     </row>
@@ -1723,11 +1723,11 @@
         <v>330</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE(A4,"%0Exits are: ",C4)</f>
+        <f t="shared" si="0"/>
         <v>A Busy Place%0Exits are: N E</v>
       </c>
       <c r="G4" t="str">
-        <f>CONCATENATE(A4, " -  Room Exits: ", C4, "  Front: ", IF(D4="", "None", D4), "  Back: ", IF(E4="", "None", E4))</f>
+        <f t="shared" si="1"/>
         <v>A Busy Place -  Room Exits: N E  Front: new  Back: None</v>
       </c>
       <c r="H4" t="str">
@@ -1735,7 +1735,7 @@
         <v>#sub {A Busy Place%0Exits are: N E} {A Busy Place -  Room Exits: N E  Front: new  Back: None}</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A4,"} {%0 %1- ",G4, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Busy Place} {%0 %1- A Busy Place -  Room Exits: N E  Front: new  Back: None}</v>
       </c>
     </row>
@@ -1756,11 +1756,11 @@
         <v>391</v>
       </c>
       <c r="F5" t="str">
-        <f>CONCATENATE(A5,"%0Exits are: ",C5)</f>
+        <f t="shared" si="0"/>
         <v>A Creepy Thicket%0Exits are: N E W</v>
       </c>
       <c r="G5" t="str">
-        <f>CONCATENATE(A5, " -  Room Exits: ", C5, "  Front: ", IF(D5="", "None", D5), "  Back: ", IF(E5="", "None", E5))</f>
+        <f t="shared" si="1"/>
         <v>A Creepy Thicket -  Room Exits: N E W  Front: wsssnesw  Back: nnesew</v>
       </c>
       <c r="H5" t="str">
@@ -1768,7 +1768,7 @@
         <v>#sub {A Creepy Thicket%0Exits are: N E W} {A Creepy Thicket -  Room Exits: N E W  Front: wsssnesw  Back: nnesew}</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A5,"} {%0 %1- ",G5, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Creepy Thicket} {%0 %1- A Creepy Thicket -  Room Exits: N E W  Front: wsssnesw  Back: nnesew}</v>
       </c>
     </row>
@@ -1786,15 +1786,19 @@
         <v>415</v>
       </c>
       <c r="F6" t="str">
-        <f>CONCATENATE(A6,"%0Exits are: ",C6)</f>
+        <f t="shared" si="0"/>
         <v>A Dark Copse%0Exits are: E W</v>
       </c>
       <c r="G6" t="str">
-        <f>CONCATENATE(A6, " -  Room Exits: ", C6, "  Front: ", IF(D6="", "None", D6), "  Back: ", IF(E6="", "None", E6))</f>
+        <f t="shared" si="1"/>
         <v>A Dark Copse -  Room Exits: E W  Front: wnnw  Back: None</v>
       </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H23" si="3">CONCATENATE("#sub {", F6, "} {", G6, "}")</f>
+        <v>#sub {A Dark Copse%0Exits are: E W} {A Dark Copse -  Room Exits: E W  Front: wnnw  Back: None}</v>
+      </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A6,"} {%0 %1- ",G6, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Dark Copse} {%0 %1- A Dark Copse -  Room Exits: E W  Front: wnnw  Back: None}</v>
       </c>
     </row>
@@ -1812,19 +1816,19 @@
         <v>233</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE(A7,"%0Exits are: ",C7)</f>
+        <f t="shared" si="0"/>
         <v>A Dark Track%0Exits are: N W</v>
       </c>
       <c r="G7" t="str">
-        <f>CONCATENATE(A7, " -  Room Exits: ", C7, "  Front: ", IF(D7="", "None", D7), "  Back: ", IF(E7="", "None", E7))</f>
+        <f t="shared" si="1"/>
         <v>A Dark Track -  Room Exits: N W  Front: wnesew  Back: None</v>
       </c>
       <c r="H7" t="str">
-        <f>CONCATENATE("#sub {", F7, "} {", G7, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Dark Track%0Exits are: N W} {A Dark Track -  Room Exits: N W  Front: wnesew  Back: None}</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A7,"} {%0 %1- ",G7, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Dark Track} {%0 %1- A Dark Track -  Room Exits: N W  Front: wnesew  Back: None}</v>
       </c>
     </row>
@@ -1842,19 +1846,19 @@
         <v>342</v>
       </c>
       <c r="F8" t="str">
-        <f>CONCATENATE(A8,"%0Exits are: ",C8)</f>
+        <f t="shared" si="0"/>
         <v>A Deep Depression%0Exits are: N W</v>
       </c>
       <c r="G8" t="str">
-        <f>CONCATENATE(A8, " -  Room Exits: ", C8, "  Front: ", IF(D8="", "None", D8), "  Back: ", IF(E8="", "None", E8))</f>
+        <f t="shared" si="1"/>
         <v>A Deep Depression -  Room Exits: N W  Front: wwewenw  Back: None</v>
       </c>
       <c r="H8" t="str">
-        <f>CONCATENATE("#sub {", F8, "} {", G8, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Deep Depression%0Exits are: N W} {A Deep Depression -  Room Exits: N W  Front: wwewenw  Back: None}</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A8,"} {%0 %1- ",G8, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Deep Depression} {%0 %1- A Deep Depression -  Room Exits: N W  Front: wwewenw  Back: None}</v>
       </c>
     </row>
@@ -1872,19 +1876,19 @@
         <v>188</v>
       </c>
       <c r="F9" t="str">
-        <f>CONCATENATE(A9,"%0Exits are: ",C9)</f>
+        <f t="shared" si="0"/>
         <v>A Gruesome Scene%0Exits are: N S</v>
       </c>
       <c r="G9" t="str">
-        <f>CONCATENATE(A9, " -  Room Exits: ", C9, "  Front: ", IF(D9="", "None", D9), "  Back: ", IF(E9="", "None", E9))</f>
+        <f t="shared" si="1"/>
         <v>A Gruesome Scene -  Room Exits: N S  Front: sesnnww  Back: None</v>
       </c>
       <c r="H9" t="str">
-        <f>CONCATENATE("#sub {", F9, "} {", G9, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Gruesome Scene%0Exits are: N S} {A Gruesome Scene -  Room Exits: N S  Front: sesnnww  Back: None}</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A9,"} {%0 %1- ",G9, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Gruesome Scene} {%0 %1- A Gruesome Scene -  Room Exits: N S  Front: sesnnww  Back: None}</v>
       </c>
     </row>
@@ -1902,19 +1906,19 @@
         <v>93</v>
       </c>
       <c r="F10" t="str">
-        <f>CONCATENATE(A10,"%0Exits are: ",C10)</f>
+        <f t="shared" si="0"/>
         <v>A Large Depression%0Exits are: S W</v>
       </c>
       <c r="G10" t="str">
-        <f>CONCATENATE(A10, " -  Room Exits: ", C10, "  Front: ", IF(D10="", "None", D10), "  Back: ", IF(E10="", "None", E10))</f>
+        <f t="shared" si="1"/>
         <v>A Large Depression -  Room Exits: S W  Front: sesw  Back: None</v>
       </c>
       <c r="H10" t="str">
-        <f>CONCATENATE("#sub {", F10, "} {", G10, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Large Depression%0Exits are: S W} {A Large Depression -  Room Exits: S W  Front: sesw  Back: None}</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A10,"} {%0 %1- ",G10, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Large Depression} {%0 %1- A Large Depression -  Room Exits: S W  Front: sesw  Back: None}</v>
       </c>
     </row>
@@ -1932,19 +1936,19 @@
         <v>80</v>
       </c>
       <c r="F11" t="str">
-        <f>CONCATENATE(A11,"%0Exits are: ",C11)</f>
+        <f t="shared" si="0"/>
         <v>A Musty Smell%0Exits are: N E</v>
       </c>
       <c r="G11" t="str">
-        <f>CONCATENATE(A11, " -  Room Exits: ", C11, "  Front: ", IF(D11="", "None", D11), "  Back: ", IF(E11="", "None", E11))</f>
+        <f t="shared" si="1"/>
         <v>A Musty Smell -  Room Exits: N E  Front: nwssw  Back: None</v>
       </c>
       <c r="H11" t="str">
-        <f>CONCATENATE("#sub {", F11, "} {", G11, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Musty Smell%0Exits are: N E} {A Musty Smell -  Room Exits: N E  Front: nwssw  Back: None}</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A11,"} {%0 %1- ",G11, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Musty Smell} {%0 %1- A Musty Smell -  Room Exits: N E  Front: nwssw  Back: None}</v>
       </c>
     </row>
@@ -1962,19 +1966,19 @@
         <v>202</v>
       </c>
       <c r="F12" t="str">
-        <f>CONCATENATE(A12,"%0Exits are: ",C12)</f>
+        <f t="shared" si="0"/>
         <v>A Narrow Run%0Exits are: E S</v>
       </c>
       <c r="G12" t="str">
-        <f>CONCATENATE(A12, " -  Room Exits: ", C12, "  Front: ", IF(D12="", "None", D12), "  Back: ", IF(E12="", "None", E12))</f>
+        <f t="shared" si="1"/>
         <v>A Narrow Run -  Room Exits: E S  Front: ewnesew  Back: None</v>
       </c>
       <c r="H12" t="str">
-        <f>CONCATENATE("#sub {", F12, "} {", G12, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Narrow Run%0Exits are: E S} {A Narrow Run -  Room Exits: E S  Front: ewnesew  Back: None}</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A12,"} {%0 %1- ",G12, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Narrow Run} {%0 %1- A Narrow Run -  Room Exits: E S  Front: ewnesew  Back: None}</v>
       </c>
     </row>
@@ -1992,19 +1996,19 @@
         <v>340</v>
       </c>
       <c r="F13" t="str">
-        <f>CONCATENATE(A13,"%0Exits are: ",C13)</f>
+        <f t="shared" si="0"/>
         <v>A Rocky Outcrop%0Exits are: E S</v>
       </c>
       <c r="G13" t="str">
-        <f>CONCATENATE(A13, " -  Room Exits: ", C13, "  Front: ", IF(D13="", "None", D13), "  Back: ", IF(E13="", "None", E13))</f>
+        <f t="shared" si="1"/>
         <v>A Rocky Outcrop -  Room Exits: E S  Front: enwsnww  Back: None</v>
       </c>
       <c r="H13" t="str">
-        <f>CONCATENATE("#sub {", F13, "} {", G13, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Rocky Outcrop%0Exits are: E S} {A Rocky Outcrop -  Room Exits: E S  Front: enwsnww  Back: None}</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A13,"} {%0 %1- ",G13, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Rocky Outcrop} {%0 %1- A Rocky Outcrop -  Room Exits: E S  Front: enwsnww  Back: None}</v>
       </c>
     </row>
@@ -2022,19 +2026,19 @@
         <v>299</v>
       </c>
       <c r="F14" t="str">
-        <f>CONCATENATE(A14,"%0Exits are: ",C14)</f>
+        <f t="shared" si="0"/>
         <v>A Rotting Windfall%0Exits are: N S W</v>
       </c>
       <c r="G14" t="str">
-        <f>CONCATENATE(A14, " -  Room Exits: ", C14, "  Front: ", IF(D14="", "None", D14), "  Back: ", IF(E14="", "None", E14))</f>
+        <f t="shared" si="1"/>
         <v>A Rotting Windfall -  Room Exits: N S W  Front: wsnnnw  Back: None</v>
       </c>
       <c r="H14" t="str">
-        <f>CONCATENATE("#sub {", F14, "} {", G14, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Rotting Windfall%0Exits are: N S W} {A Rotting Windfall -  Room Exits: N S W  Front: wsnnnw  Back: None}</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A14,"} {%0 %1- ",G14, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Rotting Windfall} {%0 %1- A Rotting Windfall -  Room Exits: N S W  Front: wsnnnw  Back: None}</v>
       </c>
     </row>
@@ -2052,19 +2056,19 @@
         <v>289</v>
       </c>
       <c r="F15" t="str">
-        <f>CONCATENATE(A15,"%0Exits are: ",C15)</f>
+        <f t="shared" si="0"/>
         <v>A Small Clearing%0Exits are: N E</v>
       </c>
       <c r="G15" t="str">
-        <f>CONCATENATE(A15, " -  Room Exits: ", C15, "  Front: ", IF(D15="", "None", D15), "  Back: ", IF(E15="", "None", E15))</f>
+        <f t="shared" si="1"/>
         <v>A Small Clearing -  Room Exits: N E  Front: nssnnnww  Back: None</v>
       </c>
       <c r="H15" t="str">
-        <f>CONCATENATE("#sub {", F15, "} {", G15, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Small Clearing%0Exits are: N E} {A Small Clearing -  Room Exits: N E  Front: nssnnnww  Back: None}</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A15,"} {%0 %1- ",G15, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Small Clearing} {%0 %1- A Small Clearing -  Room Exits: N E  Front: nssnnnww  Back: None}</v>
       </c>
     </row>
@@ -2082,19 +2086,19 @@
         <v>282</v>
       </c>
       <c r="F16" t="str">
-        <f>CONCATENATE(A16,"%0Exits are: ",C16)</f>
+        <f t="shared" si="0"/>
         <v>A Small Knoll%0Exits are: N S</v>
       </c>
       <c r="G16" t="str">
-        <f>CONCATENATE(A16, " -  Room Exits: ", C16, "  Front: ", IF(D16="", "None", D16), "  Back: ", IF(E16="", "None", E16))</f>
+        <f t="shared" si="1"/>
         <v>A Small Knoll -  Room Exits: N S  Front: nsenenw  Back: None</v>
       </c>
       <c r="H16" t="str">
-        <f>CONCATENATE("#sub {", F16, "} {", G16, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Small Knoll%0Exits are: N S} {A Small Knoll -  Room Exits: N S  Front: nsenenw  Back: None}</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A16,"} {%0 %1- ",G16, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Small Knoll} {%0 %1- A Small Knoll -  Room Exits: N S  Front: nsenenw  Back: None}</v>
       </c>
     </row>
@@ -2112,19 +2116,19 @@
         <v>11</v>
       </c>
       <c r="F17" t="str">
-        <f>CONCATENATE(A17,"%0Exits are: ",C17)</f>
+        <f t="shared" si="0"/>
         <v>A Small Spring%0Exits are: N E</v>
       </c>
       <c r="G17" t="str">
-        <f>CONCATENATE(A17, " -  Room Exits: ", C17, "  Front: ", IF(D17="", "None", D17), "  Back: ", IF(E17="", "None", E17))</f>
+        <f t="shared" si="1"/>
         <v>A Small Spring -  Room Exits: N E  Front: nnnw  Back: None</v>
       </c>
       <c r="H17" t="str">
-        <f>CONCATENATE("#sub {", F17, "} {", G17, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Small Spring%0Exits are: N E} {A Small Spring -  Room Exits: N E  Front: nnnw  Back: None}</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A17,"} {%0 %1- ",G17, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Small Spring} {%0 %1- A Small Spring -  Room Exits: N E  Front: nnnw  Back: None}</v>
       </c>
     </row>
@@ -2142,19 +2146,19 @@
         <v>314</v>
       </c>
       <c r="F18" t="str">
-        <f>CONCATENATE(A18,"%0Exits are: ",C18)</f>
+        <f t="shared" si="0"/>
         <v>A Stagnant Odor%0Exits are: N S</v>
       </c>
       <c r="G18" t="str">
-        <f>CONCATENATE(A18, " -  Room Exits: ", C18, "  Front: ", IF(D18="", "None", D18), "  Back: ", IF(E18="", "None", E18))</f>
+        <f t="shared" si="1"/>
         <v>A Stagnant Odor -  Room Exits: N S  Front: nsnsnww  Back: None</v>
       </c>
       <c r="H18" t="str">
-        <f>CONCATENATE("#sub {", F18, "} {", G18, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Stagnant Odor%0Exits are: N S} {A Stagnant Odor -  Room Exits: N S  Front: nsnsnww  Back: None}</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A18,"} {%0 %1- ",G18, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Stagnant Odor} {%0 %1- A Stagnant Odor -  Room Exits: N S  Front: nsnsnww  Back: None}</v>
       </c>
     </row>
@@ -2172,19 +2176,19 @@
         <v>412</v>
       </c>
       <c r="F19" t="str">
-        <f>CONCATENATE(A19,"%0Exits are: ",C19)</f>
+        <f t="shared" si="0"/>
         <v>A Strange Barrow%0Exits are: N W</v>
       </c>
       <c r="G19" t="str">
-        <f>CONCATENATE(A19, " -  Room Exits: ", C19, "  Front: ", IF(D19="", "None", D19), "  Back: ", IF(E19="", "None", E19))</f>
+        <f t="shared" si="1"/>
         <v>A Strange Barrow -  Room Exits: N W  Front: nwwwww  Back: None</v>
       </c>
       <c r="H19" t="str">
-        <f>CONCATENATE("#sub {", F19, "} {", G19, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Strange Barrow%0Exits are: N W} {A Strange Barrow -  Room Exits: N W  Front: nwwwww  Back: None}</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A19,"} {%0 %1- ",G19, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Strange Barrow} {%0 %1- A Strange Barrow -  Room Exits: N W  Front: nwwwww  Back: None}</v>
       </c>
     </row>
@@ -2202,19 +2206,19 @@
         <v>94</v>
       </c>
       <c r="F20" t="str">
-        <f>CONCATENATE(A20,"%0Exits are: ",C20)</f>
+        <f t="shared" si="0"/>
         <v>A Strange Vapour%0Exits are: N E S W</v>
       </c>
       <c r="G20" t="str">
-        <f>CONCATENATE(A20, " -  Room Exits: ", C20, "  Front: ", IF(D20="", "None", D20), "  Back: ", IF(E20="", "None", E20))</f>
+        <f t="shared" si="1"/>
         <v>A Strange Vapour -  Room Exits: N E S W  Front: esw  Back: None</v>
       </c>
       <c r="H20" t="str">
-        <f>CONCATENATE("#sub {", F20, "} {", G20, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Strange Vapour%0Exits are: N E S W} {A Strange Vapour -  Room Exits: N E S W  Front: esw  Back: None}</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A20,"} {%0 %1- ",G20, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Strange Vapour} {%0 %1- A Strange Vapour -  Room Exits: N E S W  Front: esw  Back: None}</v>
       </c>
     </row>
@@ -2232,19 +2236,19 @@
         <v>401</v>
       </c>
       <c r="F21" t="str">
-        <f>CONCATENATE(A21,"%0Exits are: ",C21)</f>
+        <f t="shared" si="0"/>
         <v>A Stray Boulder%0Exits are: E S W</v>
       </c>
       <c r="G21" t="str">
-        <f>CONCATENATE(A21, " -  Room Exits: ", C21, "  Front: ", IF(D21="", "None", D21), "  Back: ", IF(E21="", "None", E21))</f>
+        <f t="shared" si="1"/>
         <v>A Stray Boulder -  Room Exits: E S W  Front: sewnnsnnnww  Back: None</v>
       </c>
       <c r="H21" t="str">
-        <f>CONCATENATE("#sub {", F21, "} {", G21, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Stray Boulder%0Exits are: E S W} {A Stray Boulder -  Room Exits: E S W  Front: sewnnsnnnww  Back: None}</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A21,"} {%0 %1- ",G21, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Stray Boulder} {%0 %1- A Stray Boulder -  Room Exits: E S W  Front: sewnnsnnnww  Back: None}</v>
       </c>
     </row>
@@ -2265,19 +2269,19 @@
         <v>132</v>
       </c>
       <c r="F22" t="str">
-        <f>CONCATENATE(A22,"%0Exits are: ",C22)</f>
+        <f t="shared" si="0"/>
         <v>A Tragic Scene%0Exits are: N E S</v>
       </c>
       <c r="G22" t="str">
-        <f>CONCATENATE(A22, " -  Room Exits: ", C22, "  Front: ", IF(D22="", "None", D22), "  Back: ", IF(E22="", "None", E22))</f>
+        <f t="shared" si="1"/>
         <v>A Tragic Scene -  Room Exits: N E S  Front: ssnww  Back: eeneenesene</v>
       </c>
       <c r="H22" t="str">
-        <f>CONCATENATE("#sub {", F22, "} {", G22, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Tragic Scene%0Exits are: N E S} {A Tragic Scene -  Room Exits: N E S  Front: ssnww  Back: eeneenesene}</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A22,"} {%0 %1- ",G22, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Tragic Scene} {%0 %1- A Tragic Scene -  Room Exits: N E S  Front: ssnww  Back: eeneenesene}</v>
       </c>
     </row>
@@ -2295,19 +2299,19 @@
         <v>321</v>
       </c>
       <c r="F23" t="str">
-        <f>CONCATENATE(A23,"%0Exits are: ",C23)</f>
+        <f t="shared" si="0"/>
         <v>A Turn%0Exits are: E W</v>
       </c>
       <c r="G23" t="str">
-        <f>CONCATENATE(A23, " -  Room Exits: ", C23, "  Front: ", IF(D23="", "None", D23), "  Back: ", IF(E23="", "None", E23))</f>
+        <f t="shared" si="1"/>
         <v>A Turn -  Room Exits: E W  Front: wsesew  Back: None</v>
       </c>
       <c r="H23" t="str">
-        <f>CONCATENATE("#sub {", F23, "} {", G23, "}")</f>
+        <f t="shared" si="3"/>
         <v>#sub {A Turn%0Exits are: E W} {A Turn -  Room Exits: E W  Front: wsesew  Back: None}</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A23,"} {%0 %1- ",G23, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- A Turn} {%0 %1- A Turn -  Room Exits: E W  Front: wsesew  Back: None}</v>
       </c>
     </row>
@@ -2325,19 +2329,19 @@
         <v>348</v>
       </c>
       <c r="F24" t="str">
-        <f>CONCATENATE(A24,"%0Exits are: ",C24)</f>
+        <f t="shared" si="0"/>
         <v>Accursed Vale%0Exits are: N E</v>
       </c>
       <c r="G24" t="str">
-        <f>CONCATENATE(A24, " -  Room Exits: ", C24, "  Front: ", IF(D24="", "None", D24), "  Back: ", IF(E24="", "None", E24))</f>
+        <f t="shared" si="1"/>
         <v>Accursed Vale -  Room Exits: N E  Front: nwsew  Back: None</v>
       </c>
       <c r="H24" t="str">
-        <f>CONCATENATE("#sub {", F24, "} {", G24, "}")</f>
+        <f t="shared" ref="H7:H38" si="4">CONCATENATE("#sub {", F24, "} {", G24, "}")</f>
         <v>#sub {Accursed Vale%0Exits are: N E} {Accursed Vale -  Room Exits: N E  Front: nwsew  Back: None}</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A24,"} {%0 %1- ",G24, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Accursed Vale} {%0 %1- Accursed Vale -  Room Exits: N E  Front: nwsew  Back: None}</v>
       </c>
     </row>
@@ -2355,19 +2359,19 @@
         <v>347</v>
       </c>
       <c r="F25" t="str">
-        <f>CONCATENATE(A25,"%0Exits are: ",C25)</f>
+        <f t="shared" si="0"/>
         <v>An Ancient Ossuary%0Exits are: E S W</v>
       </c>
       <c r="G25" t="str">
-        <f>CONCATENATE(A25, " -  Room Exits: ", C25, "  Front: ", IF(D25="", "None", D25), "  Back: ", IF(E25="", "None", E25))</f>
+        <f t="shared" si="1"/>
         <v>An Ancient Ossuary -  Room Exits: E S W  Front: wesnnww  Back: None</v>
       </c>
       <c r="H25" t="str">
-        <f>CONCATENATE("#sub {", F25, "} {", G25, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {An Ancient Ossuary%0Exits are: E S W} {An Ancient Ossuary -  Room Exits: E S W  Front: wesnnww  Back: None}</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A25,"} {%0 %1- ",G25, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- An Ancient Ossuary} {%0 %1- An Ancient Ossuary -  Room Exits: E S W  Front: wesnnww  Back: None}</v>
       </c>
     </row>
@@ -2385,19 +2389,19 @@
         <v>327</v>
       </c>
       <c r="F26" t="str">
-        <f>CONCATENATE(A26,"%0Exits are: ",C26)</f>
+        <f t="shared" si="0"/>
         <v>An Inverted Forest%0Exits are: S W</v>
       </c>
       <c r="G26" t="str">
-        <f>CONCATENATE(A26, " -  Room Exits: ", C26, "  Front: ", IF(D26="", "None", D26), "  Back: ", IF(E26="", "None", E26))</f>
+        <f t="shared" si="1"/>
         <v>An Inverted Forest -  Room Exits: S W  Front: wsew  Back: None</v>
       </c>
       <c r="H26" t="str">
-        <f>CONCATENATE("#sub {", F26, "} {", G26, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {An Inverted Forest%0Exits are: S W} {An Inverted Forest -  Room Exits: S W  Front: wsew  Back: None}</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A26,"} {%0 %1- ",G26, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- An Inverted Forest} {%0 %1- An Inverted Forest -  Room Exits: S W  Front: wsew  Back: None}</v>
       </c>
     </row>
@@ -2415,19 +2419,19 @@
         <v>230</v>
       </c>
       <c r="F27" t="str">
-        <f>CONCATENATE(A27,"%0Exits are: ",C27)</f>
+        <f t="shared" si="0"/>
         <v>An Old Camp%0Exits are: E S W</v>
       </c>
       <c r="G27" t="str">
-        <f>CONCATENATE(A27, " -  Room Exits: ", C27, "  Front: ", IF(D27="", "None", D27), "  Back: ", IF(E27="", "None", E27))</f>
+        <f t="shared" si="1"/>
         <v>An Old Camp -  Room Exits: E S W  Front: wwesew  Back: None</v>
       </c>
       <c r="H27" t="str">
-        <f>CONCATENATE("#sub {", F27, "} {", G27, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {An Old Camp%0Exits are: E S W} {An Old Camp -  Room Exits: E S W  Front: wwesew  Back: None}</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A27,"} {%0 %1- ",G27, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- An Old Camp} {%0 %1- An Old Camp -  Room Exits: E S W  Front: wwesew  Back: None}</v>
       </c>
     </row>
@@ -2448,19 +2452,19 @@
         <v>60</v>
       </c>
       <c r="F28" t="str">
-        <f>CONCATENATE(A28,"%0Exits are: ",C28)</f>
+        <f t="shared" si="0"/>
         <v>Another Dead End%0Exits are: E S W</v>
       </c>
       <c r="G28" t="str">
-        <f>CONCATENATE(A28, " -  Room Exits: ", C28, "  Front: ", IF(D28="", "None", D28), "  Back: ", IF(E28="", "None", E28))</f>
+        <f t="shared" si="1"/>
         <v>Another Dead End -  Room Exits: E S W  Front: sssnww  Back: seeneenesene</v>
       </c>
       <c r="H28" t="str">
-        <f>CONCATENATE("#sub {", F28, "} {", G28, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Another Dead End%0Exits are: E S W} {Another Dead End -  Room Exits: E S W  Front: sssnww  Back: seeneenesene}</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A28,"} {%0 %1- ",G28, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Another Dead End} {%0 %1- Another Dead End -  Room Exits: E S W  Front: sssnww  Back: seeneenesene}</v>
       </c>
     </row>
@@ -2478,19 +2482,19 @@
         <v>193</v>
       </c>
       <c r="F29" t="str">
-        <f>CONCATENATE(A29,"%0Exits are: ",C29)</f>
+        <f t="shared" si="0"/>
         <v>Ash Pit%0Exits are: N E S</v>
       </c>
       <c r="G29" t="str">
-        <f>CONCATENATE(A29, " -  Room Exits: ", C29, "  Front: ", IF(D29="", "None", D29), "  Back: ", IF(E29="", "None", E29))</f>
+        <f t="shared" si="1"/>
         <v>Ash Pit -  Room Exits: N E S  Front: nnw  Back: None</v>
       </c>
       <c r="H29" t="str">
-        <f>CONCATENATE("#sub {", F29, "} {", G29, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Ash Pit%0Exits are: N E S} {Ash Pit -  Room Exits: N E S  Front: nnw  Back: None}</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A29,"} {%0 %1- ",G29, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Ash Pit} {%0 %1- Ash Pit -  Room Exits: N E S  Front: nnw  Back: None}</v>
       </c>
     </row>
@@ -2508,19 +2512,19 @@
         <v>10</v>
       </c>
       <c r="F30" t="str">
-        <f>CONCATENATE(A30,"%0Exits are: ",C30)</f>
+        <f t="shared" si="0"/>
         <v>Baleful Darkness%0Exits are: E S</v>
       </c>
       <c r="G30" t="str">
-        <f>CONCATENATE(A30, " -  Room Exits: ", C30, "  Front: ", IF(D30="", "None", D30), "  Back: ", IF(E30="", "None", E30))</f>
+        <f t="shared" si="1"/>
         <v>Baleful Darkness -  Room Exits: E S  Front: ennnnww  Back: None</v>
       </c>
       <c r="H30" t="str">
-        <f>CONCATENATE("#sub {", F30, "} {", G30, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Baleful Darkness%0Exits are: E S} {Baleful Darkness -  Room Exits: E S  Front: ennnnww  Back: None}</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A30,"} {%0 %1- ",G30, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Baleful Darkness} {%0 %1- Baleful Darkness -  Room Exits: E S  Front: ennnnww  Back: None}</v>
       </c>
     </row>
@@ -2538,19 +2542,19 @@
         <v>397</v>
       </c>
       <c r="F31" t="str">
-        <f>CONCATENATE(A31,"%0Exits are: ",C31)</f>
+        <f t="shared" si="0"/>
         <v>Bearded Old Man%0Exits are: N E S</v>
       </c>
       <c r="G31" t="str">
-        <f>CONCATENATE(A31, " -  Room Exits: ", C31, "  Front: ", IF(D31="", "None", D31), "  Back: ", IF(E31="", "None", E31))</f>
+        <f t="shared" si="1"/>
         <v>Bearded Old Man -  Room Exits: N E S  Front: newnnewennw  Back: None</v>
       </c>
       <c r="H31" t="str">
-        <f>CONCATENATE("#sub {", F31, "} {", G31, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Bearded Old Man%0Exits are: N E S} {Bearded Old Man -  Room Exits: N E S  Front: newnnewennw  Back: None}</v>
       </c>
       <c r="I31" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A31,"} {%0 %1- ",G31, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Bearded Old Man} {%0 %1- Bearded Old Man -  Room Exits: N E S  Front: newnnewennw  Back: None}</v>
       </c>
     </row>
@@ -2568,19 +2572,19 @@
         <v>346</v>
       </c>
       <c r="F32" t="str">
-        <f>CONCATENATE(A32,"%0Exits are: ",C32)</f>
+        <f t="shared" si="0"/>
         <v>Black Ferns%0Exits are: N E</v>
       </c>
       <c r="G32" t="str">
-        <f>CONCATENATE(A32, " -  Room Exits: ", C32, "  Front: ", IF(D32="", "None", D32), "  Back: ", IF(E32="", "None", E32))</f>
+        <f t="shared" si="1"/>
         <v>Black Ferns -  Room Exits: N E  Front: ewwnnww  Back: None</v>
       </c>
       <c r="H32" t="str">
-        <f>CONCATENATE("#sub {", F32, "} {", G32, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Black Ferns%0Exits are: N E} {Black Ferns -  Room Exits: N E  Front: ewwnnww  Back: None}</v>
       </c>
       <c r="I32" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A32,"} {%0 %1- ",G32, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Black Ferns} {%0 %1- Black Ferns -  Room Exits: N E  Front: ewwnnww  Back: None}</v>
       </c>
     </row>
@@ -2598,19 +2602,19 @@
         <v>312</v>
       </c>
       <c r="F33" t="str">
-        <f>CONCATENATE(A33,"%0Exits are: ",C33)</f>
+        <f t="shared" si="0"/>
         <v>Black Vines%0Exits are: E S</v>
       </c>
       <c r="G33" t="str">
-        <f>CONCATENATE(A33, " -  Room Exits: ", C33, "  Front: ", IF(D33="", "None", D33), "  Back: ", IF(E33="", "None", E33))</f>
+        <f t="shared" si="1"/>
         <v>Black Vines -  Room Exits: E S  Front: nnsew  Back: None</v>
       </c>
       <c r="H33" t="str">
-        <f>CONCATENATE("#sub {", F33, "} {", G33, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Black Vines%0Exits are: E S} {Black Vines -  Room Exits: E S  Front: nnsew  Back: None}</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A33,"} {%0 %1- ",G33, "}")</f>
+        <f t="shared" si="2"/>
         <v>#sub {%0 %1- Black Vines} {%0 %1- Black Vines -  Room Exits: E S  Front: nnsew  Back: None}</v>
       </c>
     </row>
@@ -2628,19 +2632,19 @@
         <v>3</v>
       </c>
       <c r="F34" t="str">
-        <f>CONCATENATE(A34,"%0Exits are: ",C34)</f>
+        <f t="shared" ref="F34:F65" si="5">CONCATENATE(A34,"%0Exits are: ",C34)</f>
         <v>Black Wood%0Exits are: N E W</v>
       </c>
       <c r="G34" t="str">
-        <f>CONCATENATE(A34, " -  Room Exits: ", C34, "  Front: ", IF(D34="", "None", D34), "  Back: ", IF(E34="", "None", E34))</f>
+        <f t="shared" ref="G34:G65" si="6">CONCATENATE(A34, " -  Room Exits: ", C34, "  Front: ", IF(D34="", "None", D34), "  Back: ", IF(E34="", "None", E34))</f>
         <v>Black Wood -  Room Exits: N E W  Front: nwesew  Back: None</v>
       </c>
       <c r="H34" t="str">
-        <f>CONCATENATE("#sub {", F34, "} {", G34, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Black Wood%0Exits are: N E W} {Black Wood -  Room Exits: N E W  Front: nwesew  Back: None}</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A34,"} {%0 %1- ",G34, "}")</f>
+        <f t="shared" ref="I34:I65" si="7">CONCATENATE("#sub {%0 %1- ",A34,"} {%0 %1- ",G34, "}")</f>
         <v>#sub {%0 %1- Black Wood} {%0 %1- Black Wood -  Room Exits: N E W  Front: nwesew  Back: None}</v>
       </c>
     </row>
@@ -2658,19 +2662,19 @@
         <v>246</v>
       </c>
       <c r="F35" t="str">
-        <f>CONCATENATE(A35,"%0Exits are: ",C35)</f>
+        <f t="shared" si="5"/>
         <v>Bleeding Trees%0Exits are: S W</v>
       </c>
       <c r="G35" t="str">
-        <f>CONCATENATE(A35, " -  Room Exits: ", C35, "  Front: ", IF(D35="", "None", D35), "  Back: ", IF(E35="", "None", E35))</f>
+        <f t="shared" si="6"/>
         <v>Bleeding Trees -  Room Exits: S W  Front: sewenw  Back: None</v>
       </c>
       <c r="H35" t="str">
-        <f>CONCATENATE("#sub {", F35, "} {", G35, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Bleeding Trees%0Exits are: S W} {Bleeding Trees -  Room Exits: S W  Front: sewenw  Back: None}</v>
       </c>
       <c r="I35" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A35,"} {%0 %1- ",G35, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Bleeding Trees} {%0 %1- Bleeding Trees -  Room Exits: S W  Front: sewenw  Back: None}</v>
       </c>
     </row>
@@ -2688,19 +2692,19 @@
         <v>281</v>
       </c>
       <c r="F36" t="str">
-        <f>CONCATENATE(A36,"%0Exits are: ",C36)</f>
+        <f t="shared" si="5"/>
         <v>Bog of Darkness%0Exits are: N S W</v>
       </c>
       <c r="G36" t="str">
-        <f>CONCATENATE(A36, " -  Room Exits: ", C36, "  Front: ", IF(D36="", "None", D36), "  Back: ", IF(E36="", "None", E36))</f>
+        <f t="shared" si="6"/>
         <v>Bog of Darkness -  Room Exits: N S W  Front: wwesewenw  Back: None</v>
       </c>
       <c r="H36" t="str">
-        <f>CONCATENATE("#sub {", F36, "} {", G36, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Bog of Darkness%0Exits are: N S W} {Bog of Darkness -  Room Exits: N S W  Front: wwesewenw  Back: None}</v>
       </c>
       <c r="I36" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A36,"} {%0 %1- ",G36, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Bog of Darkness} {%0 %1- Bog of Darkness -  Room Exits: N S W  Front: wwesewenw  Back: None}</v>
       </c>
     </row>
@@ -2718,19 +2722,19 @@
         <v>379</v>
       </c>
       <c r="F37" t="str">
-        <f>CONCATENATE(A37,"%0Exits are: ",C37)</f>
+        <f t="shared" si="5"/>
         <v>Brackish Waters%0Exits are: S W</v>
       </c>
       <c r="G37" t="str">
-        <f>CONCATENATE(A37, " -  Room Exits: ", C37, "  Front: ", IF(D37="", "None", D37), "  Back: ", IF(E37="", "None", E37))</f>
+        <f t="shared" si="6"/>
         <v>Brackish Waters -  Room Exits: S W  Front: wnnsnnnww  Back: None</v>
       </c>
       <c r="H37" t="str">
-        <f>CONCATENATE("#sub {", F37, "} {", G37, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Brackish Waters%0Exits are: S W} {Brackish Waters -  Room Exits: S W  Front: wnnsnnnww  Back: None}</v>
       </c>
       <c r="I37" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A37,"} {%0 %1- ",G37, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Brackish Waters} {%0 %1- Brackish Waters -  Room Exits: S W  Front: wnnsnnnww  Back: None}</v>
       </c>
     </row>
@@ -2748,19 +2752,19 @@
         <v>5</v>
       </c>
       <c r="F38" t="str">
-        <f>CONCATENATE(A38,"%0Exits are: ",C38)</f>
+        <f t="shared" si="5"/>
         <v>Breathing Forest%0Exits are: E S</v>
       </c>
       <c r="G38" t="str">
-        <f>CONCATENATE(A38, " -  Room Exits: ", C38, "  Front: ", IF(D38="", "None", D38), "  Back: ", IF(E38="", "None", E38))</f>
+        <f t="shared" si="6"/>
         <v>Breathing Forest -  Room Exits: E S  Front: ssnennw  Back: None</v>
       </c>
       <c r="H38" t="str">
-        <f>CONCATENATE("#sub {", F38, "} {", G38, "}")</f>
+        <f t="shared" si="4"/>
         <v>#sub {Breathing Forest%0Exits are: E S} {Breathing Forest -  Room Exits: E S  Front: ssnennw  Back: None}</v>
       </c>
       <c r="I38" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A38,"} {%0 %1- ",G38, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Breathing Forest} {%0 %1- Breathing Forest -  Room Exits: E S  Front: ssnennw  Back: None}</v>
       </c>
     </row>
@@ -2778,19 +2782,19 @@
         <v>287</v>
       </c>
       <c r="F39" t="str">
-        <f>CONCATENATE(A39,"%0Exits are: ",C39)</f>
+        <f t="shared" si="5"/>
         <v>Broken Land%0Exits are: N S W</v>
       </c>
       <c r="G39" t="str">
-        <f>CONCATENATE(A39, " -  Room Exits: ", C39, "  Front: ", IF(D39="", "None", D39), "  Back: ", IF(E39="", "None", E39))</f>
+        <f t="shared" si="6"/>
         <v>Broken Land -  Room Exits: N S W  Front: snnnww  Back: None</v>
       </c>
       <c r="H39" t="str">
-        <f>CONCATENATE("#sub {", F39, "} {", G39, "}")</f>
+        <f t="shared" ref="H39:H70" si="8">CONCATENATE("#sub {", F39, "} {", G39, "}")</f>
         <v>#sub {Broken Land%0Exits are: N S W} {Broken Land -  Room Exits: N S W  Front: snnnww  Back: None}</v>
       </c>
       <c r="I39" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A39,"} {%0 %1- ",G39, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Broken Land} {%0 %1- Broken Land -  Room Exits: N S W  Front: snnnww  Back: None}</v>
       </c>
     </row>
@@ -2808,19 +2812,19 @@
         <v>110</v>
       </c>
       <c r="F40" t="str">
-        <f>CONCATENATE(A40,"%0Exits are: ",C40)</f>
+        <f t="shared" si="5"/>
         <v>Broken Rocks%0Exits are: N S W</v>
       </c>
       <c r="G40" t="str">
-        <f>CONCATENATE(A40, " -  Room Exits: ", C40, "  Front: ", IF(D40="", "None", D40), "  Back: ", IF(E40="", "None", E40))</f>
+        <f t="shared" si="6"/>
         <v>Broken Rocks -  Room Exits: N S W  Front: wesew  Back: None</v>
       </c>
       <c r="H40" t="str">
-        <f>CONCATENATE("#sub {", F40, "} {", G40, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Broken Rocks%0Exits are: N S W} {Broken Rocks -  Room Exits: N S W  Front: wesew  Back: None}</v>
       </c>
       <c r="I40" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A40,"} {%0 %1- ",G40, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Broken Rocks} {%0 %1- Broken Rocks -  Room Exits: N S W  Front: wesew  Back: None}</v>
       </c>
     </row>
@@ -2838,19 +2842,19 @@
         <v>129</v>
       </c>
       <c r="F41" t="str">
-        <f>CONCATENATE(A41,"%0Exits are: ",C41)</f>
+        <f t="shared" si="5"/>
         <v>Brothel of Trees%0Exits are: N E S W</v>
       </c>
       <c r="G41" t="str">
-        <f>CONCATENATE(A41, " -  Room Exits: ", C41, "  Front: ", IF(D41="", "None", D41), "  Back: ", IF(E41="", "None", E41))</f>
+        <f t="shared" si="6"/>
         <v>Brothel of Trees -  Room Exits: N E S W  Front: nnww  Back: None</v>
       </c>
       <c r="H41" t="str">
-        <f>CONCATENATE("#sub {", F41, "} {", G41, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Brothel of Trees%0Exits are: N E S W} {Brothel of Trees -  Room Exits: N E S W  Front: nnww  Back: None}</v>
       </c>
       <c r="I41" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A41,"} {%0 %1- ",G41, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Brothel of Trees} {%0 %1- Brothel of Trees -  Room Exits: N E S W  Front: nnww  Back: None}</v>
       </c>
     </row>
@@ -2868,19 +2872,19 @@
         <v>395</v>
       </c>
       <c r="F42" t="str">
-        <f>CONCATENATE(A42,"%0Exits are: ",C42)</f>
+        <f t="shared" si="5"/>
         <v>Change in Course%0Exits are: N E W</v>
       </c>
       <c r="G42" t="str">
-        <f>CONCATENATE(A42, " -  Room Exits: ", C42, "  Front: ", IF(D42="", "None", D42), "  Back: ", IF(E42="", "None", E42))</f>
+        <f t="shared" si="6"/>
         <v>Change in Course -  Room Exits: N E W  Front: nnnewennw  Back: None</v>
       </c>
       <c r="H42" t="str">
-        <f>CONCATENATE("#sub {", F42, "} {", G42, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Change in Course%0Exits are: N E W} {Change in Course -  Room Exits: N E W  Front: nnnewennw  Back: None}</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A42,"} {%0 %1- ",G42, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Change in Course} {%0 %1- Change in Course -  Room Exits: N E W  Front: nnnewennw  Back: None}</v>
       </c>
     </row>
@@ -2898,19 +2902,19 @@
         <v>122</v>
       </c>
       <c r="F43" t="str">
-        <f>CONCATENATE(A43,"%0Exits are: ",C43)</f>
+        <f t="shared" si="5"/>
         <v>Charred Trees%0Exits are: N E</v>
       </c>
       <c r="G43" t="str">
-        <f>CONCATENATE(A43, " -  Room Exits: ", C43, "  Front: ", IF(D43="", "None", D43), "  Back: ", IF(E43="", "None", E43))</f>
+        <f t="shared" si="6"/>
         <v>Charred Trees -  Room Exits: N E  Front: esew  Back: None</v>
       </c>
       <c r="H43" t="str">
-        <f>CONCATENATE("#sub {", F43, "} {", G43, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Charred Trees%0Exits are: N E} {Charred Trees -  Room Exits: N E  Front: esew  Back: None}</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A43,"} {%0 %1- ",G43, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Charred Trees} {%0 %1- Charred Trees -  Room Exits: N E  Front: esew  Back: None}</v>
       </c>
     </row>
@@ -2928,19 +2932,19 @@
         <v>213</v>
       </c>
       <c r="F44" t="str">
-        <f>CONCATENATE(A44,"%0Exits are: ",C44)</f>
+        <f t="shared" si="5"/>
         <v>Choked Path%0Exits are: N S W</v>
       </c>
       <c r="G44" t="str">
-        <f>CONCATENATE(A44, " -  Room Exits: ", C44, "  Front: ", IF(D44="", "None", D44), "  Back: ", IF(E44="", "None", E44))</f>
+        <f t="shared" si="6"/>
         <v>Choked Path -  Room Exits: N S W  Front: nsnww  Back: None</v>
       </c>
       <c r="H44" t="str">
-        <f>CONCATENATE("#sub {", F44, "} {", G44, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Choked Path%0Exits are: N S W} {Choked Path -  Room Exits: N S W  Front: nsnww  Back: None}</v>
       </c>
       <c r="I44" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A44,"} {%0 %1- ",G44, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Choked Path} {%0 %1- Choked Path -  Room Exits: N S W  Front: nsnww  Back: None}</v>
       </c>
     </row>
@@ -2958,19 +2962,19 @@
         <v>241</v>
       </c>
       <c r="F45" t="str">
-        <f>CONCATENATE(A45,"%0Exits are: ",C45)</f>
+        <f t="shared" si="5"/>
         <v>Churning Trees%0Exits are: S W</v>
       </c>
       <c r="G45" t="str">
-        <f>CONCATENATE(A45, " -  Room Exits: ", C45, "  Front: ", IF(D45="", "None", D45), "  Back: ", IF(E45="", "None", E45))</f>
+        <f t="shared" si="6"/>
         <v>Churning Trees -  Room Exits: S W  Front: wensnww  Back: None</v>
       </c>
       <c r="H45" t="str">
-        <f>CONCATENATE("#sub {", F45, "} {", G45, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Churning Trees%0Exits are: S W} {Churning Trees -  Room Exits: S W  Front: wensnww  Back: None}</v>
       </c>
       <c r="I45" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A45,"} {%0 %1- ",G45, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Churning Trees} {%0 %1- Churning Trees -  Room Exits: S W  Front: wensnww  Back: None}</v>
       </c>
     </row>
@@ -2988,19 +2992,19 @@
         <v>267</v>
       </c>
       <c r="F46" t="str">
-        <f>CONCATENATE(A46,"%0Exits are: ",C46)</f>
+        <f t="shared" si="5"/>
         <v>Circle of Trees%0Exits are: E S W</v>
       </c>
       <c r="G46" t="str">
-        <f>CONCATENATE(A46, " -  Room Exits: ", C46, "  Front: ", IF(D46="", "None", D46), "  Back: ", IF(E46="", "None", E46))</f>
+        <f t="shared" si="6"/>
         <v>Circle of Trees -  Room Exits: E S W  Front: sew  Back: None</v>
       </c>
       <c r="H46" t="str">
-        <f>CONCATENATE("#sub {", F46, "} {", G46, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Circle of Trees%0Exits are: E S W} {Circle of Trees -  Room Exits: E S W  Front: sew  Back: None}</v>
       </c>
       <c r="I46" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A46,"} {%0 %1- ",G46, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Circle of Trees} {%0 %1- Circle of Trees -  Room Exits: E S W  Front: sew  Back: None}</v>
       </c>
     </row>
@@ -3018,19 +3022,19 @@
         <v>218</v>
       </c>
       <c r="F47" t="str">
-        <f>CONCATENATE(A47,"%0Exits are: ",C47)</f>
+        <f t="shared" si="5"/>
         <v>Cluster of Oaks%0Exits are: N E S W</v>
       </c>
       <c r="G47" t="str">
-        <f>CONCATENATE(A47, " -  Room Exits: ", C47, "  Front: ", IF(D47="", "None", D47), "  Back: ", IF(E47="", "None", E47))</f>
+        <f t="shared" si="6"/>
         <v>Cluster of Oaks -  Room Exits: N E S W  Front: snesw  Back: None</v>
       </c>
       <c r="H47" t="str">
-        <f>CONCATENATE("#sub {", F47, "} {", G47, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Cluster of Oaks%0Exits are: N E S W} {Cluster of Oaks -  Room Exits: N E S W  Front: snesw  Back: None}</v>
       </c>
       <c r="I47" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A47,"} {%0 %1- ",G47, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Cluster of Oaks} {%0 %1- Cluster of Oaks -  Room Exits: N E S W  Front: snesw  Back: None}</v>
       </c>
     </row>
@@ -3048,19 +3052,19 @@
         <v>160</v>
       </c>
       <c r="F48" t="str">
-        <f>CONCATENATE(A48,"%0Exits are: ",C48)</f>
+        <f t="shared" si="5"/>
         <v>Conic Mushrooms%0Exits are: N S</v>
       </c>
       <c r="G48" t="str">
-        <f>CONCATENATE(A48, " -  Room Exits: ", C48, "  Front: ", IF(D48="", "None", D48), "  Back: ", IF(E48="", "None", E48))</f>
+        <f t="shared" si="6"/>
         <v>Conic Mushrooms -  Room Exits: N S  Front: ssnenw  Back: None</v>
       </c>
       <c r="H48" t="str">
-        <f>CONCATENATE("#sub {", F48, "} {", G48, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Conic Mushrooms%0Exits are: N S} {Conic Mushrooms -  Room Exits: N S  Front: ssnenw  Back: None}</v>
       </c>
       <c r="I48" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A48,"} {%0 %1- ",G48, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Conic Mushrooms} {%0 %1- Conic Mushrooms -  Room Exits: N S  Front: ssnenw  Back: None}</v>
       </c>
     </row>
@@ -3078,19 +3082,19 @@
         <v>190</v>
       </c>
       <c r="F49" t="str">
-        <f>CONCATENATE(A49,"%0Exits are: ",C49)</f>
+        <f t="shared" si="5"/>
         <v>Corrupt Trees%0Exits are: N S</v>
       </c>
       <c r="G49" t="str">
-        <f>CONCATENATE(A49, " -  Room Exits: ", C49, "  Front: ", IF(D49="", "None", D49), "  Back: ", IF(E49="", "None", E49))</f>
+        <f t="shared" si="6"/>
         <v>Corrupt Trees -  Room Exits: N S  Front: nsesnnww  Back: None</v>
       </c>
       <c r="H49" t="str">
-        <f>CONCATENATE("#sub {", F49, "} {", G49, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Corrupt Trees%0Exits are: N S} {Corrupt Trees -  Room Exits: N S  Front: nsesnnww  Back: None}</v>
       </c>
       <c r="I49" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A49,"} {%0 %1- ",G49, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Corrupt Trees} {%0 %1- Corrupt Trees -  Room Exits: N S  Front: nsesnnww  Back: None}</v>
       </c>
     </row>
@@ -3108,19 +3112,19 @@
         <v>300</v>
       </c>
       <c r="F50" t="str">
-        <f>CONCATENATE(A50,"%0Exits are: ",C50)</f>
+        <f t="shared" si="5"/>
         <v>Crowded Forest Floor%0Exits are: N S W</v>
       </c>
       <c r="G50" t="str">
-        <f>CONCATENATE(A50, " -  Room Exits: ", C50, "  Front: ", IF(D50="", "None", D50), "  Back: ", IF(E50="", "None", E50))</f>
+        <f t="shared" si="6"/>
         <v>Crowded Forest Floor -  Room Exits: N S W  Front: nsnenw  Back: None</v>
       </c>
       <c r="H50" t="str">
-        <f>CONCATENATE("#sub {", F50, "} {", G50, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Crowded Forest Floor%0Exits are: N S W} {Crowded Forest Floor -  Room Exits: N S W  Front: nsnenw  Back: None}</v>
       </c>
       <c r="I50" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A50,"} {%0 %1- ",G50, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Crowded Forest Floor} {%0 %1- Crowded Forest Floor -  Room Exits: N S W  Front: nsnenw  Back: None}</v>
       </c>
     </row>
@@ -3138,19 +3142,19 @@
         <v>99</v>
       </c>
       <c r="F51" t="str">
-        <f>CONCATENATE(A51,"%0Exits are: ",C51)</f>
+        <f t="shared" si="5"/>
         <v>Crowded Path%0Exits are: N S</v>
       </c>
       <c r="G51" t="str">
-        <f>CONCATENATE(A51, " -  Room Exits: ", C51, "  Front: ", IF(D51="", "None", D51), "  Back: ", IF(E51="", "None", E51))</f>
+        <f t="shared" si="6"/>
         <v>Crowded Path -  Room Exits: N S  Front: swnwenw  Back: None</v>
       </c>
       <c r="H51" t="str">
-        <f>CONCATENATE("#sub {", F51, "} {", G51, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Crowded Path%0Exits are: N S} {Crowded Path -  Room Exits: N S  Front: swnwenw  Back: None}</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A51,"} {%0 %1- ",G51, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Crowded Path} {%0 %1- Crowded Path -  Room Exits: N S  Front: swnwenw  Back: None}</v>
       </c>
     </row>
@@ -3168,19 +3172,19 @@
         <v>137</v>
       </c>
       <c r="F52" t="str">
-        <f>CONCATENATE(A52,"%0Exits are: ",C52)</f>
+        <f t="shared" si="5"/>
         <v>Cul De Sac%0Exits are: E W</v>
       </c>
       <c r="G52" t="str">
-        <f>CONCATENATE(A52, " -  Room Exits: ", C52, "  Front: ", IF(D52="", "None", D52), "  Back: ", IF(E52="", "None", E52))</f>
+        <f t="shared" si="6"/>
         <v>Cul De Sac -  Room Exits: E W  Front: wennw  Back: None</v>
       </c>
       <c r="H52" t="str">
-        <f>CONCATENATE("#sub {", F52, "} {", G52, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Cul De Sac%0Exits are: E W} {Cul De Sac -  Room Exits: E W  Front: wennw  Back: None}</v>
       </c>
       <c r="I52" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A52,"} {%0 %1- ",G52, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Cul De Sac} {%0 %1- Cul De Sac -  Room Exits: E W  Front: wennw  Back: None}</v>
       </c>
     </row>
@@ -3198,19 +3202,19 @@
         <v>356</v>
       </c>
       <c r="F53" t="str">
-        <f>CONCATENATE(A53,"%0Exits are: ",C53)</f>
+        <f t="shared" si="5"/>
         <v>Curving Path%0Exits are: N S</v>
       </c>
       <c r="G53" t="str">
-        <f>CONCATENATE(A53, " -  Room Exits: ", C53, "  Front: ", IF(D53="", "None", D53), "  Back: ", IF(E53="", "None", E53))</f>
+        <f t="shared" si="6"/>
         <v>Curving Path -  Room Exits: N S  Front: snewennw  Back: None</v>
       </c>
       <c r="H53" t="str">
-        <f>CONCATENATE("#sub {", F53, "} {", G53, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Curving Path%0Exits are: N S} {Curving Path -  Room Exits: N S  Front: snewennw  Back: None}</v>
       </c>
       <c r="I53" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A53,"} {%0 %1- ",G53, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Curving Path} {%0 %1- Curving Path -  Room Exits: N S  Front: snewennw  Back: None}</v>
       </c>
     </row>
@@ -3228,19 +3232,19 @@
         <v>354</v>
       </c>
       <c r="F54" t="str">
-        <f>CONCATENATE(A54,"%0Exits are: ",C54)</f>
+        <f t="shared" si="5"/>
         <v>Damp Woods%0Exits are: E S</v>
       </c>
       <c r="G54" t="str">
-        <f>CONCATENATE(A54, " -  Room Exits: ", C54, "  Front: ", IF(D54="", "None", D54), "  Back: ", IF(E54="", "None", E54))</f>
+        <f t="shared" si="6"/>
         <v>Damp Woods -  Room Exits: E S  Front: eeesw  Back: None</v>
       </c>
       <c r="H54" t="str">
-        <f>CONCATENATE("#sub {", F54, "} {", G54, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Damp Woods%0Exits are: E S} {Damp Woods -  Room Exits: E S  Front: eeesw  Back: None}</v>
       </c>
       <c r="I54" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A54,"} {%0 %1- ",G54, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Damp Woods} {%0 %1- Damp Woods -  Room Exits: E S  Front: eeesw  Back: None}</v>
       </c>
     </row>
@@ -3258,19 +3262,19 @@
         <v>104</v>
       </c>
       <c r="F55" t="str">
-        <f>CONCATENATE(A55,"%0Exits are: ",C55)</f>
+        <f t="shared" si="5"/>
         <v>Dark Dense Forest%0Exits are: N E W</v>
       </c>
       <c r="G55" t="str">
-        <f>CONCATENATE(A55, " -  Room Exits: ", C55, "  Front: ", IF(D55="", "None", D55), "  Back: ", IF(E55="", "None", E55))</f>
+        <f t="shared" si="6"/>
         <v>Dark Dense Forest -  Room Exits: N E W  Front: wessesw  Back: None</v>
       </c>
       <c r="H55" t="str">
-        <f>CONCATENATE("#sub {", F55, "} {", G55, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Dense Forest%0Exits are: N E W} {Dark Dense Forest -  Room Exits: N E W  Front: wessesw  Back: None}</v>
       </c>
       <c r="I55" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A55,"} {%0 %1- ",G55, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Dense Forest} {%0 %1- Dark Dense Forest -  Room Exits: N E W  Front: wessesw  Back: None}</v>
       </c>
     </row>
@@ -3291,19 +3295,19 @@
         <v>146</v>
       </c>
       <c r="F56" t="str">
-        <f>CONCATENATE(A56,"%0Exits are: ",C56)</f>
+        <f t="shared" si="5"/>
         <v>Dark Forest Continues%0Exits are: N E S</v>
       </c>
       <c r="G56" t="str">
-        <f>CONCATENATE(A56, " -  Room Exits: ", C56, "  Front: ", IF(D56="", "None", D56), "  Back: ", IF(E56="", "None", E56))</f>
+        <f t="shared" si="6"/>
         <v>Dark Forest Continues -  Room Exits: N E S  Front: essnenw  Back: esene</v>
       </c>
       <c r="H56" t="str">
-        <f>CONCATENATE("#sub {", F56, "} {", G56, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Forest Continues%0Exits are: N E S} {Dark Forest Continues -  Room Exits: N E S  Front: essnenw  Back: esene}</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A56,"} {%0 %1- ",G56, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Forest Continues} {%0 %1- Dark Forest Continues -  Room Exits: N E S  Front: essnenw  Back: esene}</v>
       </c>
     </row>
@@ -3321,19 +3325,19 @@
         <v>316</v>
       </c>
       <c r="F57" t="str">
-        <f>CONCATENATE(A57,"%0Exits are: ",C57)</f>
+        <f t="shared" si="5"/>
         <v>Dark Forest Path%0Exits are: S W</v>
       </c>
       <c r="G57" t="str">
-        <f>CONCATENATE(A57, " -  Room Exits: ", C57, "  Front: ", IF(D57="", "None", D57), "  Back: ", IF(E57="", "None", E57))</f>
+        <f t="shared" si="6"/>
         <v>Dark Forest Path -  Room Exits: S W  Front: snsnww  Back: None</v>
       </c>
       <c r="H57" t="str">
-        <f>CONCATENATE("#sub {", F57, "} {", G57, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Forest Path%0Exits are: S W} {Dark Forest Path -  Room Exits: S W  Front: snsnww  Back: None}</v>
       </c>
       <c r="I57" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A57,"} {%0 %1- ",G57, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Forest Path} {%0 %1- Dark Forest Path -  Room Exits: S W  Front: snsnww  Back: None}</v>
       </c>
     </row>
@@ -3354,19 +3358,19 @@
         <v>410</v>
       </c>
       <c r="F58" t="str">
-        <f>CONCATENATE(A58,"%0Exits are: ",C58)</f>
+        <f t="shared" si="5"/>
         <v>Dark Green Moss%0Exits are: N S</v>
       </c>
       <c r="G58" t="str">
-        <f>CONCATENATE(A58, " -  Room Exits: ", C58, "  Front: ", IF(D58="", "None", D58), "  Back: ", IF(E58="", "None", E58))</f>
+        <f t="shared" si="6"/>
         <v>Dark Green Moss -  Room Exits: N S  Front: nww  Back: nwnneeseeneenesene</v>
       </c>
       <c r="H58" t="str">
-        <f>CONCATENATE("#sub {", F58, "} {", G58, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Green Moss%0Exits are: N S} {Dark Green Moss -  Room Exits: N S  Front: nww  Back: nwnneeseeneenesene}</v>
       </c>
       <c r="I58" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A58,"} {%0 %1- ",G58, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Green Moss} {%0 %1- Dark Green Moss -  Room Exits: N S  Front: nww  Back: nwnneeseeneenesene}</v>
       </c>
     </row>
@@ -3384,19 +3388,19 @@
         <v>338</v>
       </c>
       <c r="F59" t="str">
-        <f>CONCATENATE(A59,"%0Exits are: ",C59)</f>
+        <f t="shared" si="5"/>
         <v>Dark Halls%0Exits are: N E</v>
       </c>
       <c r="G59" t="str">
-        <f>CONCATENATE(A59, " -  Room Exits: ", C59, "  Front: ", IF(D59="", "None", D59), "  Back: ", IF(E59="", "None", E59))</f>
+        <f t="shared" si="6"/>
         <v>Dark Halls -  Room Exits: N E  Front: nsesew  Back: None</v>
       </c>
       <c r="H59" t="str">
-        <f>CONCATENATE("#sub {", F59, "} {", G59, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Halls%0Exits are: N E} {Dark Halls -  Room Exits: N E  Front: nsesew  Back: None}</v>
       </c>
       <c r="I59" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A59,"} {%0 %1- ",G59, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Halls} {%0 %1- Dark Halls -  Room Exits: N E  Front: nsesew  Back: None}</v>
       </c>
     </row>
@@ -3414,19 +3418,19 @@
         <v>187</v>
       </c>
       <c r="F60" t="str">
-        <f>CONCATENATE(A60,"%0Exits are: ",C60)</f>
+        <f t="shared" si="5"/>
         <v>Dark Hollow%0Exits are: N E</v>
       </c>
       <c r="G60" t="str">
-        <f>CONCATENATE(A60, " -  Room Exits: ", C60, "  Front: ", IF(D60="", "None", D60), "  Back: ", IF(E60="", "None", E60))</f>
+        <f t="shared" si="6"/>
         <v>Dark Hollow -  Room Exits: N E  Front: nnsewenw  Back: None</v>
       </c>
       <c r="H60" t="str">
-        <f>CONCATENATE("#sub {", F60, "} {", G60, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Hollow%0Exits are: N E} {Dark Hollow -  Room Exits: N E  Front: nnsewenw  Back: None}</v>
       </c>
       <c r="I60" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A60,"} {%0 %1- ",G60, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Hollow} {%0 %1- Dark Hollow -  Room Exits: N E  Front: nnsewenw  Back: None}</v>
       </c>
     </row>
@@ -3444,19 +3448,19 @@
         <v>85</v>
       </c>
       <c r="F61" t="str">
-        <f>CONCATENATE(A61,"%0Exits are: ",C61)</f>
+        <f t="shared" si="5"/>
         <v>Dark Massive Forest%0Exits are: N S W</v>
       </c>
       <c r="G61" t="str">
-        <f>CONCATENATE(A61, " -  Room Exits: ", C61, "  Front: ", IF(D61="", "None", D61), "  Back: ", IF(E61="", "None", E61))</f>
+        <f t="shared" si="6"/>
         <v>Dark Massive Forest -  Room Exits: N S W  Front: ssesw  Back: None</v>
       </c>
       <c r="H61" t="str">
-        <f>CONCATENATE("#sub {", F61, "} {", G61, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Massive Forest%0Exits are: N S W} {Dark Massive Forest -  Room Exits: N S W  Front: ssesw  Back: None}</v>
       </c>
       <c r="I61" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A61,"} {%0 %1- ",G61, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Massive Forest} {%0 %1- Dark Massive Forest -  Room Exits: N S W  Front: ssesw  Back: None}</v>
       </c>
     </row>
@@ -3474,19 +3478,19 @@
         <v>1</v>
       </c>
       <c r="F62" t="str">
-        <f>CONCATENATE(A62,"%0Exits are: ",C62)</f>
+        <f t="shared" si="5"/>
         <v>Dark Pit%0Exits are: N E S</v>
       </c>
       <c r="G62" t="str">
-        <f>CONCATENATE(A62, " -  Room Exits: ", C62, "  Front: ", IF(D62="", "None", D62), "  Back: ", IF(E62="", "None", E62))</f>
+        <f t="shared" si="6"/>
         <v>Dark Pit -  Room Exits: N E S  Front: nennw  Back: None</v>
       </c>
       <c r="H62" t="str">
-        <f>CONCATENATE("#sub {", F62, "} {", G62, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Pit%0Exits are: N E S} {Dark Pit -  Room Exits: N E S  Front: nennw  Back: None}</v>
       </c>
       <c r="I62" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A62,"} {%0 %1- ",G62, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Pit} {%0 %1- Dark Pit -  Room Exits: N E S  Front: nennw  Back: None}</v>
       </c>
     </row>
@@ -3504,19 +3508,19 @@
         <v>117</v>
       </c>
       <c r="F63" t="str">
-        <f>CONCATENATE(A63,"%0Exits are: ",C63)</f>
+        <f t="shared" si="5"/>
         <v>Dark Putrid Waters%0Exits are: N S</v>
       </c>
       <c r="G63" t="str">
-        <f>CONCATENATE(A63, " -  Room Exits: ", C63, "  Front: ", IF(D63="", "None", D63), "  Back: ", IF(E63="", "None", E63))</f>
+        <f t="shared" si="6"/>
         <v>Dark Putrid Waters -  Room Exits: N S  Front: ssesew  Back: None</v>
       </c>
       <c r="H63" t="str">
-        <f>CONCATENATE("#sub {", F63, "} {", G63, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Putrid Waters%0Exits are: N S} {Dark Putrid Waters -  Room Exits: N S  Front: ssesew  Back: None}</v>
       </c>
       <c r="I63" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A63,"} {%0 %1- ",G63, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Putrid Waters} {%0 %1- Dark Putrid Waters -  Room Exits: N S  Front: ssesew  Back: None}</v>
       </c>
     </row>
@@ -3534,19 +3538,19 @@
         <v>199</v>
       </c>
       <c r="F64" t="str">
-        <f>CONCATENATE(A64,"%0Exits are: ",C64)</f>
+        <f t="shared" si="5"/>
         <v>Dark Valley Forest%0Exits are: N S W</v>
       </c>
       <c r="G64" t="str">
-        <f>CONCATENATE(A64, " -  Room Exits: ", C64, "  Front: ", IF(D64="", "None", D64), "  Back: ", IF(E64="", "None", E64))</f>
+        <f t="shared" si="6"/>
         <v>Dark Valley Forest -  Room Exits: N S W  Front: nenw  Back: None</v>
       </c>
       <c r="H64" t="str">
-        <f>CONCATENATE("#sub {", F64, "} {", G64, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dark Valley Forest%0Exits are: N S W} {Dark Valley Forest -  Room Exits: N S W  Front: nenw  Back: None}</v>
       </c>
       <c r="I64" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A64,"} {%0 %1- ",G64, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Dark Valley Forest} {%0 %1- Dark Valley Forest -  Room Exits: N S W  Front: nenw  Back: None}</v>
       </c>
     </row>
@@ -3564,19 +3568,19 @@
         <v>55</v>
       </c>
       <c r="F65" t="str">
-        <f>CONCATENATE(A65,"%0Exits are: ",C65)</f>
+        <f t="shared" si="5"/>
         <v>Darkling Path%0Exits are: N S W</v>
       </c>
       <c r="G65" t="str">
-        <f>CONCATENATE(A65, " -  Room Exits: ", C65, "  Front: ", IF(D65="", "None", D65), "  Back: ", IF(E65="", "None", E65))</f>
+        <f t="shared" si="6"/>
         <v>Darkling Path -  Room Exits: N S W  Front: wenw  Back: None</v>
       </c>
       <c r="H65" t="str">
-        <f>CONCATENATE("#sub {", F65, "} {", G65, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Darkling Path%0Exits are: N S W} {Darkling Path -  Room Exits: N S W  Front: wenw  Back: None}</v>
       </c>
       <c r="I65" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A65,"} {%0 %1- ",G65, "}")</f>
+        <f t="shared" si="7"/>
         <v>#sub {%0 %1- Darkling Path} {%0 %1- Darkling Path -  Room Exits: N S W  Front: wenw  Back: None}</v>
       </c>
     </row>
@@ -3594,19 +3598,19 @@
         <v>176</v>
       </c>
       <c r="F66" t="str">
-        <f>CONCATENATE(A66,"%0Exits are: ",C66)</f>
+        <f t="shared" ref="F66:F97" si="9">CONCATENATE(A66,"%0Exits are: ",C66)</f>
         <v>Darkness%0Exits are: E S W</v>
       </c>
       <c r="G66" t="str">
-        <f>CONCATENATE(A66, " -  Room Exits: ", C66, "  Front: ", IF(D66="", "None", D66), "  Back: ", IF(E66="", "None", E66))</f>
+        <f t="shared" ref="G66:G97" si="10">CONCATENATE(A66, " -  Room Exits: ", C66, "  Front: ", IF(D66="", "None", D66), "  Back: ", IF(E66="", "None", E66))</f>
         <v>Darkness -  Room Exits: E S W  Front: wnnww  Back: None</v>
       </c>
       <c r="H66" t="str">
-        <f>CONCATENATE("#sub {", F66, "} {", G66, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Darkness%0Exits are: E S W} {Darkness -  Room Exits: E S W  Front: wnnww  Back: None}</v>
       </c>
       <c r="I66" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A66,"} {%0 %1- ",G66, "}")</f>
+        <f t="shared" ref="I66:I97" si="11">CONCATENATE("#sub {%0 %1- ",A66,"} {%0 %1- ",G66, "}")</f>
         <v>#sub {%0 %1- Darkness} {%0 %1- Darkness -  Room Exits: E S W  Front: wnnww  Back: None}</v>
       </c>
     </row>
@@ -3624,19 +3628,19 @@
         <v>279</v>
       </c>
       <c r="F67" t="str">
-        <f>CONCATENATE(A67,"%0Exits are: ",C67)</f>
+        <f t="shared" si="9"/>
         <v>Dead Trees%0Exits are: N E</v>
       </c>
       <c r="G67" t="str">
-        <f>CONCATENATE(A67, " -  Room Exits: ", C67, "  Front: ", IF(D67="", "None", D67), "  Back: ", IF(E67="", "None", E67))</f>
+        <f t="shared" si="10"/>
         <v>Dead Trees -  Room Exits: N E  Front: esewenw  Back: None</v>
       </c>
       <c r="H67" t="str">
-        <f>CONCATENATE("#sub {", F67, "} {", G67, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Dead Trees%0Exits are: N E} {Dead Trees -  Room Exits: N E  Front: esewenw  Back: None}</v>
       </c>
       <c r="I67" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A67,"} {%0 %1- ",G67, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dead Trees} {%0 %1- Dead Trees -  Room Exits: N E  Front: esewenw  Back: None}</v>
       </c>
     </row>
@@ -3654,19 +3658,19 @@
         <v>380</v>
       </c>
       <c r="F68" t="str">
-        <f>CONCATENATE(A68,"%0Exits are: ",C68)</f>
+        <f t="shared" si="9"/>
         <v>Decaying Marsh%0Exits are: N S</v>
       </c>
       <c r="G68" t="str">
-        <f>CONCATENATE(A68, " -  Room Exits: ", C68, "  Front: ", IF(D68="", "None", D68), "  Back: ", IF(E68="", "None", E68))</f>
+        <f t="shared" si="10"/>
         <v>Decaying Marsh -  Room Exits: N S  Front: nwnnsnnnww  Back: None</v>
       </c>
       <c r="H68" t="str">
-        <f>CONCATENATE("#sub {", F68, "} {", G68, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Decaying Marsh%0Exits are: N S} {Decaying Marsh -  Room Exits: N S  Front: nwnnsnnnww  Back: None}</v>
       </c>
       <c r="I68" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A68,"} {%0 %1- ",G68, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Decaying Marsh} {%0 %1- Decaying Marsh -  Room Exits: N S  Front: nwnnsnnnww  Back: None}</v>
       </c>
     </row>
@@ -3684,19 +3688,19 @@
         <v>381</v>
       </c>
       <c r="F69" t="str">
-        <f>CONCATENATE(A69,"%0Exits are: ",C69)</f>
+        <f t="shared" si="9"/>
         <v>Deep in the Swamp%0Exits are: N E W</v>
       </c>
       <c r="G69" t="str">
-        <f>CONCATENATE(A69, " -  Room Exits: ", C69, "  Front: ", IF(D69="", "None", D69), "  Back: ", IF(E69="", "None", E69))</f>
+        <f t="shared" si="10"/>
         <v>Deep in the Swamp -  Room Exits: N E W  Front: ennsnnnww  Back: None</v>
       </c>
       <c r="H69" t="str">
-        <f>CONCATENATE("#sub {", F69, "} {", G69, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Deep in the Swamp%0Exits are: N E W} {Deep in the Swamp -  Room Exits: N E W  Front: ennsnnnww  Back: None}</v>
       </c>
       <c r="I69" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A69,"} {%0 %1- ",G69, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Deep in the Swamp} {%0 %1- Deep in the Swamp -  Room Exits: N E W  Front: ennsnnnww  Back: None}</v>
       </c>
     </row>
@@ -3714,19 +3718,19 @@
         <v>71</v>
       </c>
       <c r="F70" t="str">
-        <f>CONCATENATE(A70,"%0Exits are: ",C70)</f>
+        <f t="shared" si="9"/>
         <v>Deep Moss%0Exits are: N W</v>
       </c>
       <c r="G70" t="str">
-        <f>CONCATENATE(A70, " -  Room Exits: ", C70, "  Front: ", IF(D70="", "None", D70), "  Back: ", IF(E70="", "None", E70))</f>
+        <f t="shared" si="10"/>
         <v>Deep Moss -  Room Exits: N W  Front: nwsnww  Back: None</v>
       </c>
       <c r="H70" t="str">
-        <f>CONCATENATE("#sub {", F70, "} {", G70, "}")</f>
+        <f t="shared" si="8"/>
         <v>#sub {Deep Moss%0Exits are: N W} {Deep Moss -  Room Exits: N W  Front: nwsnww  Back: None}</v>
       </c>
       <c r="I70" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A70,"} {%0 %1- ",G70, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Deep Moss} {%0 %1- Deep Moss -  Room Exits: N W  Front: nwsnww  Back: None}</v>
       </c>
     </row>
@@ -3744,19 +3748,19 @@
         <v>394</v>
       </c>
       <c r="F71" t="str">
-        <f>CONCATENATE(A71,"%0Exits are: ",C71)</f>
+        <f t="shared" si="9"/>
         <v>Deep Waters%0Exits are: E S W</v>
       </c>
       <c r="G71" t="str">
-        <f>CONCATENATE(A71, " -  Room Exits: ", C71, "  Front: ", IF(D71="", "None", D71), "  Back: ", IF(E71="", "None", E71))</f>
+        <f t="shared" si="10"/>
         <v>Deep Waters -  Room Exits: E S W  Front: eennsnnnww  Back: None</v>
       </c>
       <c r="H71" t="str">
-        <f>CONCATENATE("#sub {", F71, "} {", G71, "}")</f>
+        <f t="shared" ref="H71:H102" si="12">CONCATENATE("#sub {", F71, "} {", G71, "}")</f>
         <v>#sub {Deep Waters%0Exits are: E S W} {Deep Waters -  Room Exits: E S W  Front: eennsnnnww  Back: None}</v>
       </c>
       <c r="I71" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A71,"} {%0 %1- ",G71, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Deep Waters} {%0 %1- Deep Waters -  Room Exits: E S W  Front: eennsnnnww  Back: None}</v>
       </c>
     </row>
@@ -3774,19 +3778,19 @@
         <v>298</v>
       </c>
       <c r="F72" t="str">
-        <f>CONCATENATE(A72,"%0Exits are: ",C72)</f>
+        <f t="shared" si="9"/>
         <v>Dense Brush%0Exits are: E S</v>
       </c>
       <c r="G72" t="str">
-        <f>CONCATENATE(A72, " -  Room Exits: ", C72, "  Front: ", IF(D72="", "None", D72), "  Back: ", IF(E72="", "None", E72))</f>
+        <f t="shared" si="10"/>
         <v>Dense Brush -  Room Exits: E S  Front: eeessesw  Back: None</v>
       </c>
       <c r="H72" t="str">
-        <f>CONCATENATE("#sub {", F72, "} {", G72, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dense Brush%0Exits are: E S} {Dense Brush -  Room Exits: E S  Front: eeessesw  Back: None}</v>
       </c>
       <c r="I72" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A72,"} {%0 %1- ",G72, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dense Brush} {%0 %1- Dense Brush -  Room Exits: E S  Front: eeessesw  Back: None}</v>
       </c>
     </row>
@@ -3804,19 +3808,19 @@
         <v>302</v>
       </c>
       <c r="F73" t="str">
-        <f>CONCATENATE(A73,"%0Exits are: ",C73)</f>
+        <f t="shared" si="9"/>
         <v>Dense Dark Woodland%0Exits are: N E S</v>
       </c>
       <c r="G73" t="str">
-        <f>CONCATENATE(A73, " -  Room Exits: ", C73, "  Front: ", IF(D73="", "None", D73), "  Back: ", IF(E73="", "None", E73))</f>
+        <f t="shared" si="10"/>
         <v>Dense Dark Woodland -  Room Exits: N E S  Front: nesew  Back: None</v>
       </c>
       <c r="H73" t="str">
-        <f>CONCATENATE("#sub {", F73, "} {", G73, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dense Dark Woodland%0Exits are: N E S} {Dense Dark Woodland -  Room Exits: N E S  Front: nesew  Back: None}</v>
       </c>
       <c r="I73" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A73,"} {%0 %1- ",G73, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dense Dark Woodland} {%0 %1- Dense Dark Woodland -  Room Exits: N E S  Front: nesew  Back: None}</v>
       </c>
     </row>
@@ -3834,19 +3838,19 @@
         <v>210</v>
       </c>
       <c r="F74" t="str">
-        <f>CONCATENATE(A74,"%0Exits are: ",C74)</f>
+        <f t="shared" si="9"/>
         <v>Dense Underbrush%0Exits are: N W</v>
       </c>
       <c r="G74" t="str">
-        <f>CONCATENATE(A74, " -  Room Exits: ", C74, "  Front: ", IF(D74="", "None", D74), "  Back: ", IF(E74="", "None", E74))</f>
+        <f t="shared" si="10"/>
         <v>Dense Underbrush -  Room Exits: N W  Front: wnnsnww  Back: None</v>
       </c>
       <c r="H74" t="str">
-        <f>CONCATENATE("#sub {", F74, "} {", G74, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dense Underbrush%0Exits are: N W} {Dense Underbrush -  Room Exits: N W  Front: wnnsnww  Back: None}</v>
       </c>
       <c r="I74" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A74,"} {%0 %1- ",G74, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dense Underbrush} {%0 %1- Dense Underbrush -  Room Exits: N W  Front: wnnsnww  Back: None}</v>
       </c>
     </row>
@@ -3861,19 +3865,19 @@
         <v>2</v>
       </c>
       <c r="F75" t="str">
-        <f>CONCATENATE(A75,"%0Exits are: ",C75)</f>
+        <f t="shared" si="9"/>
         <v>Dim Vale%0Exits are: S W</v>
       </c>
       <c r="G75" t="str">
-        <f>CONCATENATE(A75, " -  Room Exits: ", C75, "  Front: ", IF(D75="", "None", D75), "  Back: ", IF(E75="", "None", E75))</f>
+        <f t="shared" si="10"/>
         <v>Dim Vale -  Room Exits: S W  Front: snnw  Back: None</v>
       </c>
       <c r="H75" t="str">
-        <f>CONCATENATE("#sub {", F75, "} {", G75, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dim Vale%0Exits are: S W} {Dim Vale -  Room Exits: S W  Front: snnw  Back: None}</v>
       </c>
       <c r="I75" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A75,"} {%0 %1- ",G75, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dim Vale} {%0 %1- Dim Vale -  Room Exits: S W  Front: snnw  Back: None}</v>
       </c>
     </row>
@@ -3894,19 +3898,19 @@
         <v>58</v>
       </c>
       <c r="F76" t="str">
-        <f>CONCATENATE(A76,"%0Exits are: ",C76)</f>
+        <f t="shared" si="9"/>
         <v>Dire Trees%0Exits are: E S W</v>
       </c>
       <c r="G76" t="str">
-        <f>CONCATENATE(A76, " -  Room Exits: ", C76, "  Front: ", IF(D76="", "None", D76), "  Back: ", IF(E76="", "None", E76))</f>
+        <f t="shared" si="10"/>
         <v>Dire Trees -  Room Exits: E S W  Front: esssnww  Back: eseeneenesene</v>
       </c>
       <c r="H76" t="str">
-        <f>CONCATENATE("#sub {", F76, "} {", G76, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dire Trees%0Exits are: E S W} {Dire Trees -  Room Exits: E S W  Front: esssnww  Back: eseeneenesene}</v>
       </c>
       <c r="I76" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A76,"} {%0 %1- ",G76, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dire Trees} {%0 %1- Dire Trees -  Room Exits: E S W  Front: esssnww  Back: eseeneenesene}</v>
       </c>
     </row>
@@ -3924,19 +3928,19 @@
         <v>278</v>
       </c>
       <c r="F77" t="str">
-        <f>CONCATENATE(A77,"%0Exits are: ",C77)</f>
+        <f t="shared" si="9"/>
         <v>Distrubing Noises%0Exits are: N S W</v>
       </c>
       <c r="G77" t="str">
-        <f>CONCATENATE(A77, " -  Room Exits: ", C77, "  Front: ", IF(D77="", "None", D77), "  Back: ", IF(E77="", "None", E77))</f>
+        <f t="shared" si="10"/>
         <v>Distrubing Noises -  Room Exits: N S W  Front: ssnesw  Back: None</v>
       </c>
       <c r="H77" t="str">
-        <f>CONCATENATE("#sub {", F77, "} {", G77, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Distrubing Noises%0Exits are: N S W} {Distrubing Noises -  Room Exits: N S W  Front: ssnesw  Back: None}</v>
       </c>
       <c r="I77" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A77,"} {%0 %1- ",G77, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Distrubing Noises} {%0 %1- Distrubing Noises -  Room Exits: N S W  Front: ssnesw  Back: None}</v>
       </c>
     </row>
@@ -3954,19 +3958,19 @@
         <v>120</v>
       </c>
       <c r="F78" t="str">
-        <f>CONCATENATE(A78,"%0Exits are: ",C78)</f>
+        <f t="shared" si="9"/>
         <v>Disturbing Undergrowth%0Exits are: N S</v>
       </c>
       <c r="G78" t="str">
-        <f>CONCATENATE(A78, " -  Room Exits: ", C78, "  Front: ", IF(D78="", "None", D78), "  Back: ", IF(E78="", "None", E78))</f>
+        <f t="shared" si="10"/>
         <v>Disturbing Undergrowth -  Room Exits: N S  Front: nnsssnesw  Back: None</v>
       </c>
       <c r="H78" t="str">
-        <f>CONCATENATE("#sub {", F78, "} {", G78, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Disturbing Undergrowth%0Exits are: N S} {Disturbing Undergrowth -  Room Exits: N S  Front: nnsssnesw  Back: None}</v>
       </c>
       <c r="I78" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A78,"} {%0 %1- ",G78, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Disturbing Undergrowth} {%0 %1- Disturbing Undergrowth -  Room Exits: N S  Front: nnsssnesw  Back: None}</v>
       </c>
     </row>
@@ -3984,19 +3988,19 @@
         <v>403</v>
       </c>
       <c r="F79" t="str">
-        <f>CONCATENATE(A79,"%0Exits are: ",C79)</f>
+        <f t="shared" si="9"/>
         <v>Drier Marshland%0Exits are: N E S</v>
       </c>
       <c r="G79" t="str">
-        <f>CONCATENATE(A79, " -  Room Exits: ", C79, "  Front: ", IF(D79="", "None", D79), "  Back: ", IF(E79="", "None", E79))</f>
+        <f t="shared" si="10"/>
         <v>Drier Marshland -  Room Exits: N E S  Front: eewsesew  Back: None</v>
       </c>
       <c r="H79" t="str">
-        <f>CONCATENATE("#sub {", F79, "} {", G79, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Drier Marshland%0Exits are: N E S} {Drier Marshland -  Room Exits: N E S  Front: eewsesew  Back: None}</v>
       </c>
       <c r="I79" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A79,"} {%0 %1- ",G79, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Drier Marshland} {%0 %1- Drier Marshland -  Room Exits: N E S  Front: eewsesew  Back: None}</v>
       </c>
     </row>
@@ -4014,19 +4018,19 @@
         <v>403</v>
       </c>
       <c r="F80" t="str">
-        <f>CONCATENATE(A80,"%0Exits are: ",C80)</f>
+        <f t="shared" si="9"/>
         <v>Drifting Track%0Exits are: N E W</v>
       </c>
       <c r="G80" t="str">
-        <f>CONCATENATE(A80, " -  Room Exits: ", C80, "  Front: ", IF(D80="", "None", D80), "  Back: ", IF(E80="", "None", E80))</f>
+        <f t="shared" si="10"/>
         <v>Drifting Track -  Room Exits: N E W  Front: eewsesew  Back: None</v>
       </c>
       <c r="H80" t="str">
-        <f>CONCATENATE("#sub {", F80, "} {", G80, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Drifting Track%0Exits are: N E W} {Drifting Track -  Room Exits: N E W  Front: eewsesew  Back: None}</v>
       </c>
       <c r="I80" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A80,"} {%0 %1- ",G80, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Drifting Track} {%0 %1- Drifting Track -  Room Exits: N E W  Front: eewsesew  Back: None}</v>
       </c>
     </row>
@@ -4047,19 +4051,19 @@
         <v>139</v>
       </c>
       <c r="F81" t="str">
-        <f>CONCATENATE(A81,"%0Exits are: ",C81)</f>
+        <f t="shared" si="9"/>
         <v>Dripping Moss%0Exits are: E S W</v>
       </c>
       <c r="G81" t="str">
-        <f>CONCATENATE(A81, " -  Room Exits: ", C81, "  Front: ", IF(D81="", "None", D81), "  Back: ", IF(E81="", "None", E81))</f>
+        <f t="shared" si="10"/>
         <v>Dripping Moss -  Room Exits: E S W  Front: wsnnww  Back: eenesene</v>
       </c>
       <c r="H81" t="str">
-        <f>CONCATENATE("#sub {", F81, "} {", G81, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dripping Moss%0Exits are: E S W} {Dripping Moss -  Room Exits: E S W  Front: wsnnww  Back: eenesene}</v>
       </c>
       <c r="I81" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A81,"} {%0 %1- ",G81, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dripping Moss} {%0 %1- Dripping Moss -  Room Exits: E S W  Front: wsnnww  Back: eenesene}</v>
       </c>
     </row>
@@ -4077,19 +4081,19 @@
         <v>297</v>
       </c>
       <c r="F82" t="str">
-        <f>CONCATENATE(A82,"%0Exits are: ",C82)</f>
+        <f t="shared" si="9"/>
         <v>Dusky Wood%0Exits are: E S W</v>
       </c>
       <c r="G82" t="str">
-        <f>CONCATENATE(A82, " -  Room Exits: ", C82, "  Front: ", IF(D82="", "None", D82), "  Back: ", IF(E82="", "None", E82))</f>
+        <f t="shared" si="10"/>
         <v>Dusky Wood -  Room Exits: E S W  Front: eessesw  Back: None</v>
       </c>
       <c r="H82" t="str">
-        <f>CONCATENATE("#sub {", F82, "} {", G82, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dusky Wood%0Exits are: E S W} {Dusky Wood -  Room Exits: E S W  Front: eessesw  Back: None}</v>
       </c>
       <c r="I82" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A82,"} {%0 %1- ",G82, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dusky Wood} {%0 %1- Dusky Wood -  Room Exits: E S W  Front: eessesw  Back: None}</v>
       </c>
     </row>
@@ -4107,19 +4111,19 @@
         <v>228</v>
       </c>
       <c r="F83" t="str">
-        <f>CONCATENATE(A83,"%0Exits are: ",C83)</f>
+        <f t="shared" si="9"/>
         <v>Dusty Hollow%0Exits are: E S</v>
       </c>
       <c r="G83" t="str">
-        <f>CONCATENATE(A83, " -  Room Exits: ", C83, "  Front: ", IF(D83="", "None", D83), "  Back: ", IF(E83="", "None", E83))</f>
+        <f t="shared" si="10"/>
         <v>Dusty Hollow -  Room Exits: E S  Front: ennw  Back: None</v>
       </c>
       <c r="H83" t="str">
-        <f>CONCATENATE("#sub {", F83, "} {", G83, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dusty Hollow%0Exits are: E S} {Dusty Hollow -  Room Exits: E S  Front: ennw  Back: None}</v>
       </c>
       <c r="I83" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A83,"} {%0 %1- ",G83, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dusty Hollow} {%0 %1- Dusty Hollow -  Room Exits: E S  Front: ennw  Back: None}</v>
       </c>
     </row>
@@ -4137,19 +4141,19 @@
         <v>359</v>
       </c>
       <c r="F84" t="str">
-        <f>CONCATENATE(A84,"%0Exits are: ",C84)</f>
+        <f t="shared" si="9"/>
         <v>Dusty Smell%0Exits are: N S</v>
       </c>
       <c r="G84" t="str">
-        <f>CONCATENATE(A84, " -  Room Exits: ", C84, "  Front: ", IF(D84="", "None", D84), "  Back: ", IF(E84="", "None", E84))</f>
+        <f t="shared" si="10"/>
         <v>Dusty Smell -  Room Exits: N S  Front: sewwnnww  Back: None</v>
       </c>
       <c r="H84" t="str">
-        <f>CONCATENATE("#sub {", F84, "} {", G84, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Dusty Smell%0Exits are: N S} {Dusty Smell -  Room Exits: N S  Front: sewwnnww  Back: None}</v>
       </c>
       <c r="I84" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A84,"} {%0 %1- ",G84, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Dusty Smell} {%0 %1- Dusty Smell -  Room Exits: N S  Front: sewwnnww  Back: None}</v>
       </c>
     </row>
@@ -4167,19 +4171,19 @@
         <v>396</v>
       </c>
       <c r="F85" t="str">
-        <f>CONCATENATE(A85,"%0Exits are: ",C85)</f>
+        <f t="shared" si="9"/>
         <v>Eerie Marsh%0Exits are: E S W</v>
       </c>
       <c r="G85" t="str">
-        <f>CONCATENATE(A85, " -  Room Exits: ", C85, "  Front: ", IF(D85="", "None", D85), "  Back: ", IF(E85="", "None", E85))</f>
+        <f t="shared" si="10"/>
         <v>Eerie Marsh -  Room Exits: E S W  Front: ssnnewennw  Back: None</v>
       </c>
       <c r="H85" t="str">
-        <f>CONCATENATE("#sub {", F85, "} {", G85, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Eerie Marsh%0Exits are: E S W} {Eerie Marsh -  Room Exits: E S W  Front: ssnnewennw  Back: None}</v>
       </c>
       <c r="I85" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A85,"} {%0 %1- ",G85, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Eerie Marsh} {%0 %1- Eerie Marsh -  Room Exits: E S W  Front: ssnnewennw  Back: None}</v>
       </c>
     </row>
@@ -4197,19 +4201,19 @@
         <v>228</v>
       </c>
       <c r="F86" t="str">
-        <f>CONCATENATE(A86,"%0Exits are: ",C86)</f>
+        <f t="shared" si="9"/>
         <v>Endless Path%0Exits are: N E</v>
       </c>
       <c r="G86" t="str">
-        <f>CONCATENATE(A86, " -  Room Exits: ", C86, "  Front: ", IF(D86="", "None", D86), "  Back: ", IF(E86="", "None", E86))</f>
+        <f t="shared" si="10"/>
         <v>Endless Path -  Room Exits: N E  Front: ennw  Back: None</v>
       </c>
       <c r="H86" t="str">
-        <f>CONCATENATE("#sub {", F86, "} {", G86, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Endless Path%0Exits are: N E} {Endless Path -  Room Exits: N E  Front: ennw  Back: None}</v>
       </c>
       <c r="I86" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A86,"} {%0 %1- ",G86, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Endless Path} {%0 %1- Endless Path -  Room Exits: N E  Front: ennw  Back: None}</v>
       </c>
     </row>
@@ -4227,19 +4231,19 @@
         <v>226</v>
       </c>
       <c r="F87" t="str">
-        <f>CONCATENATE(A87,"%0Exits are: ",C87)</f>
+        <f t="shared" si="9"/>
         <v>Entrance to Path%0Exits are: E W</v>
       </c>
       <c r="G87" t="str">
-        <f>CONCATENATE(A87, " -  Room Exits: ", C87, "  Front: ", IF(D87="", "None", D87), "  Back: ", IF(E87="", "None", E87))</f>
+        <f t="shared" si="10"/>
         <v>Entrance to Path -  Room Exits: E W  Front: eesw  Back: None</v>
       </c>
       <c r="H87" t="str">
-        <f>CONCATENATE("#sub {", F87, "} {", G87, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Entrance to Path%0Exits are: E W} {Entrance to Path -  Room Exits: E W  Front: eesw  Back: None}</v>
       </c>
       <c r="I87" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A87,"} {%0 %1- ",G87, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Entrance to Path} {%0 %1- Entrance to Path -  Room Exits: E W  Front: eesw  Back: None}</v>
       </c>
     </row>
@@ -4257,19 +4261,19 @@
         <v>47</v>
       </c>
       <c r="F88" t="str">
-        <f>CONCATENATE(A88,"%0Exits are: ",C88)</f>
+        <f t="shared" si="9"/>
         <v>Entrance to the Hidden Vale%0Exits are: E W</v>
       </c>
       <c r="G88" t="str">
-        <f>CONCATENATE(A88, " -  Room Exits: ", C88, "  Front: ", IF(D88="", "None", D88), "  Back: ", IF(E88="", "None", E88))</f>
+        <f t="shared" si="10"/>
         <v>Entrance to the Hidden Vale -  Room Exits: E W  Front: None  Back: enneeseeneenesene</v>
       </c>
       <c r="H88" t="str">
-        <f>CONCATENATE("#sub {", F88, "} {", G88, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Entrance to the Hidden Vale%0Exits are: E W} {Entrance to the Hidden Vale -  Room Exits: E W  Front: None  Back: enneeseeneenesene}</v>
       </c>
       <c r="I88" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A88,"} {%0 %1- ",G88, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Entrance to the Hidden Vale} {%0 %1- Entrance to the Hidden Vale -  Room Exits: E W  Front: None  Back: enneeseeneenesene}</v>
       </c>
     </row>
@@ -4287,19 +4291,19 @@
         <v>295</v>
       </c>
       <c r="F89" t="str">
-        <f>CONCATENATE(A89,"%0Exits are: ",C89)</f>
+        <f t="shared" si="9"/>
         <v>Eryn Lome%0Exits are: N E S W</v>
       </c>
       <c r="G89" t="str">
-        <f>CONCATENATE(A89, " -  Room Exits: ", C89, "  Front: ", IF(D89="", "None", D89), "  Back: ", IF(E89="", "None", E89))</f>
+        <f t="shared" si="10"/>
         <v>Eryn Lome -  Room Exits: N E S W  Front: snennw  Back: None</v>
       </c>
       <c r="H89" t="str">
-        <f>CONCATENATE("#sub {", F89, "} {", G89, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Eryn Lome%0Exits are: N E S W} {Eryn Lome -  Room Exits: N E S W  Front: snennw  Back: None}</v>
       </c>
       <c r="I89" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A89,"} {%0 %1- ",G89, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Eryn Lome} {%0 %1- Eryn Lome -  Room Exits: N E S W  Front: snennw  Back: None}</v>
       </c>
     </row>
@@ -4317,19 +4321,19 @@
         <v>296</v>
       </c>
       <c r="F90" t="str">
-        <f>CONCATENATE(A90,"%0Exits are: ",C90)</f>
+        <f t="shared" si="9"/>
         <v>Eryn Wethrin%0Exits are: E S</v>
       </c>
       <c r="G90" t="str">
-        <f>CONCATENATE(A90, " -  Room Exits: ", C90, "  Front: ", IF(D90="", "None", D90), "  Back: ", IF(E90="", "None", E90))</f>
+        <f t="shared" si="10"/>
         <v>Eryn Wethrin -  Room Exits: E S  Front: esnennw  Back: None</v>
       </c>
       <c r="H90" t="str">
-        <f>CONCATENATE("#sub {", F90, "} {", G90, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Eryn Wethrin%0Exits are: E S} {Eryn Wethrin -  Room Exits: E S  Front: esnennw  Back: None}</v>
       </c>
       <c r="I90" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A90,"} {%0 %1- ",G90, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Eryn Wethrin} {%0 %1- Eryn Wethrin -  Room Exits: E S  Front: esnennw  Back: None}</v>
       </c>
     </row>
@@ -4347,19 +4351,19 @@
         <v>296</v>
       </c>
       <c r="F91" t="str">
-        <f>CONCATENATE(A91,"%0Exits are: ",C91)</f>
+        <f t="shared" si="9"/>
         <v>Faint Path%0Exits are: E W</v>
       </c>
       <c r="G91" t="str">
-        <f>CONCATENATE(A91, " -  Room Exits: ", C91, "  Front: ", IF(D91="", "None", D91), "  Back: ", IF(E91="", "None", E91))</f>
+        <f t="shared" si="10"/>
         <v>Faint Path -  Room Exits: E W  Front: esnennw  Back: None</v>
       </c>
       <c r="H91" t="str">
-        <f>CONCATENATE("#sub {", F91, "} {", G91, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Faint Path%0Exits are: E W} {Faint Path -  Room Exits: E W  Front: esnennw  Back: None}</v>
       </c>
       <c r="I91" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A91,"} {%0 %1- ",G91, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Faint Path} {%0 %1- Faint Path -  Room Exits: E W  Front: esnennw  Back: None}</v>
       </c>
     </row>
@@ -4377,19 +4381,19 @@
         <v>72</v>
       </c>
       <c r="F92" t="str">
-        <f>CONCATENATE(A92,"%0Exits are: ",C92)</f>
+        <f t="shared" si="9"/>
         <v>Fallen Leaves%0Exits are: N S W</v>
       </c>
       <c r="G92" t="str">
-        <f>CONCATENATE(A92, " -  Room Exits: ", C92, "  Front: ", IF(D92="", "None", D92), "  Back: ", IF(E92="", "None", E92))</f>
+        <f t="shared" si="10"/>
         <v>Fallen Leaves -  Room Exits: N S W  Front: snwsnww  Back: None</v>
       </c>
       <c r="H92" t="str">
-        <f>CONCATENATE("#sub {", F92, "} {", G92, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Fallen Leaves%0Exits are: N S W} {Fallen Leaves -  Room Exits: N S W  Front: snwsnww  Back: None}</v>
       </c>
       <c r="I92" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A92,"} {%0 %1- ",G92, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Fallen Leaves} {%0 %1- Fallen Leaves -  Room Exits: N S W  Front: snwsnww  Back: None}</v>
       </c>
     </row>
@@ -4407,19 +4411,19 @@
         <v>66</v>
       </c>
       <c r="F93" t="str">
-        <f>CONCATENATE(A93,"%0Exits are: ",C93)</f>
+        <f t="shared" si="9"/>
         <v>Fallen Trees%0Exits are: N E S W</v>
       </c>
       <c r="G93" t="str">
-        <f>CONCATENATE(A93, " -  Room Exits: ", C93, "  Front: ", IF(D93="", "None", D93), "  Back: ", IF(E93="", "None", E93))</f>
+        <f t="shared" si="10"/>
         <v>Fallen Trees -  Room Exits: N E S W  Front: snww  Back: None</v>
       </c>
       <c r="H93" t="str">
-        <f>CONCATENATE("#sub {", F93, "} {", G93, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Fallen Trees%0Exits are: N E S W} {Fallen Trees -  Room Exits: N E S W  Front: snww  Back: None}</v>
       </c>
       <c r="I93" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A93,"} {%0 %1- ",G93, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Fallen Trees} {%0 %1- Fallen Trees -  Room Exits: N E S W  Front: snww  Back: None}</v>
       </c>
     </row>
@@ -4437,19 +4441,19 @@
         <v>170</v>
       </c>
       <c r="F94" t="str">
-        <f>CONCATENATE(A94,"%0Exits are: ",C94)</f>
+        <f t="shared" si="9"/>
         <v>False Hope%0Exits are: N W</v>
       </c>
       <c r="G94" t="str">
-        <f>CONCATENATE(A94, " -  Room Exits: ", C94, "  Front: ", IF(D94="", "None", D94), "  Back: ", IF(E94="", "None", E94))</f>
+        <f t="shared" si="10"/>
         <v>False Hope -  Room Exits: N W  Front: nnnww  Back: None</v>
       </c>
       <c r="H94" t="str">
-        <f>CONCATENATE("#sub {", F94, "} {", G94, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {False Hope%0Exits are: N W} {False Hope -  Room Exits: N W  Front: nnnww  Back: None}</v>
       </c>
       <c r="I94" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A94,"} {%0 %1- ",G94, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- False Hope} {%0 %1- False Hope -  Room Exits: N W  Front: nnnww  Back: None}</v>
       </c>
     </row>
@@ -4467,19 +4471,19 @@
         <v>400</v>
       </c>
       <c r="F95" t="str">
-        <f>CONCATENATE(A95,"%0Exits are: ",C95)</f>
+        <f t="shared" si="9"/>
         <v>Flooded Forest%0Exits are: E S</v>
       </c>
       <c r="G95" t="str">
-        <f>CONCATENATE(A95, " -  Room Exits: ", C95, "  Front: ", IF(D95="", "None", D95), "  Back: ", IF(E95="", "None", E95))</f>
+        <f t="shared" si="10"/>
         <v>Flooded Forest -  Room Exits: E S  Front: snnnewennw  Back: None</v>
       </c>
       <c r="H95" t="str">
-        <f>CONCATENATE("#sub {", F95, "} {", G95, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Flooded Forest%0Exits are: E S} {Flooded Forest -  Room Exits: E S  Front: snnnewennw  Back: None}</v>
       </c>
       <c r="I95" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A95,"} {%0 %1- ",G95, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Flooded Forest} {%0 %1- Flooded Forest -  Room Exits: E S  Front: snnnewennw  Back: None}</v>
       </c>
     </row>
@@ -4497,19 +4501,19 @@
         <v>264</v>
       </c>
       <c r="F96" t="str">
-        <f>CONCATENATE(A96,"%0Exits are: ",C96)</f>
+        <f t="shared" si="9"/>
         <v>Forest Guardians%0Exits are: N S W</v>
       </c>
       <c r="G96" t="str">
-        <f>CONCATENATE(A96, " -  Room Exits: ", C96, "  Front: ", IF(D96="", "None", D96), "  Back: ", IF(E96="", "None", E96))</f>
+        <f t="shared" si="10"/>
         <v>Forest Guardians -  Room Exits: N S W  Front: nsewenw  Back: None</v>
       </c>
       <c r="H96" t="str">
-        <f>CONCATENATE("#sub {", F96, "} {", G96, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Forest Guardians%0Exits are: N S W} {Forest Guardians -  Room Exits: N S W  Front: nsewenw  Back: None}</v>
       </c>
       <c r="I96" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A96,"} {%0 %1- ",G96, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Forest Guardians} {%0 %1- Forest Guardians -  Room Exits: N S W  Front: nsewenw  Back: None}</v>
       </c>
     </row>
@@ -4527,19 +4531,19 @@
         <v>253</v>
       </c>
       <c r="F97" t="str">
-        <f>CONCATENATE(A97,"%0Exits are: ",C97)</f>
+        <f t="shared" si="9"/>
         <v>Forest Ledge%0Exits are: E S</v>
       </c>
       <c r="G97" t="str">
-        <f>CONCATENATE(A97, " -  Room Exits: ", C97, "  Front: ", IF(D97="", "None", D97), "  Back: ", IF(E97="", "None", E97))</f>
+        <f t="shared" si="10"/>
         <v>Forest Ledge -  Room Exits: E S  Front: senenw  Back: None</v>
       </c>
       <c r="H97" t="str">
-        <f>CONCATENATE("#sub {", F97, "} {", G97, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Forest Ledge%0Exits are: E S} {Forest Ledge -  Room Exits: E S  Front: senenw  Back: None}</v>
       </c>
       <c r="I97" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A97,"} {%0 %1- ",G97, "}")</f>
+        <f t="shared" si="11"/>
         <v>#sub {%0 %1- Forest Ledge} {%0 %1- Forest Ledge -  Room Exits: E S  Front: senenw  Back: None}</v>
       </c>
     </row>
@@ -4557,19 +4561,19 @@
         <v>170</v>
       </c>
       <c r="F98" t="str">
-        <f>CONCATENATE(A98,"%0Exits are: ",C98)</f>
+        <f t="shared" ref="F98:F129" si="13">CONCATENATE(A98,"%0Exits are: ",C98)</f>
         <v>Forest of Despair%0Exits are: N E</v>
       </c>
       <c r="G98" t="str">
-        <f>CONCATENATE(A98, " -  Room Exits: ", C98, "  Front: ", IF(D98="", "None", D98), "  Back: ", IF(E98="", "None", E98))</f>
+        <f t="shared" ref="G98:G129" si="14">CONCATENATE(A98, " -  Room Exits: ", C98, "  Front: ", IF(D98="", "None", D98), "  Back: ", IF(E98="", "None", E98))</f>
         <v>Forest of Despair -  Room Exits: N E  Front: nnnww  Back: None</v>
       </c>
       <c r="H98" t="str">
-        <f>CONCATENATE("#sub {", F98, "} {", G98, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Forest of Despair%0Exits are: N E} {Forest of Despair -  Room Exits: N E  Front: nnnww  Back: None}</v>
       </c>
       <c r="I98" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A98,"} {%0 %1- ",G98, "}")</f>
+        <f t="shared" ref="I98:I129" si="15">CONCATENATE("#sub {%0 %1- ",A98,"} {%0 %1- ",G98, "}")</f>
         <v>#sub {%0 %1- Forest of Despair} {%0 %1- Forest of Despair -  Room Exits: N E  Front: nnnww  Back: None}</v>
       </c>
     </row>
@@ -4587,19 +4591,19 @@
         <v>179</v>
       </c>
       <c r="F99" t="str">
-        <f>CONCATENATE(A99,"%0Exits are: ",C99)</f>
+        <f t="shared" si="13"/>
         <v>Forest of Endless Night%0Exits are: N E S</v>
       </c>
       <c r="G99" t="str">
-        <f>CONCATENATE(A99, " -  Room Exits: ", C99, "  Front: ", IF(D99="", "None", D99), "  Back: ", IF(E99="", "None", E99))</f>
+        <f t="shared" si="14"/>
         <v>Forest of Endless Night -  Room Exits: N E S  Front: ewenw  Back: None</v>
       </c>
       <c r="H99" t="str">
-        <f>CONCATENATE("#sub {", F99, "} {", G99, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Forest of Endless Night%0Exits are: N E S} {Forest of Endless Night -  Room Exits: N E S  Front: ewenw  Back: None}</v>
       </c>
       <c r="I99" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A99,"} {%0 %1- ",G99, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Forest of Endless Night} {%0 %1- Forest of Endless Night -  Room Exits: N E S  Front: ewenw  Back: None}</v>
       </c>
     </row>
@@ -4620,19 +4624,19 @@
         <v>134</v>
       </c>
       <c r="F100" t="str">
-        <f>CONCATENATE(A100,"%0Exits are: ",C100)</f>
+        <f t="shared" si="13"/>
         <v>Game Trail%0Exits are: E W</v>
       </c>
       <c r="G100" t="str">
-        <f>CONCATENATE(A100, " -  Room Exits: ", C100, "  Front: ", IF(D100="", "None", D100), "  Back: ", IF(E100="", "None", E100))</f>
+        <f t="shared" si="14"/>
         <v>Game Trail -  Room Exits: E W  Front: ewennw  Back: eneenesene</v>
       </c>
       <c r="H100" t="str">
-        <f>CONCATENATE("#sub {", F100, "} {", G100, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Game Trail%0Exits are: E W} {Game Trail -  Room Exits: E W  Front: ewennw  Back: eneenesene}</v>
       </c>
       <c r="I100" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A100,"} {%0 %1- ",G100, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Game Trail} {%0 %1- Game Trail -  Room Exits: E W  Front: ewennw  Back: eneenesene}</v>
       </c>
     </row>
@@ -4650,19 +4654,19 @@
         <v>223</v>
       </c>
       <c r="F101" t="str">
-        <f>CONCATENATE(A101,"%0Exits are: ",C101)</f>
+        <f t="shared" si="13"/>
         <v>Ghastly Trees%0Exits are: N W</v>
       </c>
       <c r="G101" t="str">
-        <f>CONCATENATE(A101, " -  Room Exits: ", C101, "  Front: ", IF(D101="", "None", D101), "  Back: ", IF(E101="", "None", E101))</f>
+        <f t="shared" si="14"/>
         <v>Ghastly Trees -  Room Exits: N W  Front: nesw  Back: None</v>
       </c>
       <c r="H101" t="str">
-        <f>CONCATENATE("#sub {", F101, "} {", G101, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Ghastly Trees%0Exits are: N W} {Ghastly Trees -  Room Exits: N W  Front: nesw  Back: None}</v>
       </c>
       <c r="I101" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A101,"} {%0 %1- ",G101, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Ghastly Trees} {%0 %1- Ghastly Trees -  Room Exits: N W  Front: nesw  Back: None}</v>
       </c>
     </row>
@@ -4683,19 +4687,19 @@
         <v>158</v>
       </c>
       <c r="F102" t="str">
-        <f>CONCATENATE(A102,"%0Exits are: ",C102)</f>
+        <f t="shared" si="13"/>
         <v>Giant Ancient Trees%0Exits are: N E W U</v>
       </c>
       <c r="G102" t="str">
-        <f>CONCATENATE(A102, " -  Room Exits: ", C102, "  Front: ", IF(D102="", "None", D102), "  Back: ", IF(E102="", "None", E102))</f>
+        <f t="shared" si="14"/>
         <v>Giant Ancient Trees -  Room Exits: N E W U  Front: nnnnnww  Back: ne</v>
       </c>
       <c r="H102" t="str">
-        <f>CONCATENATE("#sub {", F102, "} {", G102, "}")</f>
+        <f t="shared" si="12"/>
         <v>#sub {Giant Ancient Trees%0Exits are: N E W U} {Giant Ancient Trees -  Room Exits: N E W U  Front: nnnnnww  Back: ne}</v>
       </c>
       <c r="I102" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A102,"} {%0 %1- ",G102, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Giant Ancient Trees} {%0 %1- Giant Ancient Trees -  Room Exits: N E W U  Front: nnnnnww  Back: ne}</v>
       </c>
     </row>
@@ -4716,19 +4720,19 @@
         <v>154</v>
       </c>
       <c r="F103" t="str">
-        <f>CONCATENATE(A103,"%0Exits are: ",C103)</f>
+        <f t="shared" si="13"/>
         <v>Gleaming Eyes%0Exits are: N E S</v>
       </c>
       <c r="G103" t="str">
-        <f>CONCATENATE(A103, " -  Room Exits: ", C103, "  Front: ", IF(D103="", "None", D103), "  Back: ", IF(E103="", "None", E103))</f>
+        <f t="shared" si="14"/>
         <v>Gleaming Eyes -  Room Exits: N E S  Front: snenw  Back: ene</v>
       </c>
       <c r="H103" t="str">
-        <f>CONCATENATE("#sub {", F103, "} {", G103, "}")</f>
+        <f t="shared" ref="H103:H134" si="16">CONCATENATE("#sub {", F103, "} {", G103, "}")</f>
         <v>#sub {Gleaming Eyes%0Exits are: N E S} {Gleaming Eyes -  Room Exits: N E S  Front: snenw  Back: ene}</v>
       </c>
       <c r="I103" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A103,"} {%0 %1- ",G103, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Gleaming Eyes} {%0 %1- Gleaming Eyes -  Room Exits: N E S  Front: snenw  Back: ene}</v>
       </c>
     </row>
@@ -4746,19 +4750,19 @@
         <v>78</v>
       </c>
       <c r="F104" t="str">
-        <f>CONCATENATE(A104,"%0Exits are: ",C104)</f>
+        <f t="shared" si="13"/>
         <v>Gloomy Trees%0Exits are: E S</v>
       </c>
       <c r="G104" t="str">
-        <f>CONCATENATE(A104, " -  Room Exits: ", C104, "  Front: ", IF(D104="", "None", D104), "  Back: ", IF(E104="", "None", E104))</f>
+        <f t="shared" si="14"/>
         <v>Gloomy Trees -  Room Exits: E S  Front: esnnnww  Back: None</v>
       </c>
       <c r="H104" t="str">
-        <f>CONCATENATE("#sub {", F104, "} {", G104, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Gloomy Trees%0Exits are: E S} {Gloomy Trees -  Room Exits: E S  Front: esnnnww  Back: None}</v>
       </c>
       <c r="I104" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A104,"} {%0 %1- ",G104, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Gloomy Trees} {%0 %1- Gloomy Trees -  Room Exits: E S  Front: esnnnww  Back: None}</v>
       </c>
     </row>
@@ -4776,19 +4780,19 @@
         <v>310</v>
       </c>
       <c r="F105" t="str">
-        <f>CONCATENATE(A105,"%0Exits are: ",C105)</f>
+        <f t="shared" si="13"/>
         <v>Grasping Thorns%0Exits are: N W</v>
       </c>
       <c r="G105" t="str">
-        <f>CONCATENATE(A105, " -  Room Exits: ", C105, "  Front: ", IF(D105="", "None", D105), "  Back: ", IF(E105="", "None", E105))</f>
+        <f t="shared" si="14"/>
         <v>Grasping Thorns -  Room Exits: N W  Front: wwnnww  Back: None</v>
       </c>
       <c r="H105" t="str">
-        <f>CONCATENATE("#sub {", F105, "} {", G105, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Grasping Thorns%0Exits are: N W} {Grasping Thorns -  Room Exits: N W  Front: wwnnww  Back: None}</v>
       </c>
       <c r="I105" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A105,"} {%0 %1- ",G105, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Grasping Thorns} {%0 %1- Grasping Thorns -  Room Exits: N W  Front: wwnnww  Back: None}</v>
       </c>
     </row>
@@ -4806,19 +4810,19 @@
         <v>122</v>
       </c>
       <c r="F106" t="str">
-        <f>CONCATENATE(A106,"%0Exits are: ",C106)</f>
+        <f t="shared" si="13"/>
         <v>Hairy Trees%0Exits are: N E S</v>
       </c>
       <c r="G106" t="str">
-        <f>CONCATENATE(A106, " -  Room Exits: ", C106, "  Front: ", IF(D106="", "None", D106), "  Back: ", IF(E106="", "None", E106))</f>
+        <f t="shared" si="14"/>
         <v>Hairy Trees -  Room Exits: N E S  Front: esew  Back: None</v>
       </c>
       <c r="H106" t="str">
-        <f>CONCATENATE("#sub {", F106, "} {", G106, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Hairy Trees%0Exits are: N E S} {Hairy Trees -  Room Exits: N E S  Front: esew  Back: None}</v>
       </c>
       <c r="I106" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A106,"} {%0 %1- ",G106, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Hairy Trees} {%0 %1- Hairy Trees -  Room Exits: N E S  Front: esew  Back: None}</v>
       </c>
     </row>
@@ -4836,19 +4840,19 @@
         <v>343</v>
       </c>
       <c r="F107" t="str">
-        <f>CONCATENATE(A107,"%0Exits are: ",C107)</f>
+        <f t="shared" si="13"/>
         <v>Heartless Trees%0Exits are: S W</v>
       </c>
       <c r="G107" t="str">
-        <f>CONCATENATE(A107, " -  Room Exits: ", C107, "  Front: ", IF(D107="", "None", D107), "  Back: ", IF(E107="", "None", E107))</f>
+        <f t="shared" si="14"/>
         <v>Heartless Trees -  Room Exits: S W  Front: wnnwenw  Back: None</v>
       </c>
       <c r="H107" t="str">
-        <f>CONCATENATE("#sub {", F107, "} {", G107, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Heartless Trees%0Exits are: S W} {Heartless Trees -  Room Exits: S W  Front: wnnwenw  Back: None}</v>
       </c>
       <c r="I107" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A107,"} {%0 %1- ",G107, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Heartless Trees} {%0 %1- Heartless Trees -  Room Exits: S W  Front: wnnwenw  Back: None}</v>
       </c>
     </row>
@@ -4866,19 +4870,19 @@
         <v>90</v>
       </c>
       <c r="F108" t="str">
-        <f>CONCATENATE(A108,"%0Exits are: ",C108)</f>
+        <f t="shared" si="13"/>
         <v>Hedge of Thorns%0Exits are: N E S W</v>
       </c>
       <c r="G108" t="str">
-        <f>CONCATENATE(A108, " -  Room Exits: ", C108, "  Front: ", IF(D108="", "None", D108), "  Back: ", IF(E108="", "None", E108))</f>
+        <f t="shared" si="14"/>
         <v>Hedge of Thorns -  Room Exits: N E S W  Front: sessesw  Back: None</v>
       </c>
       <c r="H108" t="str">
-        <f>CONCATENATE("#sub {", F108, "} {", G108, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Hedge of Thorns%0Exits are: N E S W} {Hedge of Thorns -  Room Exits: N E S W  Front: sessesw  Back: None}</v>
       </c>
       <c r="I108" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A108,"} {%0 %1- ",G108, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Hedge of Thorns} {%0 %1- Hedge of Thorns -  Room Exits: N E S W  Front: sessesw  Back: None}</v>
       </c>
     </row>
@@ -4896,19 +4900,19 @@
         <v>352</v>
       </c>
       <c r="F109" t="str">
-        <f>CONCATENATE(A109,"%0Exits are: ",C109)</f>
+        <f t="shared" si="13"/>
         <v>High Up In a Tree%0Exits are: D</v>
       </c>
       <c r="G109" t="str">
-        <f>CONCATENATE(A109, " -  Room Exits: ", C109, "  Front: ", IF(D109="", "None", D109), "  Back: ", IF(E109="", "None", E109))</f>
+        <f t="shared" si="14"/>
         <v>High Up In a Tree -  Room Exits: D  Front: dnnnnnww  Back: None</v>
       </c>
       <c r="H109" t="str">
-        <f>CONCATENATE("#sub {", F109, "} {", G109, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {High Up In a Tree%0Exits are: D} {High Up In a Tree -  Room Exits: D  Front: dnnnnnww  Back: None}</v>
       </c>
       <c r="I109" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A109,"} {%0 %1- ",G109, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- High Up In a Tree} {%0 %1- High Up In a Tree -  Room Exits: D  Front: dnnnnnww  Back: None}</v>
       </c>
     </row>
@@ -4926,19 +4930,19 @@
         <v>291</v>
       </c>
       <c r="F110" t="str">
-        <f>CONCATENATE(A110,"%0Exits are: ",C110)</f>
+        <f t="shared" si="13"/>
         <v>Hollow Tree%0Exits are: N S</v>
       </c>
       <c r="G110" t="str">
-        <f>CONCATENATE(A110, " -  Room Exits: ", C110, "  Front: ", IF(D110="", "None", D110), "  Back: ", IF(E110="", "None", E110))</f>
+        <f t="shared" si="14"/>
         <v>Hollow Tree -  Room Exits: N S  Front: nsew  Back: None</v>
       </c>
       <c r="H110" t="str">
-        <f>CONCATENATE("#sub {", F110, "} {", G110, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Hollow Tree%0Exits are: N S} {Hollow Tree -  Room Exits: N S  Front: nsew  Back: None}</v>
       </c>
       <c r="I110" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A110,"} {%0 %1- ",G110, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Hollow Tree} {%0 %1- Hollow Tree -  Room Exits: N S  Front: nsew  Back: None}</v>
       </c>
     </row>
@@ -4956,19 +4960,19 @@
         <v>8</v>
       </c>
       <c r="F111" t="str">
-        <f>CONCATENATE(A111,"%0Exits are: ",C111)</f>
+        <f t="shared" si="13"/>
         <v>Inky Forest%0Exits are: N W</v>
       </c>
       <c r="G111" t="str">
-        <f>CONCATENATE(A111, " -  Room Exits: ", C111, "  Front: ", IF(D111="", "None", D111), "  Back: ", IF(E111="", "None", E111))</f>
+        <f t="shared" si="14"/>
         <v>Inky Forest -  Room Exits: N W  Front: wnewennw  Back: None</v>
       </c>
       <c r="H111" t="str">
-        <f>CONCATENATE("#sub {", F111, "} {", G111, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Inky Forest%0Exits are: N W} {Inky Forest -  Room Exits: N W  Front: wnewennw  Back: None}</v>
       </c>
       <c r="I111" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A111,"} {%0 %1- ",G111, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Inky Forest} {%0 %1- Inky Forest -  Room Exits: N W  Front: wnewennw  Back: None}</v>
       </c>
     </row>
@@ -4986,19 +4990,19 @@
         <v>390</v>
       </c>
       <c r="F112" t="str">
-        <f>CONCATENATE(A112,"%0Exits are: ",C112)</f>
+        <f t="shared" si="13"/>
         <v>Inside the Cave%0Exits are: S</v>
       </c>
       <c r="G112" t="str">
-        <f>CONCATENATE(A112, " -  Room Exits: ", C112, "  Front: ", IF(D112="", "None", D112), "  Back: ", IF(E112="", "None", E112))</f>
+        <f t="shared" si="14"/>
         <v>Inside the Cave -  Room Exits: S  Front: sewwesewenw  Back: None</v>
       </c>
       <c r="H112" t="str">
-        <f>CONCATENATE("#sub {", F112, "} {", G112, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Inside the Cave%0Exits are: S} {Inside the Cave -  Room Exits: S  Front: sewwesewenw  Back: None}</v>
       </c>
       <c r="I112" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A112,"} {%0 %1- ",G112, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Inside the Cave} {%0 %1- Inside the Cave -  Room Exits: S  Front: sewwesewenw  Back: None}</v>
       </c>
     </row>
@@ -5016,19 +5020,19 @@
         <v>381</v>
       </c>
       <c r="F113" t="str">
-        <f>CONCATENATE(A113,"%0Exits are: ",C113)</f>
+        <f t="shared" si="13"/>
         <v>Into the Swamp%0Exits are: N E W</v>
       </c>
       <c r="G113" t="str">
-        <f>CONCATENATE(A113, " -  Room Exits: ", C113, "  Front: ", IF(D113="", "None", D113), "  Back: ", IF(E113="", "None", E113))</f>
+        <f t="shared" si="14"/>
         <v>Into the Swamp -  Room Exits: N E W  Front: ennsnnnww  Back: None</v>
       </c>
       <c r="H113" t="str">
-        <f>CONCATENATE("#sub {", F113, "} {", G113, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Into the Swamp%0Exits are: N E W} {Into the Swamp -  Room Exits: N E W  Front: ennsnnnww  Back: None}</v>
       </c>
       <c r="I113" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A113,"} {%0 %1- ",G113, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Into the Swamp} {%0 %1- Into the Swamp -  Room Exits: N E W  Front: ennsnnnww  Back: None}</v>
       </c>
     </row>
@@ -5046,19 +5050,19 @@
         <v>168</v>
       </c>
       <c r="F114" t="str">
-        <f>CONCATENATE(A114,"%0Exits are: ",C114)</f>
+        <f t="shared" si="13"/>
         <v>Leaving the Hidden Vale%0Exits are: E W</v>
       </c>
       <c r="G114" t="str">
-        <f>CONCATENATE(A114, " -  Room Exits: ", C114, "  Front: ", IF(D114="", "None", D114), "  Back: ", IF(E114="", "None", E114))</f>
+        <f t="shared" si="14"/>
         <v>Leaving the Hidden Vale -  Room Exits: E W  Front: wnnnnww  Back: None</v>
       </c>
       <c r="H114" t="str">
-        <f>CONCATENATE("#sub {", F114, "} {", G114, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Leaving the Hidden Vale%0Exits are: E W} {Leaving the Hidden Vale -  Room Exits: E W  Front: wnnnnww  Back: None}</v>
       </c>
       <c r="I114" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A114,"} {%0 %1- ",G114, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Leaving the Hidden Vale} {%0 %1- Leaving the Hidden Vale -  Room Exits: E W  Front: wnnnnww  Back: None}</v>
       </c>
     </row>
@@ -5076,19 +5080,19 @@
         <v>116</v>
       </c>
       <c r="F115" t="str">
-        <f>CONCATENATE(A115,"%0Exits are: ",C115)</f>
+        <f t="shared" si="13"/>
         <v>Leaving the Swamp%0Exits are: N E S W</v>
       </c>
       <c r="G115" t="str">
-        <f>CONCATENATE(A115, " -  Room Exits: ", C115, "  Front: ", IF(D115="", "None", D115), "  Back: ", IF(E115="", "None", E115))</f>
+        <f t="shared" si="14"/>
         <v>Leaving the Swamp -  Room Exits: N E S W  Front: sesew  Back: None</v>
       </c>
       <c r="H115" t="str">
-        <f>CONCATENATE("#sub {", F115, "} {", G115, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Leaving the Swamp%0Exits are: N E S W} {Leaving the Swamp -  Room Exits: N E S W  Front: sesew  Back: None}</v>
       </c>
       <c r="I115" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A115,"} {%0 %1- ",G115, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Leaving the Swamp} {%0 %1- Leaving the Swamp -  Room Exits: N E S W  Front: sesew  Back: None}</v>
       </c>
     </row>
@@ -5106,19 +5110,19 @@
         <v>334</v>
       </c>
       <c r="F116" t="str">
-        <f>CONCATENATE(A116,"%0Exits are: ",C116)</f>
+        <f t="shared" si="13"/>
         <v>Lords of the Night%0Exits are: E S</v>
       </c>
       <c r="G116" t="str">
-        <f>CONCATENATE(A116, " -  Room Exits: ", C116, "  Front: ", IF(D116="", "None", D116), "  Back: ", IF(E116="", "None", E116))</f>
+        <f t="shared" si="14"/>
         <v>Lords of the Night -  Room Exits: E S  Front: esswnwenw  Back: None</v>
       </c>
       <c r="H116" t="str">
-        <f>CONCATENATE("#sub {", F116, "} {", G116, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Lords of the Night%0Exits are: E S} {Lords of the Night -  Room Exits: E S  Front: esswnwenw  Back: None}</v>
       </c>
       <c r="I116" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A116,"} {%0 %1- ",G116, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Lords of the Night} {%0 %1- Lords of the Night -  Room Exits: E S  Front: esswnwenw  Back: None}</v>
       </c>
     </row>
@@ -5136,19 +5140,19 @@
         <v>7</v>
       </c>
       <c r="F117" t="str">
-        <f>CONCATENATE(A117,"%0Exits are: ",C117)</f>
+        <f t="shared" si="13"/>
         <v>Lost Amongst the Giants%0Exits are: E S W</v>
       </c>
       <c r="G117" t="str">
-        <f>CONCATENATE(A117, " -  Room Exits: ", C117, "  Front: ", IF(D117="", "None", D117), "  Back: ", IF(E117="", "None", E117))</f>
+        <f t="shared" si="14"/>
         <v>Lost Amongst the Giants -  Room Exits: E S W  Front: wnnewennw  Back: None</v>
       </c>
       <c r="H117" t="str">
-        <f>CONCATENATE("#sub {", F117, "} {", G117, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Lost Amongst the Giants%0Exits are: E S W} {Lost Amongst the Giants -  Room Exits: E S W  Front: wnnewennw  Back: None}</v>
       </c>
       <c r="I117" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A117,"} {%0 %1- ",G117, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Lost Amongst the Giants} {%0 %1- Lost Amongst the Giants -  Room Exits: E S W  Front: wnnewennw  Back: None}</v>
       </c>
     </row>
@@ -5166,19 +5170,19 @@
         <v>74</v>
       </c>
       <c r="F118" t="str">
-        <f>CONCATENATE(A118,"%0Exits are: ",C118)</f>
+        <f t="shared" si="13"/>
         <v>Lost in the Valley%0Exits are: E S</v>
       </c>
       <c r="G118" t="str">
-        <f>CONCATENATE(A118, " -  Room Exits: ", C118, "  Front: ", IF(D118="", "None", D118), "  Back: ", IF(E118="", "None", E118))</f>
+        <f t="shared" si="14"/>
         <v>Lost in the Valley -  Room Exits: E S  Front: ensesw  Back: None</v>
       </c>
       <c r="H118" t="str">
-        <f>CONCATENATE("#sub {", F118, "} {", G118, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Lost in the Valley%0Exits are: E S} {Lost in the Valley -  Room Exits: E S  Front: ensesw  Back: None}</v>
       </c>
       <c r="I118" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A118,"} {%0 %1- ",G118, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Lost in the Valley} {%0 %1- Lost in the Valley -  Room Exits: E S  Front: ensesw  Back: None}</v>
       </c>
     </row>
@@ -5196,19 +5200,19 @@
         <v>173</v>
       </c>
       <c r="F119" t="str">
-        <f>CONCATENATE(A119,"%0Exits are: ",C119)</f>
+        <f t="shared" si="13"/>
         <v>Malevolent Pines%0Exits are: E W</v>
       </c>
       <c r="G119" t="str">
-        <f>CONCATENATE(A119, " -  Room Exits: ", C119, "  Front: ", IF(D119="", "None", D119), "  Back: ", IF(E119="", "None", E119))</f>
+        <f t="shared" si="14"/>
         <v>Malevolent Pines -  Room Exits: E W  Front: ensnsnww  Back: None</v>
       </c>
       <c r="H119" t="str">
-        <f>CONCATENATE("#sub {", F119, "} {", G119, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Malevolent Pines%0Exits are: E W} {Malevolent Pines -  Room Exits: E W  Front: ensnsnww  Back: None}</v>
       </c>
       <c r="I119" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A119,"} {%0 %1- ",G119, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Malevolent Pines} {%0 %1- Malevolent Pines -  Room Exits: E W  Front: ensnsnww  Back: None}</v>
       </c>
     </row>
@@ -5226,19 +5230,19 @@
         <v>200</v>
       </c>
       <c r="F120" t="str">
-        <f>CONCATENATE(A120,"%0Exits are: ",C120)</f>
+        <f t="shared" si="13"/>
         <v>Massive Oaks%0Exits are: N E</v>
       </c>
       <c r="G120" t="str">
-        <f>CONCATENATE(A120, " -  Room Exits: ", C120, "  Front: ", IF(D120="", "None", D120), "  Back: ", IF(E120="", "None", E120))</f>
+        <f t="shared" si="14"/>
         <v>Massive Oaks -  Room Exits: N E  Front: enw  Back: None</v>
       </c>
       <c r="H120" t="str">
-        <f>CONCATENATE("#sub {", F120, "} {", G120, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Massive Oaks%0Exits are: N E} {Massive Oaks -  Room Exits: N E  Front: enw  Back: None}</v>
       </c>
       <c r="I120" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A120,"} {%0 %1- ",G120, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Massive Oaks} {%0 %1- Massive Oaks -  Room Exits: N E  Front: enw  Back: None}</v>
       </c>
     </row>
@@ -5256,19 +5260,19 @@
         <v>319</v>
       </c>
       <c r="F121" t="str">
-        <f>CONCATENATE(A121,"%0Exits are: ",C121)</f>
+        <f t="shared" si="13"/>
         <v>Mat of Death%0Exits are: E S</v>
       </c>
       <c r="G121" t="str">
-        <f>CONCATENATE(A121, " -  Room Exits: ", C121, "  Front: ", IF(D121="", "None", D121), "  Back: ", IF(E121="", "None", E121))</f>
+        <f t="shared" si="14"/>
         <v>Mat of Death -  Room Exits: E S  Front: enwesew  Back: None</v>
       </c>
       <c r="H121" t="str">
-        <f>CONCATENATE("#sub {", F121, "} {", G121, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Mat of Death%0Exits are: E S} {Mat of Death -  Room Exits: E S  Front: enwesew  Back: None}</v>
       </c>
       <c r="I121" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A121,"} {%0 %1- ",G121, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Mat of Death} {%0 %1- Mat of Death -  Room Exits: E S  Front: enwesew  Back: None}</v>
       </c>
     </row>
@@ -5286,19 +5290,19 @@
         <v>329</v>
       </c>
       <c r="F122" t="str">
-        <f>CONCATENATE(A122,"%0Exits are: ",C122)</f>
+        <f t="shared" si="13"/>
         <v>Maze of Bracken%0Exits are: N S</v>
       </c>
       <c r="G122" t="str">
-        <f>CONCATENATE(A122, " -  Room Exits: ", C122, "  Front: ", IF(D122="", "None", D122), "  Back: ", IF(E122="", "None", E122))</f>
+        <f t="shared" si="14"/>
         <v>Maze of Bracken -  Room Exits: N S  Front: nsnnnww  Back: None</v>
       </c>
       <c r="H122" t="str">
-        <f>CONCATENATE("#sub {", F122, "} {", G122, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Maze of Bracken%0Exits are: N S} {Maze of Bracken -  Room Exits: N S  Front: nsnnnww  Back: None}</v>
       </c>
       <c r="I122" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A122,"} {%0 %1- ",G122, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Maze of Bracken} {%0 %1- Maze of Bracken -  Room Exits: N S  Front: nsnnnww  Back: None}</v>
       </c>
     </row>
@@ -5313,19 +5317,19 @@
         <v>76</v>
       </c>
       <c r="F123" t="str">
-        <f>CONCATENATE(A123,"%0Exits are: ",C123)</f>
+        <f t="shared" si="13"/>
         <v>Mirkwood%0Exits are: E S</v>
       </c>
       <c r="G123" t="str">
-        <f>CONCATENATE(A123, " -  Room Exits: ", C123, "  Front: ", IF(D123="", "None", D123), "  Back: ", IF(E123="", "None", E123))</f>
+        <f t="shared" si="14"/>
         <v>Mirkwood -  Room Exits: E S  Front: ssnnww  Back: None</v>
       </c>
       <c r="H123" t="str">
-        <f>CONCATENATE("#sub {", F123, "} {", G123, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Mirkwood%0Exits are: E S} {Mirkwood -  Room Exits: E S  Front: ssnnww  Back: None}</v>
       </c>
       <c r="I123" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A123,"} {%0 %1- ",G123, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Mirkwood} {%0 %1- Mirkwood -  Room Exits: E S  Front: ssnnww  Back: None}</v>
       </c>
     </row>
@@ -5343,19 +5347,19 @@
         <v>110</v>
       </c>
       <c r="F124" t="str">
-        <f>CONCATENATE(A124,"%0Exits are: ",C124)</f>
+        <f t="shared" si="13"/>
         <v>Mist%0Exits are: N E W</v>
       </c>
       <c r="G124" t="str">
-        <f>CONCATENATE(A124, " -  Room Exits: ", C124, "  Front: ", IF(D124="", "None", D124), "  Back: ", IF(E124="", "None", E124))</f>
+        <f t="shared" si="14"/>
         <v>Mist -  Room Exits: N E W  Front: wesew  Back: None</v>
       </c>
       <c r="H124" t="str">
-        <f>CONCATENATE("#sub {", F124, "} {", G124, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Mist%0Exits are: N E W} {Mist -  Room Exits: N E W  Front: wesew  Back: None}</v>
       </c>
       <c r="I124" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A124,"} {%0 %1- ",G124, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Mist} {%0 %1- Mist -  Room Exits: N E W  Front: wesew  Back: None}</v>
       </c>
     </row>
@@ -5373,19 +5377,19 @@
         <v>251</v>
       </c>
       <c r="F125" t="str">
-        <f>CONCATENATE(A125,"%0Exits are: ",C125)</f>
+        <f t="shared" si="13"/>
         <v>Mist Covered Bog%0Exits are: N S</v>
       </c>
       <c r="G125" t="str">
-        <f>CONCATENATE(A125, " -  Room Exits: ", C125, "  Front: ", IF(D125="", "None", D125), "  Back: ", IF(E125="", "None", E125))</f>
+        <f t="shared" si="14"/>
         <v>Mist Covered Bog -  Room Exits: N S  Front: newennw  Back: None</v>
       </c>
       <c r="H125" t="str">
-        <f>CONCATENATE("#sub {", F125, "} {", G125, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Mist Covered Bog%0Exits are: N S} {Mist Covered Bog -  Room Exits: N S  Front: newennw  Back: None}</v>
       </c>
       <c r="I125" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A125,"} {%0 %1- ",G125, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Mist Covered Bog} {%0 %1- Mist Covered Bog -  Room Exits: N S  Front: newennw  Back: None}</v>
       </c>
     </row>
@@ -5403,19 +5407,19 @@
         <v>126</v>
       </c>
       <c r="F126" t="str">
-        <f>CONCATENATE(A126,"%0Exits are: ",C126)</f>
+        <f t="shared" si="13"/>
         <v>Moist Breeze%0Exits are: N E</v>
       </c>
       <c r="G126" t="str">
-        <f>CONCATENATE(A126, " -  Room Exits: ", C126, "  Front: ", IF(D126="", "None", D126), "  Back: ", IF(E126="", "None", E126))</f>
+        <f t="shared" si="14"/>
         <v>Moist Breeze -  Room Exits: N E  Front: eewennw  Back: None</v>
       </c>
       <c r="H126" t="str">
-        <f>CONCATENATE("#sub {", F126, "} {", G126, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Moist Breeze%0Exits are: N E} {Moist Breeze -  Room Exits: N E  Front: eewennw  Back: None}</v>
       </c>
       <c r="I126" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A126,"} {%0 %1- ",G126, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Moist Breeze} {%0 %1- Moist Breeze -  Room Exits: N E  Front: eewennw  Back: None}</v>
       </c>
     </row>
@@ -5433,19 +5437,19 @@
         <v>56</v>
       </c>
       <c r="F127" t="str">
-        <f>CONCATENATE(A127,"%0Exits are: ",C127)</f>
+        <f t="shared" si="13"/>
         <v>Moody Trees%0Exits are: N E S</v>
       </c>
       <c r="G127" t="str">
-        <f>CONCATENATE(A127, " -  Room Exits: ", C127, "  Front: ", IF(D127="", "None", D127), "  Back: ", IF(E127="", "None", E127))</f>
+        <f t="shared" si="14"/>
         <v>Moody Trees -  Room Exits: N E S  Front: nwenw  Back: None</v>
       </c>
       <c r="H127" t="str">
-        <f>CONCATENATE("#sub {", F127, "} {", G127, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Moody Trees%0Exits are: N E S} {Moody Trees -  Room Exits: N E S  Front: nwenw  Back: None}</v>
       </c>
       <c r="I127" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A127,"} {%0 %1- ",G127, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Moody Trees} {%0 %1- Moody Trees -  Room Exits: N E S  Front: nwenw  Back: None}</v>
       </c>
     </row>
@@ -5463,19 +5467,19 @@
         <v>398</v>
       </c>
       <c r="F128" t="str">
-        <f>CONCATENATE(A128,"%0Exits are: ",C128)</f>
+        <f t="shared" si="13"/>
         <v>Mosquito Infested Waters%0Exits are: N S W</v>
       </c>
       <c r="G128" t="str">
-        <f>CONCATENATE(A128, " -  Room Exits: ", C128, "  Front: ", IF(D128="", "None", D128), "  Back: ", IF(E128="", "None", E128))</f>
+        <f t="shared" si="14"/>
         <v>Mosquito Infested Waters -  Room Exits: N S W  Front: nsnnewennw  Back: None</v>
       </c>
       <c r="H128" t="str">
-        <f>CONCATENATE("#sub {", F128, "} {", G128, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Mosquito Infested Waters%0Exits are: N S W} {Mosquito Infested Waters -  Room Exits: N S W  Front: nsnnewennw  Back: None}</v>
       </c>
       <c r="I128" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A128,"} {%0 %1- ",G128, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Mosquito Infested Waters} {%0 %1- Mosquito Infested Waters -  Room Exits: N S W  Front: nsnnewennw  Back: None}</v>
       </c>
     </row>
@@ -5493,19 +5497,19 @@
         <v>358</v>
       </c>
       <c r="F129" t="str">
-        <f>CONCATENATE(A129,"%0Exits are: ",C129)</f>
+        <f t="shared" si="13"/>
         <v>Mossy Trees%0Exits are: N E</v>
       </c>
       <c r="G129" t="str">
-        <f>CONCATENATE(A129, " -  Room Exits: ", C129, "  Front: ", IF(D129="", "None", D129), "  Back: ", IF(E129="", "None", E129))</f>
+        <f t="shared" si="14"/>
         <v>Mossy Trees -  Room Exits: N E  Front: ewnnwenw  Back: None</v>
       </c>
       <c r="H129" t="str">
-        <f>CONCATENATE("#sub {", F129, "} {", G129, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Mossy Trees%0Exits are: N E} {Mossy Trees -  Room Exits: N E  Front: ewnnwenw  Back: None}</v>
       </c>
       <c r="I129" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A129,"} {%0 %1- ",G129, "}")</f>
+        <f t="shared" si="15"/>
         <v>#sub {%0 %1- Mossy Trees} {%0 %1- Mossy Trees -  Room Exits: N E  Front: ewnnwenw  Back: None}</v>
       </c>
     </row>
@@ -5523,19 +5527,19 @@
         <v>378</v>
       </c>
       <c r="F130" t="str">
-        <f>CONCATENATE(A130,"%0Exits are: ",C130)</f>
+        <f t="shared" ref="F130:F161" si="17">CONCATENATE(A130,"%0Exits are: ",C130)</f>
         <v>Motionless Swamp%0Exits are: N E W</v>
       </c>
       <c r="G130" t="str">
-        <f>CONCATENATE(A130, " -  Room Exits: ", C130, "  Front: ", IF(D130="", "None", D130), "  Back: ", IF(E130="", "None", E130))</f>
+        <f t="shared" ref="G130:G161" si="18">CONCATENATE(A130, " -  Room Exits: ", C130, "  Front: ", IF(D130="", "None", D130), "  Back: ", IF(E130="", "None", E130))</f>
         <v>Motionless Swamp -  Room Exits: N E W  Front: nnsnnnww  Back: None</v>
       </c>
       <c r="H130" t="str">
-        <f>CONCATENATE("#sub {", F130, "} {", G130, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Motionless Swamp%0Exits are: N E W} {Motionless Swamp -  Room Exits: N E W  Front: nnsnnnww  Back: None}</v>
       </c>
       <c r="I130" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A130,"} {%0 %1- ",G130, "}")</f>
+        <f t="shared" ref="I130:I161" si="19">CONCATENATE("#sub {%0 %1- ",A130,"} {%0 %1- ",G130, "}")</f>
         <v>#sub {%0 %1- Motionless Swamp} {%0 %1- Motionless Swamp -  Room Exits: N E W  Front: nnsnnnww  Back: None}</v>
       </c>
     </row>
@@ -5553,19 +5557,19 @@
         <v>220</v>
       </c>
       <c r="F131" t="str">
-        <f>CONCATENATE(A131,"%0Exits are: ",C131)</f>
+        <f t="shared" si="17"/>
         <v>Muddy Path%0Exits are: N S W</v>
       </c>
       <c r="G131" t="str">
-        <f>CONCATENATE(A131, " -  Room Exits: ", C131, "  Front: ", IF(D131="", "None", D131), "  Back: ", IF(E131="", "None", E131))</f>
+        <f t="shared" si="18"/>
         <v>Muddy Path -  Room Exits: N S W  Front: wwww  Back: None</v>
       </c>
       <c r="H131" t="str">
-        <f>CONCATENATE("#sub {", F131, "} {", G131, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Muddy Path%0Exits are: N S W} {Muddy Path -  Room Exits: N S W  Front: wwww  Back: None}</v>
       </c>
       <c r="I131" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A131,"} {%0 %1- ",G131, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Muddy Path} {%0 %1- Muddy Path -  Room Exits: N S W  Front: wwww  Back: None}</v>
       </c>
     </row>
@@ -5583,19 +5587,19 @@
         <v>413</v>
       </c>
       <c r="F132" t="str">
-        <f>CONCATENATE(A132,"%0Exits are: ",C132)</f>
+        <f t="shared" si="17"/>
         <v>Murky Waters%0Exits are: N E</v>
       </c>
       <c r="G132" t="str">
-        <f>CONCATENATE(A132, " -  Room Exits: ", C132, "  Front: ", IF(D132="", "None", D132), "  Back: ", IF(E132="", "None", E132))</f>
+        <f t="shared" si="18"/>
         <v>Murky Waters -  Room Exits: N E  Front: eeennsnnnww  Back: None</v>
       </c>
       <c r="H132" t="str">
-        <f>CONCATENATE("#sub {", F132, "} {", G132, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Murky Waters%0Exits are: N E} {Murky Waters -  Room Exits: N E  Front: eeennsnnnww  Back: None}</v>
       </c>
       <c r="I132" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A132,"} {%0 %1- ",G132, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Murky Waters} {%0 %1- Murky Waters -  Room Exits: N E  Front: eeennsnnnww  Back: None}</v>
       </c>
     </row>
@@ -5613,19 +5617,19 @@
         <v>9</v>
       </c>
       <c r="F133" t="str">
-        <f>CONCATENATE(A133,"%0Exits are: ",C133)</f>
+        <f t="shared" si="17"/>
         <v>Obsidian Wood%0Exits are: E S</v>
       </c>
       <c r="G133" t="str">
-        <f>CONCATENATE(A133, " -  Room Exits: ", C133, "  Front: ", IF(D133="", "None", D133), "  Back: ", IF(E133="", "None", E133))</f>
+        <f t="shared" si="18"/>
         <v>Obsidian Wood -  Room Exits: E S  Front: enenw  Back: None</v>
       </c>
       <c r="H133" t="str">
-        <f>CONCATENATE("#sub {", F133, "} {", G133, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Obsidian Wood%0Exits are: E S} {Obsidian Wood -  Room Exits: E S  Front: enenw  Back: None}</v>
       </c>
       <c r="I133" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A133,"} {%0 %1- ",G133, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Obsidian Wood} {%0 %1- Obsidian Wood -  Room Exits: E S  Front: enenw  Back: None}</v>
       </c>
     </row>
@@ -5643,19 +5647,19 @@
         <v>306</v>
       </c>
       <c r="F134" t="str">
-        <f>CONCATENATE(A134,"%0Exits are: ",C134)</f>
+        <f t="shared" si="17"/>
         <v>Old Forest%0Exits are: E S</v>
       </c>
       <c r="G134" t="str">
-        <f>CONCATENATE(A134, " -  Room Exits: ", C134, "  Front: ", IF(D134="", "None", D134), "  Back: ", IF(E134="", "None", E134))</f>
+        <f t="shared" si="18"/>
         <v>Old Forest -  Room Exits: E S  Front: ewennw  Back: None</v>
       </c>
       <c r="H134" t="str">
-        <f>CONCATENATE("#sub {", F134, "} {", G134, "}")</f>
+        <f t="shared" si="16"/>
         <v>#sub {Old Forest%0Exits are: E S} {Old Forest -  Room Exits: E S  Front: ewennw  Back: None}</v>
       </c>
       <c r="I134" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A134,"} {%0 %1- ",G134, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Old Forest} {%0 %1- Old Forest -  Room Exits: E S  Front: ewennw  Back: None}</v>
       </c>
     </row>
@@ -5673,19 +5677,19 @@
         <v>399</v>
       </c>
       <c r="F135" t="str">
-        <f>CONCATENATE(A135,"%0Exits are: ",C135)</f>
+        <f t="shared" si="17"/>
         <v>On Spongy Ground%0Exits are: N E W</v>
       </c>
       <c r="G135" t="str">
-        <f>CONCATENATE(A135, " -  Room Exits: ", C135, "  Front: ", IF(D135="", "None", D135), "  Back: ", IF(E135="", "None", E135))</f>
+        <f t="shared" si="18"/>
         <v>On Spongy Ground -  Room Exits: N E W  Front: ewnnsnnnww  Back: None</v>
       </c>
       <c r="H135" t="str">
-        <f>CONCATENATE("#sub {", F135, "} {", G135, "}")</f>
+        <f t="shared" ref="H135:H166" si="20">CONCATENATE("#sub {", F135, "} {", G135, "}")</f>
         <v>#sub {On Spongy Ground%0Exits are: N E W} {On Spongy Ground -  Room Exits: N E W  Front: ewnnsnnnww  Back: None}</v>
       </c>
       <c r="I135" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A135,"} {%0 %1- ",G135, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- On Spongy Ground} {%0 %1- On Spongy Ground -  Room Exits: N E W  Front: ewnnsnnnww  Back: None}</v>
       </c>
     </row>
@@ -5703,19 +5707,19 @@
         <v>322</v>
       </c>
       <c r="F136" t="str">
-        <f>CONCATENATE(A136,"%0Exits are: ",C136)</f>
+        <f t="shared" si="17"/>
         <v>Opaque Darkness%0Exits are: N E W</v>
       </c>
       <c r="G136" t="str">
-        <f>CONCATENATE(A136, " -  Room Exits: ", C136, "  Front: ", IF(D136="", "None", D136), "  Back: ", IF(E136="", "None", E136))</f>
+        <f t="shared" si="18"/>
         <v>Opaque Darkness -  Room Exits: N E W  Front: esesw  Back: None</v>
       </c>
       <c r="H136" t="str">
-        <f>CONCATENATE("#sub {", F136, "} {", G136, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Opaque Darkness%0Exits are: N E W} {Opaque Darkness -  Room Exits: N E W  Front: esesw  Back: None}</v>
       </c>
       <c r="I136" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A136,"} {%0 %1- ",G136, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Opaque Darkness} {%0 %1- Opaque Darkness -  Room Exits: N E W  Front: esesw  Back: None}</v>
       </c>
     </row>
@@ -5733,19 +5737,19 @@
         <v>355</v>
       </c>
       <c r="F137" t="str">
-        <f>CONCATENATE(A137,"%0Exits are: ",C137)</f>
+        <f t="shared" si="17"/>
         <v>Oppressive Feeling%0Exits are: E W</v>
       </c>
       <c r="G137" t="str">
-        <f>CONCATENATE(A137, " -  Room Exits: ", C137, "  Front: ", IF(D137="", "None", D137), "  Back: ", IF(E137="", "None", E137))</f>
+        <f t="shared" si="18"/>
         <v>Oppressive Feeling -  Room Exits: E W  Front: www  Back: None</v>
       </c>
       <c r="H137" t="str">
-        <f>CONCATENATE("#sub {", F137, "} {", G137, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Oppressive Feeling%0Exits are: E W} {Oppressive Feeling -  Room Exits: E W  Front: www  Back: None}</v>
       </c>
       <c r="I137" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A137,"} {%0 %1- ",G137, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Oppressive Feeling} {%0 %1- Oppressive Feeling -  Room Exits: E W  Front: www  Back: None}</v>
       </c>
     </row>
@@ -5763,19 +5767,19 @@
         <v>389</v>
       </c>
       <c r="F138" t="str">
-        <f>CONCATENATE(A138,"%0Exits are: ",C138)</f>
+        <f t="shared" si="17"/>
         <v>Outside a Cave%0Exits are: N E</v>
       </c>
       <c r="G138" t="str">
-        <f>CONCATENATE(A138, " -  Room Exits: ", C138, "  Front: ", IF(D138="", "None", D138), "  Back: ", IF(E138="", "None", E138))</f>
+        <f t="shared" si="18"/>
         <v>Outside a Cave -  Room Exits: N E  Front: ewwesewenw  Back: None</v>
       </c>
       <c r="H138" t="str">
-        <f>CONCATENATE("#sub {", F138, "} {", G138, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Outside a Cave%0Exits are: N E} {Outside a Cave -  Room Exits: N E  Front: ewwesewenw  Back: None}</v>
       </c>
       <c r="I138" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A138,"} {%0 %1- ",G138, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Outside a Cave} {%0 %1- Outside a Cave -  Room Exits: N E  Front: ewwesewenw  Back: None}</v>
       </c>
     </row>
@@ -5793,19 +5797,19 @@
         <v>183</v>
       </c>
       <c r="F139" t="str">
-        <f>CONCATENATE(A139,"%0Exits are: ",C139)</f>
+        <f t="shared" si="17"/>
         <v>Overt Malice%0Exits are: N E</v>
       </c>
       <c r="G139" t="str">
-        <f>CONCATENATE(A139, " -  Room Exits: ", C139, "  Front: ", IF(D139="", "None", D139), "  Back: ", IF(E139="", "None", E139))</f>
+        <f t="shared" si="18"/>
         <v>Overt Malice -  Room Exits: N E  Front: nnwenw  Back: None</v>
       </c>
       <c r="H139" t="str">
-        <f>CONCATENATE("#sub {", F139, "} {", G139, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Overt Malice%0Exits are: N E} {Overt Malice -  Room Exits: N E  Front: nnwenw  Back: None}</v>
       </c>
       <c r="I139" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A139,"} {%0 %1- ",G139, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Overt Malice} {%0 %1- Overt Malice -  Room Exits: N E  Front: nnwenw  Back: None}</v>
       </c>
     </row>
@@ -5823,19 +5827,19 @@
         <v>272</v>
       </c>
       <c r="F140" t="str">
-        <f>CONCATENATE(A140,"%0Exits are: ",C140)</f>
+        <f t="shared" si="17"/>
         <v>Pale Mist%0Exits are: N E S</v>
       </c>
       <c r="G140" t="str">
-        <f>CONCATENATE(A140, " -  Room Exits: ", C140, "  Front: ", IF(D140="", "None", D140), "  Back: ", IF(E140="", "None", E140))</f>
+        <f t="shared" si="18"/>
         <v>Pale Mist -  Room Exits: N E S  Front: ew  Back: None</v>
       </c>
       <c r="H140" t="str">
-        <f>CONCATENATE("#sub {", F140, "} {", G140, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Pale Mist%0Exits are: N E S} {Pale Mist -  Room Exits: N E S  Front: ew  Back: None}</v>
       </c>
       <c r="I140" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A140,"} {%0 %1- ",G140, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Pale Mist} {%0 %1- Pale Mist -  Room Exits: N E S  Front: ew  Back: None}</v>
       </c>
     </row>
@@ -5853,19 +5857,19 @@
         <v>211</v>
       </c>
       <c r="F141" t="str">
-        <f>CONCATENATE(A141,"%0Exits are: ",C141)</f>
+        <f t="shared" si="17"/>
         <v>Pale Shroud%0Exits are: E S W</v>
       </c>
       <c r="G141" t="str">
-        <f>CONCATENATE(A141, " -  Room Exits: ", C141, "  Front: ", IF(D141="", "None", D141), "  Back: ", IF(E141="", "None", E141))</f>
+        <f t="shared" si="18"/>
         <v>Pale Shroud -  Room Exits: E S W  Front: ensnww  Back: None</v>
       </c>
       <c r="H141" t="str">
-        <f>CONCATENATE("#sub {", F141, "} {", G141, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Pale Shroud%0Exits are: E S W} {Pale Shroud -  Room Exits: E S W  Front: ensnww  Back: None}</v>
       </c>
       <c r="I141" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A141,"} {%0 %1- ",G141, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Pale Shroud} {%0 %1- Pale Shroud -  Room Exits: E S W  Front: ensnww  Back: None}</v>
       </c>
     </row>
@@ -5883,19 +5887,19 @@
         <v>332</v>
       </c>
       <c r="F142" t="str">
-        <f>CONCATENATE(A142,"%0Exits are: ",C142)</f>
+        <f t="shared" si="17"/>
         <v>Patch of Mushrooms%0Exits are: S W</v>
       </c>
       <c r="G142" t="str">
-        <f>CONCATENATE(A142, " -  Room Exits: ", C142, "  Front: ", IF(D142="", "None", D142), "  Back: ", IF(E142="", "None", E142))</f>
+        <f t="shared" si="18"/>
         <v>Patch of Mushrooms -  Room Exits: S W  Front: wwnew  Back: None</v>
       </c>
       <c r="H142" t="str">
-        <f>CONCATENATE("#sub {", F142, "} {", G142, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Patch of Mushrooms%0Exits are: S W} {Patch of Mushrooms -  Room Exits: S W  Front: wwnew  Back: None}</v>
       </c>
       <c r="I142" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A142,"} {%0 %1- ",G142, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Patch of Mushrooms} {%0 %1- Patch of Mushrooms -  Room Exits: S W  Front: wwnew  Back: None}</v>
       </c>
     </row>
@@ -5913,19 +5917,19 @@
         <v>311</v>
       </c>
       <c r="F143" t="str">
-        <f>CONCATENATE(A143,"%0Exits are: ",C143)</f>
+        <f t="shared" si="17"/>
         <v>Pressing Darkness%0Exits are: N E S</v>
       </c>
       <c r="G143" t="str">
-        <f>CONCATENATE(A143, " -  Room Exits: ", C143, "  Front: ", IF(D143="", "None", D143), "  Back: ", IF(E143="", "None", E143))</f>
+        <f t="shared" si="18"/>
         <v>Pressing Darkness -  Room Exits: N E S  Front: nensnww  Back: None</v>
       </c>
       <c r="H143" t="str">
-        <f>CONCATENATE("#sub {", F143, "} {", G143, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Pressing Darkness%0Exits are: N E S} {Pressing Darkness -  Room Exits: N E S  Front: nensnww  Back: None}</v>
       </c>
       <c r="I143" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A143,"} {%0 %1- ",G143, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Pressing Darkness} {%0 %1- Pressing Darkness -  Room Exits: N E S  Front: nensnww  Back: None}</v>
       </c>
     </row>
@@ -5943,19 +5947,19 @@
         <v>89</v>
       </c>
       <c r="F144" t="str">
-        <f>CONCATENATE(A144,"%0Exits are: ",C144)</f>
+        <f t="shared" si="17"/>
         <v>Quiet Corner%0Exits are: N E W</v>
       </c>
       <c r="G144" t="str">
-        <f>CONCATENATE(A144, " -  Room Exits: ", C144, "  Front: ", IF(D144="", "None", D144), "  Back: ", IF(E144="", "None", E144))</f>
+        <f t="shared" si="18"/>
         <v>Quiet Corner -  Room Exits: N E W  Front: essesw  Back: None</v>
       </c>
       <c r="H144" t="str">
-        <f>CONCATENATE("#sub {", F144, "} {", G144, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Quiet Corner%0Exits are: N E W} {Quiet Corner -  Room Exits: N E W  Front: essesw  Back: None}</v>
       </c>
       <c r="I144" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A144,"} {%0 %1- ",G144, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Quiet Corner} {%0 %1- Quiet Corner -  Room Exits: N E W  Front: essesw  Back: None}</v>
       </c>
     </row>
@@ -5973,19 +5977,19 @@
         <v>345</v>
       </c>
       <c r="F145" t="str">
-        <f>CONCATENATE(A145,"%0Exits are: ",C145)</f>
+        <f t="shared" si="17"/>
         <v>Random Stones%0Exits are: N E</v>
       </c>
       <c r="G145" t="str">
-        <f>CONCATENATE(A145, " -  Room Exits: ", C145, "  Front: ", IF(D145="", "None", D145), "  Back: ", IF(E145="", "None", E145))</f>
+        <f t="shared" si="18"/>
         <v>Random Stones -  Room Exits: N E  Front: newenw  Back: None</v>
       </c>
       <c r="H145" t="str">
-        <f>CONCATENATE("#sub {", F145, "} {", G145, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Random Stones%0Exits are: N E} {Random Stones -  Room Exits: N E  Front: newenw  Back: None}</v>
       </c>
       <c r="I145" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A145,"} {%0 %1- ",G145, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Random Stones} {%0 %1- Random Stones -  Room Exits: N E  Front: newenw  Back: None}</v>
       </c>
     </row>
@@ -6003,19 +6007,19 @@
         <v>392</v>
       </c>
       <c r="F146" t="str">
-        <f>CONCATENATE(A146,"%0Exits are: ",C146)</f>
+        <f t="shared" si="17"/>
         <v>Reaching Branches%0Exits are: N S W</v>
       </c>
       <c r="G146" t="str">
-        <f>CONCATENATE(A146, " -  Room Exits: ", C146, "  Front: ", IF(D146="", "None", D146), "  Back: ", IF(E146="", "None", E146))</f>
+        <f t="shared" si="18"/>
         <v>Reaching Branches -  Room Exits: N S W  Front: wssw  Back: None</v>
       </c>
       <c r="H146" t="str">
-        <f>CONCATENATE("#sub {", F146, "} {", G146, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Reaching Branches%0Exits are: N S W} {Reaching Branches -  Room Exits: N S W  Front: wssw  Back: None}</v>
       </c>
       <c r="I146" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A146,"} {%0 %1- ",G146, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Reaching Branches} {%0 %1- Reaching Branches -  Room Exits: N S W  Front: wssw  Back: None}</v>
       </c>
     </row>
@@ -6036,19 +6040,19 @@
         <v>54</v>
       </c>
       <c r="F147" t="str">
-        <f>CONCATENATE(A147,"%0Exits are: ",C147)</f>
+        <f t="shared" si="17"/>
         <v>Returning to the Forest%0Exits are: N E W</v>
       </c>
       <c r="G147" t="str">
-        <f>CONCATENATE(A147, " -  Room Exits: ", C147, "  Front: ", IF(D147="", "None", D147), "  Back: ", IF(E147="", "None", E147))</f>
+        <f t="shared" si="18"/>
         <v>Returning to the Forest -  Room Exits: N E W  Front: wenw  Back: eeseeneenesene</v>
       </c>
       <c r="H147" t="str">
-        <f>CONCATENATE("#sub {", F147, "} {", G147, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Returning to the Forest%0Exits are: N E W} {Returning to the Forest -  Room Exits: N E W  Front: wenw  Back: eeseeneenesene}</v>
       </c>
       <c r="I147" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A147,"} {%0 %1- ",G147, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Returning to the Forest} {%0 %1- Returning to the Forest -  Room Exits: N E W  Front: wenw  Back: eeseeneenesene}</v>
       </c>
     </row>
@@ -6066,19 +6070,19 @@
         <v>61</v>
       </c>
       <c r="F148" t="str">
-        <f>CONCATENATE(A148,"%0Exits are: ",C148)</f>
+        <f t="shared" si="17"/>
         <v>Ring of Stones%0Exits are: N S</v>
       </c>
       <c r="G148" t="str">
-        <f>CONCATENATE(A148, " -  Room Exits: ", C148, "  Front: ", IF(D148="", "None", D148), "  Back: ", IF(E148="", "None", E148))</f>
+        <f t="shared" si="18"/>
         <v>Ring of Stones -  Room Exits: N S  Front: ssnww  Back: None</v>
       </c>
       <c r="H148" t="str">
-        <f>CONCATENATE("#sub {", F148, "} {", G148, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Ring of Stones%0Exits are: N S} {Ring of Stones -  Room Exits: N S  Front: ssnww  Back: None}</v>
       </c>
       <c r="I148" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A148,"} {%0 %1- ",G148, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Ring of Stones} {%0 %1- Ring of Stones -  Room Exits: N S  Front: ssnww  Back: None}</v>
       </c>
     </row>
@@ -6096,19 +6100,19 @@
         <v>251</v>
       </c>
       <c r="F149" t="str">
-        <f>CONCATENATE(A149,"%0Exits are: ",C149)</f>
+        <f t="shared" si="17"/>
         <v>Rising Forest%0Exits are: N E S W</v>
       </c>
       <c r="G149" t="str">
-        <f>CONCATENATE(A149, " -  Room Exits: ", C149, "  Front: ", IF(D149="", "None", D149), "  Back: ", IF(E149="", "None", E149))</f>
+        <f t="shared" si="18"/>
         <v>Rising Forest -  Room Exits: N E S W  Front: newennw  Back: None</v>
       </c>
       <c r="H149" t="str">
-        <f>CONCATENATE("#sub {", F149, "} {", G149, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Rising Forest%0Exits are: N E S W} {Rising Forest -  Room Exits: N E S W  Front: newennw  Back: None}</v>
       </c>
       <c r="I149" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A149,"} {%0 %1- ",G149, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Rising Forest} {%0 %1- Rising Forest -  Room Exits: N E S W  Front: newennw  Back: None}</v>
       </c>
     </row>
@@ -6126,19 +6130,19 @@
         <v>106</v>
       </c>
       <c r="F150" t="str">
-        <f>CONCATENATE(A150,"%0Exits are: ",C150)</f>
+        <f t="shared" si="17"/>
         <v>Rocky Forest Floor%0Exits are: E S W</v>
       </c>
       <c r="G150" t="str">
-        <f>CONCATENATE(A150, " -  Room Exits: ", C150, "  Front: ", IF(D150="", "None", D150), "  Back: ", IF(E150="", "None", E150))</f>
+        <f t="shared" si="18"/>
         <v>Rocky Forest Floor -  Room Exits: E S W  Front: esnnww  Back: None</v>
       </c>
       <c r="H150" t="str">
-        <f>CONCATENATE("#sub {", F150, "} {", G150, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Rocky Forest Floor%0Exits are: E S W} {Rocky Forest Floor -  Room Exits: E S W  Front: esnnww  Back: None}</v>
       </c>
       <c r="I150" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A150,"} {%0 %1- ",G150, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Rocky Forest Floor} {%0 %1- Rocky Forest Floor -  Room Exits: E S W  Front: esnnww  Back: None}</v>
       </c>
     </row>
@@ -6156,19 +6160,19 @@
         <v>331</v>
       </c>
       <c r="F151" t="str">
-        <f>CONCATENATE(A151,"%0Exits are: ",C151)</f>
+        <f t="shared" si="17"/>
         <v>Rotting Beeches%0Exits are: N E W</v>
       </c>
       <c r="G151" t="str">
-        <f>CONCATENATE(A151, " -  Room Exits: ", C151, "  Front: ", IF(D151="", "None", D151), "  Back: ", IF(E151="", "None", E151))</f>
+        <f t="shared" si="18"/>
         <v>Rotting Beeches -  Room Exits: N E W  Front: wnew  Back: None</v>
       </c>
       <c r="H151" t="str">
-        <f>CONCATENATE("#sub {", F151, "} {", G151, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Rotting Beeches%0Exits are: N E W} {Rotting Beeches -  Room Exits: N E W  Front: wnew  Back: None}</v>
       </c>
       <c r="I151" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A151,"} {%0 %1- ",G151, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Rotting Beeches} {%0 %1- Rotting Beeches -  Room Exits: N E W  Front: wnew  Back: None}</v>
       </c>
     </row>
@@ -6186,19 +6190,19 @@
         <v>4</v>
       </c>
       <c r="F152" t="str">
-        <f>CONCATENATE(A152,"%0Exits are: ",C152)</f>
+        <f t="shared" si="17"/>
         <v>Rotting Treestump%0Exits are: N S W</v>
       </c>
       <c r="G152" t="str">
-        <f>CONCATENATE(A152, " -  Room Exits: ", C152, "  Front: ", IF(D152="", "None", D152), "  Back: ", IF(E152="", "None", E152))</f>
+        <f t="shared" si="18"/>
         <v>Rotting Treestump -  Room Exits: N S W  Front: nsesw  Back: None</v>
       </c>
       <c r="H152" t="str">
-        <f>CONCATENATE("#sub {", F152, "} {", G152, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Rotting Treestump%0Exits are: N S W} {Rotting Treestump -  Room Exits: N S W  Front: nsesw  Back: None}</v>
       </c>
       <c r="I152" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A152,"} {%0 %1- ",G152, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Rotting Treestump} {%0 %1- Rotting Treestump -  Room Exits: N S W  Front: nsesw  Back: None}</v>
       </c>
     </row>
@@ -6219,19 +6223,19 @@
         <v>393</v>
       </c>
       <c r="F153" t="str">
-        <f>CONCATENATE(A153,"%0Exits are: ",C153)</f>
+        <f t="shared" si="17"/>
         <v>Row of Elms%0Exits are: E S W</v>
       </c>
       <c r="G153" t="str">
-        <f>CONCATENATE(A153, " -  Room Exits: ", C153, "  Front: ", IF(D153="", "None", D153), "  Back: ", IF(E153="", "None", E153))</f>
+        <f t="shared" si="18"/>
         <v>Row of Elms -  Room Exits: E S W  Front: ww  Back: wnneeseeneenesene</v>
       </c>
       <c r="H153" t="str">
-        <f>CONCATENATE("#sub {", F153, "} {", G153, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Row of Elms%0Exits are: E S W} {Row of Elms -  Room Exits: E S W  Front: ww  Back: wnneeseeneenesene}</v>
       </c>
       <c r="I153" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A153,"} {%0 %1- ",G153, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Row of Elms} {%0 %1- Row of Elms -  Room Exits: E S W  Front: ww  Back: wnneeseeneenesene}</v>
       </c>
     </row>
@@ -6249,19 +6253,19 @@
         <v>100</v>
       </c>
       <c r="F154" t="str">
-        <f>CONCATENATE(A154,"%0Exits are: ",C154)</f>
+        <f t="shared" si="17"/>
         <v>Scarred Land%0Exits are: N S W</v>
       </c>
       <c r="G154" t="str">
-        <f>CONCATENATE(A154, " -  Room Exits: ", C154, "  Front: ", IF(D154="", "None", D154), "  Back: ", IF(E154="", "None", E154))</f>
+        <f t="shared" si="18"/>
         <v>Scarred Land -  Room Exits: N S W  Front: sswnwenw  Back: None</v>
       </c>
       <c r="H154" t="str">
-        <f>CONCATENATE("#sub {", F154, "} {", G154, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Scarred Land%0Exits are: N S W} {Scarred Land -  Room Exits: N S W  Front: sswnwenw  Back: None}</v>
       </c>
       <c r="I154" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A154,"} {%0 %1- ",G154, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Scarred Land} {%0 %1- Scarred Land -  Room Exits: N S W  Front: sswnwenw  Back: None}</v>
       </c>
     </row>
@@ -6279,19 +6283,19 @@
         <v>93</v>
       </c>
       <c r="F155" t="str">
-        <f>CONCATENATE(A155,"%0Exits are: ",C155)</f>
+        <f t="shared" si="17"/>
         <v>Sea of Trees%0Exits are: N S</v>
       </c>
       <c r="G155" t="str">
-        <f>CONCATENATE(A155, " -  Room Exits: ", C155, "  Front: ", IF(D155="", "None", D155), "  Back: ", IF(E155="", "None", E155))</f>
+        <f t="shared" si="18"/>
         <v>Sea of Trees -  Room Exits: N S  Front: sesw  Back: None</v>
       </c>
       <c r="H155" t="str">
-        <f>CONCATENATE("#sub {", F155, "} {", G155, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Sea of Trees%0Exits are: N S} {Sea of Trees -  Room Exits: N S  Front: sesw  Back: None}</v>
       </c>
       <c r="I155" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A155,"} {%0 %1- ",G155, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Sea of Trees} {%0 %1- Sea of Trees -  Room Exits: N S  Front: sesw  Back: None}</v>
       </c>
     </row>
@@ -6309,19 +6313,19 @@
         <v>70</v>
       </c>
       <c r="F156" t="str">
-        <f>CONCATENATE(A156,"%0Exits are: ",C156)</f>
+        <f t="shared" si="17"/>
         <v>Shadowy Hues%0Exits are: S W</v>
       </c>
       <c r="G156" t="str">
-        <f>CONCATENATE(A156, " -  Room Exits: ", C156, "  Front: ", IF(D156="", "None", D156), "  Back: ", IF(E156="", "None", E156))</f>
+        <f t="shared" si="18"/>
         <v>Shadowy Hues -  Room Exits: S W  Front: wsnww  Back: None</v>
       </c>
       <c r="H156" t="str">
-        <f>CONCATENATE("#sub {", F156, "} {", G156, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Shadowy Hues%0Exits are: S W} {Shadowy Hues -  Room Exits: S W  Front: wsnww  Back: None}</v>
       </c>
       <c r="I156" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A156,"} {%0 %1- ",G156, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Shadowy Hues} {%0 %1- Shadowy Hues -  Room Exits: S W  Front: wsnww  Back: None}</v>
       </c>
     </row>
@@ -6339,19 +6343,19 @@
         <v>402</v>
       </c>
       <c r="F157" t="str">
-        <f>CONCATENATE(A157,"%0Exits are: ",C157)</f>
+        <f t="shared" si="17"/>
         <v>Shallow Waters%0Exits are: E S W</v>
       </c>
       <c r="G157" t="str">
-        <f>CONCATENATE(A157, " -  Room Exits: ", C157, "  Front: ", IF(D157="", "None", D157), "  Back: ", IF(E157="", "None", E157))</f>
+        <f t="shared" si="18"/>
         <v>Shallow Waters -  Room Exits: E S W  Front: wennsnnnww  Back: None</v>
       </c>
       <c r="H157" t="str">
-        <f>CONCATENATE("#sub {", F157, "} {", G157, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Shallow Waters%0Exits are: E S W} {Shallow Waters -  Room Exits: E S W  Front: wennsnnnww  Back: None}</v>
       </c>
       <c r="I157" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A157,"} {%0 %1- ",G157, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Shallow Waters} {%0 %1- Shallow Waters -  Room Exits: E S W  Front: wennsnnnww  Back: None}</v>
       </c>
     </row>
@@ -6369,19 +6373,19 @@
         <v>234</v>
       </c>
       <c r="F158" t="str">
-        <f>CONCATENATE(A158,"%0Exits are: ",C158)</f>
+        <f t="shared" si="17"/>
         <v>Sharp Spears%0Exits are: N E</v>
       </c>
       <c r="G158" t="str">
-        <f>CONCATENATE(A158, " -  Room Exits: ", C158, "  Front: ", IF(D158="", "None", D158), "  Back: ", IF(E158="", "None", E158))</f>
+        <f t="shared" si="18"/>
         <v>Sharp Spears -  Room Exits: N E  Front: nwwesew  Back: None</v>
       </c>
       <c r="H158" t="str">
-        <f>CONCATENATE("#sub {", F158, "} {", G158, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Sharp Spears%0Exits are: N E} {Sharp Spears -  Room Exits: N E  Front: nwwesew  Back: None}</v>
       </c>
       <c r="I158" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A158,"} {%0 %1- ",G158, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Sharp Spears} {%0 %1- Sharp Spears -  Room Exits: N E  Front: nwwesew  Back: None}</v>
       </c>
     </row>
@@ -6399,19 +6403,19 @@
         <v>166</v>
       </c>
       <c r="F159" t="str">
-        <f>CONCATENATE(A159,"%0Exits are: ",C159)</f>
+        <f t="shared" si="17"/>
         <v>Shifting Trees%0Exits are: N S W</v>
       </c>
       <c r="G159" t="str">
-        <f>CONCATENATE(A159, " -  Room Exits: ", C159, "  Front: ", IF(D159="", "None", D159), "  Back: ", IF(E159="", "None", E159))</f>
+        <f t="shared" si="18"/>
         <v>Shifting Trees -  Room Exits: N S W  Front: nnnnww  Back: None</v>
       </c>
       <c r="H159" t="str">
-        <f>CONCATENATE("#sub {", F159, "} {", G159, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Shifting Trees%0Exits are: N S W} {Shifting Trees -  Room Exits: N S W  Front: nnnnww  Back: None}</v>
       </c>
       <c r="I159" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A159,"} {%0 %1- ",G159, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Shifting Trees} {%0 %1- Shifting Trees -  Room Exits: N S W  Front: nnnnww  Back: None}</v>
       </c>
     </row>
@@ -6429,19 +6433,19 @@
         <v>215</v>
       </c>
       <c r="F160" t="str">
-        <f>CONCATENATE(A160,"%0Exits are: ",C160)</f>
+        <f t="shared" si="17"/>
         <v>Sickly Forest%0Exits are: N E S</v>
       </c>
       <c r="G160" t="str">
-        <f>CONCATENATE(A160, " -  Room Exits: ", C160, "  Front: ", IF(D160="", "None", D160), "  Back: ", IF(E160="", "None", E160))</f>
+        <f t="shared" si="18"/>
         <v>Sickly Forest -  Room Exits: N E S  Front: nnsnww  Back: None</v>
       </c>
       <c r="H160" t="str">
-        <f>CONCATENATE("#sub {", F160, "} {", G160, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Sickly Forest%0Exits are: N E S} {Sickly Forest -  Room Exits: N E S  Front: nnsnww  Back: None}</v>
       </c>
       <c r="I160" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A160,"} {%0 %1- ",G160, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Sickly Forest} {%0 %1- Sickly Forest -  Room Exits: N E S  Front: nnsnww  Back: None}</v>
       </c>
     </row>
@@ -6459,19 +6463,19 @@
         <v>91</v>
       </c>
       <c r="F161" t="str">
-        <f>CONCATENATE(A161,"%0Exits are: ",C161)</f>
+        <f t="shared" si="17"/>
         <v>Silent Arena%0Exits are: N S</v>
       </c>
       <c r="G161" t="str">
-        <f>CONCATENATE(A161, " -  Room Exits: ", C161, "  Front: ", IF(D161="", "None", D161), "  Back: ", IF(E161="", "None", E161))</f>
+        <f t="shared" si="18"/>
         <v>Silent Arena -  Room Exits: N S  Front: nsessesw  Back: None</v>
       </c>
       <c r="H161" t="str">
-        <f>CONCATENATE("#sub {", F161, "} {", G161, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Silent Arena%0Exits are: N S} {Silent Arena -  Room Exits: N S  Front: nsessesw  Back: None}</v>
       </c>
       <c r="I161" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A161,"} {%0 %1- ",G161, "}")</f>
+        <f t="shared" si="19"/>
         <v>#sub {%0 %1- Silent Arena} {%0 %1- Silent Arena -  Room Exits: N S  Front: nsessesw  Back: None}</v>
       </c>
     </row>
@@ -6489,19 +6493,19 @@
         <v>238</v>
       </c>
       <c r="F162" t="str">
-        <f>CONCATENATE(A162,"%0Exits are: ",C162)</f>
+        <f t="shared" ref="F162:F193" si="21">CONCATENATE(A162,"%0Exits are: ",C162)</f>
         <v>Silent Trees%0Exits are: E S</v>
       </c>
       <c r="G162" t="str">
-        <f>CONCATENATE(A162, " -  Room Exits: ", C162, "  Front: ", IF(D162="", "None", D162), "  Back: ", IF(E162="", "None", E162))</f>
+        <f t="shared" ref="G162:G193" si="22">CONCATENATE(A162, " -  Room Exits: ", C162, "  Front: ", IF(D162="", "None", D162), "  Back: ", IF(E162="", "None", E162))</f>
         <v>Silent Trees -  Room Exits: E S  Front: snnnw  Back: None</v>
       </c>
       <c r="H162" t="str">
-        <f>CONCATENATE("#sub {", F162, "} {", G162, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Silent Trees%0Exits are: E S} {Silent Trees -  Room Exits: E S  Front: snnnw  Back: None}</v>
       </c>
       <c r="I162" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A162,"} {%0 %1- ",G162, "}")</f>
+        <f t="shared" ref="I162:I193" si="23">CONCATENATE("#sub {%0 %1- ",A162,"} {%0 %1- ",G162, "}")</f>
         <v>#sub {%0 %1- Silent Trees} {%0 %1- Silent Trees -  Room Exits: E S  Front: snnnw  Back: None}</v>
       </c>
     </row>
@@ -6519,19 +6523,19 @@
         <v>236</v>
       </c>
       <c r="F163" t="str">
-        <f>CONCATENATE(A163,"%0Exits are: ",C163)</f>
+        <f t="shared" si="21"/>
         <v>Sleeping Forest%0Exits are: E S</v>
       </c>
       <c r="G163" t="str">
-        <f>CONCATENATE(A163, " -  Room Exits: ", C163, "  Front: ", IF(D163="", "None", D163), "  Back: ", IF(E163="", "None", E163))</f>
+        <f t="shared" si="22"/>
         <v>Sleeping Forest -  Room Exits: E S  Front: eswwww  Back: None</v>
       </c>
       <c r="H163" t="str">
-        <f>CONCATENATE("#sub {", F163, "} {", G163, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Sleeping Forest%0Exits are: E S} {Sleeping Forest -  Room Exits: E S  Front: eswwww  Back: None}</v>
       </c>
       <c r="I163" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A163,"} {%0 %1- ",G163, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Sleeping Forest} {%0 %1- Sleeping Forest -  Room Exits: E S  Front: eswwww  Back: None}</v>
       </c>
     </row>
@@ -6549,19 +6553,19 @@
         <v>191</v>
       </c>
       <c r="F164" t="str">
-        <f>CONCATENATE(A164,"%0Exits are: ",C164)</f>
+        <f t="shared" si="21"/>
         <v>Slushy Ground%0Exits are: N S</v>
       </c>
       <c r="G164" t="str">
-        <f>CONCATENATE(A164, " -  Room Exits: ", C164, "  Front: ", IF(D164="", "None", D164), "  Back: ", IF(E164="", "None", E164))</f>
+        <f t="shared" si="22"/>
         <v>Slushy Ground -  Room Exits: N S  Front: snwenw  Back: None</v>
       </c>
       <c r="H164" t="str">
-        <f>CONCATENATE("#sub {", F164, "} {", G164, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Slushy Ground%0Exits are: N S} {Slushy Ground -  Room Exits: N S  Front: snwenw  Back: None}</v>
       </c>
       <c r="I164" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A164,"} {%0 %1- ",G164, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Slushy Ground} {%0 %1- Slushy Ground -  Room Exits: N S  Front: snwenw  Back: None}</v>
       </c>
     </row>
@@ -6579,19 +6583,19 @@
         <v>277</v>
       </c>
       <c r="F165" t="str">
-        <f>CONCATENATE(A165,"%0Exits are: ",C165)</f>
+        <f t="shared" si="21"/>
         <v>Smell of Decay%0Exits are: E W</v>
       </c>
       <c r="G165" t="str">
-        <f>CONCATENATE(A165, " -  Room Exits: ", C165, "  Front: ", IF(D165="", "None", D165), "  Back: ", IF(E165="", "None", E165))</f>
+        <f t="shared" si="22"/>
         <v>Smell of Decay -  Room Exits: E W  Front: wewenw  Back: None</v>
       </c>
       <c r="H165" t="str">
-        <f>CONCATENATE("#sub {", F165, "} {", G165, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Smell of Decay%0Exits are: E W} {Smell of Decay -  Room Exits: E W  Front: wewenw  Back: None}</v>
       </c>
       <c r="I165" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A165,"} {%0 %1- ",G165, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Smell of Decay} {%0 %1- Smell of Decay -  Room Exits: E W  Front: wewenw  Back: None}</v>
       </c>
     </row>
@@ -6612,19 +6616,19 @@
         <v>152</v>
       </c>
       <c r="F166" t="str">
-        <f>CONCATENATE(A166,"%0Exits are: ",C166)</f>
+        <f t="shared" si="21"/>
         <v>Snare of Pines%0Exits are: E S W</v>
       </c>
       <c r="G166" t="str">
-        <f>CONCATENATE(A166, " -  Room Exits: ", C166, "  Front: ", IF(D166="", "None", D166), "  Back: ", IF(E166="", "None", E166))</f>
+        <f t="shared" si="22"/>
         <v>Snare of Pines -  Room Exits: E S W  Front: ssnenw  Back: sene</v>
       </c>
       <c r="H166" t="str">
-        <f>CONCATENATE("#sub {", F166, "} {", G166, "}")</f>
+        <f t="shared" si="20"/>
         <v>#sub {Snare of Pines%0Exits are: E S W} {Snare of Pines -  Room Exits: E S W  Front: ssnenw  Back: sene}</v>
       </c>
       <c r="I166" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A166,"} {%0 %1- ",G166, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Snare of Pines} {%0 %1- Snare of Pines -  Room Exits: E S W  Front: ssnenw  Back: sene}</v>
       </c>
     </row>
@@ -6642,19 +6646,19 @@
         <v>304</v>
       </c>
       <c r="F167" t="str">
-        <f>CONCATENATE(A167,"%0Exits are: ",C167)</f>
+        <f t="shared" si="21"/>
         <v>Solid Ground Once Again%0Exits are: N E S</v>
       </c>
       <c r="G167" t="str">
-        <f>CONCATENATE(A167, " -  Room Exits: ", C167, "  Front: ", IF(D167="", "None", D167), "  Back: ", IF(E167="", "None", E167))</f>
+        <f t="shared" si="22"/>
         <v>Solid Ground Once Again -  Room Exits: N E S  Front: nnewennw  Back: None</v>
       </c>
       <c r="H167" t="str">
-        <f>CONCATENATE("#sub {", F167, "} {", G167, "}")</f>
+        <f t="shared" ref="H167:H198" si="24">CONCATENATE("#sub {", F167, "} {", G167, "}")</f>
         <v>#sub {Solid Ground Once Again%0Exits are: N E S} {Solid Ground Once Again -  Room Exits: N E S  Front: nnewennw  Back: None}</v>
       </c>
       <c r="I167" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A167,"} {%0 %1- ",G167, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Solid Ground Once Again} {%0 %1- Solid Ground Once Again -  Room Exits: N E S  Front: nnewennw  Back: None}</v>
       </c>
     </row>
@@ -6672,19 +6676,19 @@
         <v>176</v>
       </c>
       <c r="F168" t="str">
-        <f>CONCATENATE(A168,"%0Exits are: ",C168)</f>
+        <f t="shared" si="21"/>
         <v>Split Path%0Exits are: E W</v>
       </c>
       <c r="G168" t="str">
-        <f>CONCATENATE(A168, " -  Room Exits: ", C168, "  Front: ", IF(D168="", "None", D168), "  Back: ", IF(E168="", "None", E168))</f>
+        <f t="shared" si="22"/>
         <v>Split Path -  Room Exits: E W  Front: wnnww  Back: None</v>
       </c>
       <c r="H168" t="str">
-        <f>CONCATENATE("#sub {", F168, "} {", G168, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Split Path%0Exits are: E W} {Split Path -  Room Exits: E W  Front: wnnww  Back: None}</v>
       </c>
       <c r="I168" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A168,"} {%0 %1- ",G168, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Split Path} {%0 %1- Split Path -  Room Exits: E W  Front: wnnww  Back: None}</v>
       </c>
     </row>
@@ -6702,19 +6706,19 @@
         <v>102</v>
       </c>
       <c r="F169" t="str">
-        <f>CONCATENATE(A169,"%0Exits are: ",C169)</f>
+        <f t="shared" si="21"/>
         <v>Spongy Ground%0Exits are: N E S W</v>
       </c>
       <c r="G169" t="str">
-        <f>CONCATENATE(A169, " -  Room Exits: ", C169, "  Front: ", IF(D169="", "None", D169), "  Back: ", IF(E169="", "None", E169))</f>
+        <f t="shared" si="22"/>
         <v>Spongy Ground -  Room Exits: N E S W  Front: sssesw  Back: None</v>
       </c>
       <c r="H169" t="str">
-        <f>CONCATENATE("#sub {", F169, "} {", G169, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Spongy Ground%0Exits are: N E S W} {Spongy Ground -  Room Exits: N E S W  Front: sssesw  Back: None}</v>
       </c>
       <c r="I169" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A169,"} {%0 %1- ",G169, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Spongy Ground} {%0 %1- Spongy Ground -  Room Exits: N E S W  Front: sssesw  Back: None}</v>
       </c>
     </row>
@@ -6735,19 +6739,19 @@
         <v>52</v>
       </c>
       <c r="F170" t="str">
-        <f>CONCATENATE(A170,"%0Exits are: ",C170)</f>
+        <f t="shared" si="21"/>
         <v>Strange Lights%0Exits are: N E S</v>
       </c>
       <c r="G170" t="str">
-        <f>CONCATENATE(A170, " -  Room Exits: ", C170, "  Front: ", IF(D170="", "None", D170), "  Back: ", IF(E170="", "None", E170))</f>
+        <f t="shared" si="22"/>
         <v>Strange Lights -  Room Exits: N E S  Front: nwenw  Back: neeseeneenesene</v>
       </c>
       <c r="H170" t="str">
-        <f>CONCATENATE("#sub {", F170, "} {", G170, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Strange Lights%0Exits are: N E S} {Strange Lights -  Room Exits: N E S  Front: nwenw  Back: neeseeneenesene}</v>
       </c>
       <c r="I170" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A170,"} {%0 %1- ",G170, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Strange Lights} {%0 %1- Strange Lights -  Room Exits: N E S  Front: nwenw  Back: neeseeneenesene}</v>
       </c>
     </row>
@@ -6765,19 +6769,19 @@
         <v>370</v>
       </c>
       <c r="F171" t="str">
-        <f>CONCATENATE(A171,"%0Exits are: ",C171)</f>
+        <f t="shared" si="21"/>
         <v>Strange Marsh%0Exits are: N S W</v>
       </c>
       <c r="G171" t="str">
-        <f>CONCATENATE(A171, " -  Room Exits: ", C171, "  Front: ", IF(D171="", "None", D171), "  Back: ", IF(E171="", "None", E171))</f>
+        <f t="shared" si="22"/>
         <v>Strange Marsh -  Room Exits: N S W  Front: snnewennw  Back: None</v>
       </c>
       <c r="H171" t="str">
-        <f>CONCATENATE("#sub {", F171, "} {", G171, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Strange Marsh%0Exits are: N S W} {Strange Marsh -  Room Exits: N S W  Front: snnewennw  Back: None}</v>
       </c>
       <c r="I171" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A171,"} {%0 %1- ",G171, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Strange Marsh} {%0 %1- Strange Marsh -  Room Exits: N S W  Front: snnewennw  Back: None}</v>
       </c>
     </row>
@@ -6795,19 +6799,19 @@
         <v>236</v>
       </c>
       <c r="F172" t="str">
-        <f>CONCATENATE(A172,"%0Exits are: ",C172)</f>
+        <f t="shared" si="21"/>
         <v>Strangled Forest%0Exits are: N E</v>
       </c>
       <c r="G172" t="str">
-        <f>CONCATENATE(A172, " -  Room Exits: ", C172, "  Front: ", IF(D172="", "None", D172), "  Back: ", IF(E172="", "None", E172))</f>
+        <f t="shared" si="22"/>
         <v>Strangled Forest -  Room Exits: N E  Front: eswwww  Back: None</v>
       </c>
       <c r="H172" t="str">
-        <f>CONCATENATE("#sub {", F172, "} {", G172, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Strangled Forest%0Exits are: N E} {Strangled Forest -  Room Exits: N E  Front: eswwww  Back: None}</v>
       </c>
       <c r="I172" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A172,"} {%0 %1- ",G172, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Strangled Forest} {%0 %1- Strangled Forest -  Room Exits: N E  Front: eswwww  Back: None}</v>
       </c>
     </row>
@@ -6825,19 +6829,19 @@
         <v>256</v>
       </c>
       <c r="F173" t="str">
-        <f>CONCATENATE(A173,"%0Exits are: ",C173)</f>
+        <f t="shared" si="21"/>
         <v>Sunken Path%0Exits are: N E S W</v>
       </c>
       <c r="G173" t="str">
-        <f>CONCATENATE(A173, " -  Room Exits: ", C173, "  Front: ", IF(D173="", "None", D173), "  Back: ", IF(E173="", "None", E173))</f>
+        <f t="shared" si="22"/>
         <v>Sunken Path -  Room Exits: N E S W  Front: wennnnww  Back: None</v>
       </c>
       <c r="H173" t="str">
-        <f>CONCATENATE("#sub {", F173, "} {", G173, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Sunken Path%0Exits are: N E S W} {Sunken Path -  Room Exits: N E S W  Front: wennnnww  Back: None}</v>
       </c>
       <c r="I173" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A173,"} {%0 %1- ",G173, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Sunken Path} {%0 %1- Sunken Path -  Room Exits: N E S W  Front: wennnnww  Back: None}</v>
       </c>
     </row>
@@ -6855,19 +6859,19 @@
         <v>261</v>
       </c>
       <c r="F174" t="str">
-        <f>CONCATENATE(A174,"%0Exits are: ",C174)</f>
+        <f t="shared" si="21"/>
         <v>Surreal Forest%0Exits are: N E S</v>
       </c>
       <c r="G174" t="str">
-        <f>CONCATENATE(A174, " -  Room Exits: ", C174, "  Front: ", IF(D174="", "None", D174), "  Back: ", IF(E174="", "None", E174))</f>
+        <f t="shared" si="22"/>
         <v>Surreal Forest -  Room Exits: N E S  Front: ennww  Back: None</v>
       </c>
       <c r="H174" t="str">
-        <f>CONCATENATE("#sub {", F174, "} {", G174, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Surreal Forest%0Exits are: N E S} {Surreal Forest -  Room Exits: N E S  Front: ennww  Back: None}</v>
       </c>
       <c r="I174" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A174,"} {%0 %1- ",G174, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Surreal Forest} {%0 %1- Surreal Forest -  Room Exits: N E S  Front: ennww  Back: None}</v>
       </c>
     </row>
@@ -6885,19 +6889,19 @@
         <v>313</v>
       </c>
       <c r="F175" t="str">
-        <f>CONCATENATE(A175,"%0Exits are: ",C175)</f>
+        <f t="shared" si="21"/>
         <v>Taur-e-Duath%0Exits are: N W</v>
       </c>
       <c r="G175" t="str">
-        <f>CONCATENATE(A175, " -  Room Exits: ", C175, "  Front: ", IF(D175="", "None", D175), "  Back: ", IF(E175="", "None", E175))</f>
+        <f t="shared" si="22"/>
         <v>Taur-e-Duath -  Room Exits: N W  Front: nesnennw  Back: None</v>
       </c>
       <c r="H175" t="str">
-        <f>CONCATENATE("#sub {", F175, "} {", G175, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Taur-e-Duath%0Exits are: N W} {Taur-e-Duath -  Room Exits: N W  Front: nesnennw  Back: None}</v>
       </c>
       <c r="I175" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A175,"} {%0 %1- ",G175, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Taur-e-Duath} {%0 %1- Taur-e-Duath -  Room Exits: N W  Front: nesnennw  Back: None}</v>
       </c>
     </row>
@@ -6915,19 +6919,19 @@
         <v>280</v>
       </c>
       <c r="F176" t="str">
-        <f>CONCATENATE(A176,"%0Exits are: ",C176)</f>
+        <f t="shared" si="21"/>
         <v>Taur-nu-Fuin%0Exits are: E S W</v>
       </c>
       <c r="G176" t="str">
-        <f>CONCATENATE(A176, " -  Room Exits: ", C176, "  Front: ", IF(D176="", "None", D176), "  Back: ", IF(E176="", "None", E176))</f>
+        <f t="shared" si="22"/>
         <v>Taur-nu-Fuin -  Room Exits: E S W  Front: wesewenw  Back: None</v>
       </c>
       <c r="H176" t="str">
-        <f>CONCATENATE("#sub {", F176, "} {", G176, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Taur-nu-Fuin%0Exits are: E S W} {Taur-nu-Fuin -  Room Exits: E S W  Front: wesewenw  Back: None}</v>
       </c>
       <c r="I176" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A176,"} {%0 %1- ",G176, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Taur-nu-Fuin} {%0 %1- Taur-nu-Fuin -  Room Exits: E S W  Front: wesewenw  Back: None}</v>
       </c>
     </row>
@@ -6945,19 +6949,19 @@
         <v>274</v>
       </c>
       <c r="F177" t="str">
-        <f>CONCATENATE(A177,"%0Exits are: ",C177)</f>
+        <f t="shared" si="21"/>
         <v>Taur-nu-Morna%0Exits are: N S W</v>
       </c>
       <c r="G177" t="str">
-        <f>CONCATENATE(A177, " -  Room Exits: ", C177, "  Front: ", IF(D177="", "None", D177), "  Back: ", IF(E177="", "None", E177))</f>
+        <f t="shared" si="22"/>
         <v>Taur-nu-Morna -  Room Exits: N S W  Front: sw  Back: None</v>
       </c>
       <c r="H177" t="str">
-        <f>CONCATENATE("#sub {", F177, "} {", G177, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Taur-nu-Morna%0Exits are: N S W} {Taur-nu-Morna -  Room Exits: N S W  Front: sw  Back: None}</v>
       </c>
       <c r="I177" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A177,"} {%0 %1- ",G177, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Taur-nu-Morna} {%0 %1- Taur-nu-Morna -  Room Exits: N S W  Front: sw  Back: None}</v>
       </c>
     </row>
@@ -6975,19 +6979,19 @@
         <v>62</v>
       </c>
       <c r="F178" t="str">
-        <f>CONCATENATE(A178,"%0Exits are: ",C178)</f>
+        <f t="shared" si="21"/>
         <v>The Barrier%0Exits are: N S</v>
       </c>
       <c r="G178" t="str">
-        <f>CONCATENATE(A178, " -  Room Exits: ", C178, "  Front: ", IF(D178="", "None", D178), "  Back: ", IF(E178="", "None", E178))</f>
+        <f t="shared" si="22"/>
         <v>The Barrier -  Room Exits: N S  Front: sssnww  Back: None</v>
       </c>
       <c r="H178" t="str">
-        <f>CONCATENATE("#sub {", F178, "} {", G178, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Barrier%0Exits are: N S} {The Barrier -  Room Exits: N S  Front: sssnww  Back: None}</v>
       </c>
       <c r="I178" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A178,"} {%0 %1- ",G178, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Barrier} {%0 %1- The Barrier -  Room Exits: N S  Front: sssnww  Back: None}</v>
       </c>
     </row>
@@ -7005,19 +7009,19 @@
         <v>6</v>
       </c>
       <c r="F179" t="str">
-        <f>CONCATENATE(A179,"%0Exits are: ",C179)</f>
+        <f t="shared" si="21"/>
         <v>The Channel%0Exits are: E W</v>
       </c>
       <c r="G179" t="str">
-        <f>CONCATENATE(A179, " -  Room Exits: ", C179, "  Front: ", IF(D179="", "None", D179), "  Back: ", IF(E179="", "None", E179))</f>
+        <f t="shared" si="22"/>
         <v>The Channel -  Room Exits: E W  Front: ewnnewennw  Back: None</v>
       </c>
       <c r="H179" t="str">
-        <f>CONCATENATE("#sub {", F179, "} {", G179, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Channel%0Exits are: E W} {The Channel -  Room Exits: E W  Front: ewnnewennw  Back: None}</v>
       </c>
       <c r="I179" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A179,"} {%0 %1- ",G179, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Channel} {%0 %1- The Channel -  Room Exits: E W  Front: ewnnewennw  Back: None}</v>
       </c>
     </row>
@@ -7035,19 +7039,19 @@
         <v>113</v>
       </c>
       <c r="F180" t="str">
-        <f>CONCATENATE(A180,"%0Exits are: ",C180)</f>
+        <f t="shared" si="21"/>
         <v>The Dark Wood%0Exits are: N E S</v>
       </c>
       <c r="G180" t="str">
-        <f>CONCATENATE(A180, " -  Room Exits: ", C180, "  Front: ", IF(D180="", "None", D180), "  Back: ", IF(E180="", "None", E180))</f>
+        <f t="shared" si="22"/>
         <v>The Dark Wood -  Room Exits: N E S  Front: swesew  Back: None</v>
       </c>
       <c r="H180" t="str">
-        <f>CONCATENATE("#sub {", F180, "} {", G180, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Dark Wood%0Exits are: N E S} {The Dark Wood -  Room Exits: N E S  Front: swesew  Back: None}</v>
       </c>
       <c r="I180" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A180,"} {%0 %1- ",G180, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Dark Wood} {%0 %1- The Dark Wood -  Room Exits: N E S  Front: swesew  Back: None}</v>
       </c>
     </row>
@@ -7065,19 +7069,19 @@
         <v>336</v>
       </c>
       <c r="F181" t="str">
-        <f>CONCATENATE(A181,"%0Exits are: ",C181)</f>
+        <f t="shared" si="21"/>
         <v>The Great Pine%0Exits are: N E W</v>
       </c>
       <c r="G181" t="str">
-        <f>CONCATENATE(A181, " -  Room Exits: ", C181, "  Front: ", IF(D181="", "None", D181), "  Back: ", IF(E181="", "None", E181))</f>
+        <f t="shared" si="22"/>
         <v>The Great Pine -  Room Exits: N E W  Front: esnww  Back: None</v>
       </c>
       <c r="H181" t="str">
-        <f>CONCATENATE("#sub {", F181, "} {", G181, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Great Pine%0Exits are: N E W} {The Great Pine -  Room Exits: N E W  Front: esnww  Back: None}</v>
       </c>
       <c r="I181" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A181,"} {%0 %1- ",G181, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Great Pine} {%0 %1- The Great Pine -  Room Exits: N E W  Front: esnww  Back: None}</v>
       </c>
     </row>
@@ -7095,19 +7099,19 @@
         <v>336</v>
       </c>
       <c r="F182" t="str">
-        <f>CONCATENATE(A182,"%0Exits are: ",C182)</f>
+        <f t="shared" si="21"/>
         <v>The Great Pine%0Exits are: N E W</v>
       </c>
       <c r="G182" t="str">
-        <f>CONCATENATE(A182, " -  Room Exits: ", C182, "  Front: ", IF(D182="", "None", D182), "  Back: ", IF(E182="", "None", E182))</f>
+        <f t="shared" si="22"/>
         <v>The Great Pine -  Room Exits: N E W  Front: esnww  Back: None</v>
       </c>
       <c r="H182" t="str">
-        <f>CONCATENATE("#sub {", F182, "} {", G182, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Great Pine%0Exits are: N E W} {The Great Pine -  Room Exits: N E W  Front: esnww  Back: None}</v>
       </c>
       <c r="I182" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A182,"} {%0 %1- ",G182, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Great Pine} {%0 %1- The Great Pine -  Room Exits: N E W  Front: esnww  Back: None}</v>
       </c>
     </row>
@@ -7125,19 +7129,19 @@
         <v>405</v>
       </c>
       <c r="F183" t="str">
-        <f>CONCATENATE(A183,"%0Exits are: ",C183)</f>
+        <f t="shared" si="21"/>
         <v>The Ground Grows Soft%0Exits are: N W</v>
       </c>
       <c r="G183" t="str">
-        <f>CONCATENATE(A183, " -  Room Exits: ", C183, "  Front: ", IF(D183="", "None", D183), "  Back: ", IF(E183="", "None", E183))</f>
+        <f t="shared" si="22"/>
         <v>The Ground Grows Soft -  Room Exits: N W  Front: nnnenw  Back: None</v>
       </c>
       <c r="H183" t="str">
-        <f>CONCATENATE("#sub {", F183, "} {", G183, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Ground Grows Soft%0Exits are: N W} {The Ground Grows Soft -  Room Exits: N W  Front: nnnenw  Back: None}</v>
       </c>
       <c r="I183" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A183,"} {%0 %1- ",G183, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Ground Grows Soft} {%0 %1- The Ground Grows Soft -  Room Exits: N W  Front: nnnenw  Back: None}</v>
       </c>
     </row>
@@ -7155,19 +7159,19 @@
         <v>98</v>
       </c>
       <c r="F184" t="str">
-        <f>CONCATENATE(A184,"%0Exits are: ",C184)</f>
+        <f t="shared" si="21"/>
         <v>The Path%0Exits are: N S W</v>
       </c>
       <c r="G184" t="str">
-        <f>CONCATENATE(A184, " -  Room Exits: ", C184, "  Front: ", IF(D184="", "None", D184), "  Back: ", IF(E184="", "None", E184))</f>
+        <f t="shared" si="22"/>
         <v>The Path -  Room Exits: N S W  Front: wnwenw  Back: None</v>
       </c>
       <c r="H184" t="str">
-        <f>CONCATENATE("#sub {", F184, "} {", G184, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {The Path%0Exits are: N S W} {The Path -  Room Exits: N S W  Front: wnwenw  Back: None}</v>
       </c>
       <c r="I184" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A184,"} {%0 %1- ",G184, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- The Path} {%0 %1- The Path -  Room Exits: N S W  Front: wnwenw  Back: None}</v>
       </c>
     </row>
@@ -7185,19 +7189,19 @@
         <v>174</v>
       </c>
       <c r="F185" t="str">
-        <f>CONCATENATE(A185,"%0Exits are: ",C185)</f>
+        <f t="shared" si="21"/>
         <v>Thick Bramble%0Exits are: N E</v>
       </c>
       <c r="G185" t="str">
-        <f>CONCATENATE(A185, " -  Room Exits: ", C185, "  Front: ", IF(D185="", "None", D185), "  Back: ", IF(E185="", "None", E185))</f>
+        <f t="shared" si="22"/>
         <v>Thick Bramble -  Room Exits: N E  Front: ewnnww  Back: None</v>
       </c>
       <c r="H185" t="str">
-        <f>CONCATENATE("#sub {", F185, "} {", G185, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Thick Bramble%0Exits are: N E} {Thick Bramble -  Room Exits: N E  Front: ewnnww  Back: None}</v>
       </c>
       <c r="I185" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A185,"} {%0 %1- ",G185, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Thick Bramble} {%0 %1- Thick Bramble -  Room Exits: N E  Front: ewnnww  Back: None}</v>
       </c>
     </row>
@@ -7215,19 +7219,19 @@
         <v>404</v>
       </c>
       <c r="F186" t="str">
-        <f>CONCATENATE(A186,"%0Exits are: ",C186)</f>
+        <f t="shared" si="21"/>
         <v>Thick Underbrush%0Exits are: N S</v>
       </c>
       <c r="G186" t="str">
-        <f>CONCATENATE(A186, " -  Room Exits: ", C186, "  Front: ", IF(D186="", "None", D186), "  Back: ", IF(E186="", "None", E186))</f>
+        <f t="shared" si="22"/>
         <v>Thick Underbrush -  Room Exits: N S  Front: nnenw  Back: None</v>
       </c>
       <c r="H186" t="str">
-        <f>CONCATENATE("#sub {", F186, "} {", G186, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Thick Underbrush%0Exits are: N S} {Thick Underbrush -  Room Exits: N S  Front: nnenw  Back: None}</v>
       </c>
       <c r="I186" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A186,"} {%0 %1- ",G186, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Thick Underbrush} {%0 %1- Thick Underbrush -  Room Exits: N S  Front: nnenw  Back: None}</v>
       </c>
     </row>
@@ -7245,19 +7249,19 @@
         <v>407</v>
       </c>
       <c r="F187" t="str">
-        <f>CONCATENATE(A187,"%0Exits are: ",C187)</f>
+        <f t="shared" si="21"/>
         <v>Thick, Dark Forest%0Exits are: N S</v>
       </c>
       <c r="G187" t="str">
-        <f>CONCATENATE(A187, " -  Room Exits: ", C187, "  Front: ", IF(D187="", "None", D187), "  Back: ", IF(E187="", "None", E187))</f>
+        <f t="shared" si="22"/>
         <v>Thick, Dark Forest -  Room Exits: N S  Front: sennww  Back: None</v>
       </c>
       <c r="H187" t="str">
-        <f>CONCATENATE("#sub {", F187, "} {", G187, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Thick, Dark Forest%0Exits are: N S} {Thick, Dark Forest -  Room Exits: N S  Front: sennww  Back: None}</v>
       </c>
       <c r="I187" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A187,"} {%0 %1- ",G187, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Thick, Dark Forest} {%0 %1- Thick, Dark Forest -  Room Exits: N S  Front: sennww  Back: None}</v>
       </c>
     </row>
@@ -7278,19 +7282,19 @@
         <v>50</v>
       </c>
       <c r="F188" t="str">
-        <f>CONCATENATE(A188,"%0Exits are: ",C188)</f>
+        <f t="shared" si="21"/>
         <v>Thin Trail On Hill%0Exits are: N E S W</v>
       </c>
       <c r="G188" t="str">
-        <f>CONCATENATE(A188, " -  Room Exits: ", C188, "  Front: ", IF(D188="", "None", D188), "  Back: ", IF(E188="", "None", E188))</f>
+        <f t="shared" si="22"/>
         <v>Thin Trail On Hill -  Room Exits: N E S W  Front: w  Back: nneeseeneenesene</v>
       </c>
       <c r="H188" t="str">
-        <f>CONCATENATE("#sub {", F188, "} {", G188, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Thin Trail On Hill%0Exits are: N E S W} {Thin Trail On Hill -  Room Exits: N E S W  Front: w  Back: nneeseeneenesene}</v>
       </c>
       <c r="I188" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A188,"} {%0 %1- ",G188, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Thin Trail On Hill} {%0 %1- Thin Trail On Hill -  Room Exits: N E S W  Front: w  Back: nneeseeneenesene}</v>
       </c>
     </row>
@@ -7308,19 +7312,19 @@
         <v>197</v>
       </c>
       <c r="F189" t="str">
-        <f>CONCATENATE(A189,"%0Exits are: ",C189)</f>
+        <f t="shared" si="21"/>
         <v>Thundering Darkness%0Exits are: N E S</v>
       </c>
       <c r="G189" t="str">
-        <f>CONCATENATE(A189, " -  Room Exits: ", C189, "  Front: ", IF(D189="", "None", D189), "  Back: ", IF(E189="", "None", E189))</f>
+        <f t="shared" si="22"/>
         <v>Thundering Darkness -  Room Exits: N E S  Front: nssnenw  Back: None</v>
       </c>
       <c r="H189" t="str">
-        <f>CONCATENATE("#sub {", F189, "} {", G189, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Thundering Darkness%0Exits are: N E S} {Thundering Darkness -  Room Exits: N E S  Front: nssnenw  Back: None}</v>
       </c>
       <c r="I189" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A189,"} {%0 %1- ",G189, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Thundering Darkness} {%0 %1- Thundering Darkness -  Room Exits: N E S  Front: nssnenw  Back: None}</v>
       </c>
     </row>
@@ -7338,19 +7342,19 @@
         <v>159</v>
       </c>
       <c r="F190" t="str">
-        <f>CONCATENATE(A190,"%0Exits are: ",C190)</f>
+        <f t="shared" si="21"/>
         <v>Timeless Trees%0Exits are: N S</v>
       </c>
       <c r="G190" t="str">
-        <f>CONCATENATE(A190, " -  Room Exits: ", C190, "  Front: ", IF(D190="", "None", D190), "  Back: ", IF(E190="", "None", E190))</f>
+        <f t="shared" si="22"/>
         <v>Timeless Trees -  Room Exits: N S  Front: snenw  Back: None</v>
       </c>
       <c r="H190" t="str">
-        <f>CONCATENATE("#sub {", F190, "} {", G190, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Timeless Trees%0Exits are: N S} {Timeless Trees -  Room Exits: N S  Front: snenw  Back: None}</v>
       </c>
       <c r="I190" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A190,"} {%0 %1- ",G190, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Timeless Trees} {%0 %1- Timeless Trees -  Room Exits: N S  Front: snenw  Back: None}</v>
       </c>
     </row>
@@ -7368,19 +7372,19 @@
         <v>113</v>
       </c>
       <c r="F191" t="str">
-        <f>CONCATENATE(A191,"%0Exits are: ",C191)</f>
+        <f t="shared" si="21"/>
         <v>Tortured Land%0Exits are: E S</v>
       </c>
       <c r="G191" t="str">
-        <f>CONCATENATE(A191, " -  Room Exits: ", C191, "  Front: ", IF(D191="", "None", D191), "  Back: ", IF(E191="", "None", E191))</f>
+        <f t="shared" si="22"/>
         <v>Tortured Land -  Room Exits: E S  Front: swesew  Back: None</v>
       </c>
       <c r="H191" t="str">
-        <f>CONCATENATE("#sub {", F191, "} {", G191, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Tortured Land%0Exits are: E S} {Tortured Land -  Room Exits: E S  Front: swesew  Back: None}</v>
       </c>
       <c r="I191" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A191,"} {%0 %1- ",G191, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Tortured Land} {%0 %1- Tortured Land -  Room Exits: E S  Front: swesew  Back: None}</v>
       </c>
     </row>
@@ -7398,19 +7402,19 @@
         <v>244</v>
       </c>
       <c r="F192" t="str">
-        <f>CONCATENATE(A192,"%0Exits are: ",C192)</f>
+        <f t="shared" si="21"/>
         <v>Twisted Pines%0Exits are: N E S</v>
       </c>
       <c r="G192" t="str">
-        <f>CONCATENATE(A192, " -  Room Exits: ", C192, "  Front: ", IF(D192="", "None", D192), "  Back: ", IF(E192="", "None", E192))</f>
+        <f t="shared" si="22"/>
         <v>Twisted Pines -  Room Exits: N E S  Front: sssnesw  Back: None</v>
       </c>
       <c r="H192" t="str">
-        <f>CONCATENATE("#sub {", F192, "} {", G192, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Twisted Pines%0Exits are: N E S} {Twisted Pines -  Room Exits: N E S  Front: sssnesw  Back: None}</v>
       </c>
       <c r="I192" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A192,"} {%0 %1- ",G192, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Twisted Pines} {%0 %1- Twisted Pines -  Room Exits: N E S  Front: sssnesw  Back: None}</v>
       </c>
     </row>
@@ -7431,19 +7435,19 @@
         <v>144</v>
       </c>
       <c r="F193" t="str">
-        <f>CONCATENATE(A193,"%0Exits are: ",C193)</f>
+        <f t="shared" si="21"/>
         <v>Twisted Trail%0Exits are: N E W</v>
       </c>
       <c r="G193" t="str">
-        <f>CONCATENATE(A193, " -  Room Exits: ", C193, "  Front: ", IF(D193="", "None", D193), "  Back: ", IF(E193="", "None", E193))</f>
+        <f t="shared" si="22"/>
         <v>Twisted Trail -  Room Exits: N E W  Front: nessnenw  Back: nesene</v>
       </c>
       <c r="H193" t="str">
-        <f>CONCATENATE("#sub {", F193, "} {", G193, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Twisted Trail%0Exits are: N E W} {Twisted Trail -  Room Exits: N E W  Front: nessnenw  Back: nesene}</v>
       </c>
       <c r="I193" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A193,"} {%0 %1- ",G193, "}")</f>
+        <f t="shared" si="23"/>
         <v>#sub {%0 %1- Twisted Trail} {%0 %1- Twisted Trail -  Room Exits: N E W  Front: nessnenw  Back: nesene}</v>
       </c>
     </row>
@@ -7461,19 +7465,19 @@
         <v>83</v>
       </c>
       <c r="F194" t="str">
-        <f>CONCATENATE(A194,"%0Exits are: ",C194)</f>
+        <f t="shared" ref="F194:F199" si="25">CONCATENATE(A194,"%0Exits are: ",C194)</f>
         <v>Unclimbable Cliff%0Exits are: N E S W</v>
       </c>
       <c r="G194" t="str">
-        <f>CONCATENATE(A194, " -  Room Exits: ", C194, "  Front: ", IF(D194="", "None", D194), "  Back: ", IF(E194="", "None", E194))</f>
+        <f t="shared" ref="G194:G199" si="26">CONCATENATE(A194, " -  Room Exits: ", C194, "  Front: ", IF(D194="", "None", D194), "  Back: ", IF(E194="", "None", E194))</f>
         <v>Unclimbable Cliff -  Room Exits: N E S W  Front: swwww  Back: None</v>
       </c>
       <c r="H194" t="str">
-        <f>CONCATENATE("#sub {", F194, "} {", G194, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Unclimbable Cliff%0Exits are: N E S W} {Unclimbable Cliff -  Room Exits: N E S W  Front: swwww  Back: None}</v>
       </c>
       <c r="I194" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A194,"} {%0 %1- ",G194, "}")</f>
+        <f t="shared" ref="I194:I199" si="27">CONCATENATE("#sub {%0 %1- ",A194,"} {%0 %1- ",G194, "}")</f>
         <v>#sub {%0 %1- Unclimbable Cliff} {%0 %1- Unclimbable Cliff -  Room Exits: N E S W  Front: swwww  Back: None}</v>
       </c>
     </row>
@@ -7494,19 +7498,19 @@
         <v>408</v>
       </c>
       <c r="F195" t="str">
-        <f>CONCATENATE(A195,"%0Exits are: ",C195)</f>
+        <f t="shared" si="25"/>
         <v>Unkempt Forest%0Exits are: N S W</v>
       </c>
       <c r="G195" t="str">
-        <f>CONCATENATE(A195, " -  Room Exits: ", C195, "  Front: ", IF(D195="", "None", D195), "  Back: ", IF(E195="", "None", E195))</f>
+        <f t="shared" si="26"/>
         <v>Unkempt Forest -  Room Exits: N S W  Front: nw  Back: nnneeseeneenesene</v>
       </c>
       <c r="H195" t="str">
-        <f>CONCATENATE("#sub {", F195, "} {", G195, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Unkempt Forest%0Exits are: N S W} {Unkempt Forest -  Room Exits: N S W  Front: nw  Back: nnneeseeneenesene}</v>
       </c>
       <c r="I195" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A195,"} {%0 %1- ",G195, "}")</f>
+        <f t="shared" si="27"/>
         <v>#sub {%0 %1- Unkempt Forest} {%0 %1- Unkempt Forest -  Room Exits: N S W  Front: nw  Back: nnneeseeneenesene}</v>
       </c>
     </row>
@@ -7527,19 +7531,19 @@
         <v>136</v>
       </c>
       <c r="F196" t="str">
-        <f>CONCATENATE(A196,"%0Exits are: ",C196)</f>
+        <f t="shared" si="25"/>
         <v>Vigilent Forest%0Exits are: N E W</v>
       </c>
       <c r="G196" t="str">
-        <f>CONCATENATE(A196, " -  Room Exits: ", C196, "  Front: ", IF(D196="", "None", D196), "  Back: ", IF(E196="", "None", E196))</f>
+        <f t="shared" si="26"/>
         <v>Vigilent Forest -  Room Exits: N E W  Front: wennw  Back: neenesene</v>
       </c>
       <c r="H196" t="str">
-        <f>CONCATENATE("#sub {", F196, "} {", G196, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Vigilent Forest%0Exits are: N E W} {Vigilent Forest -  Room Exits: N E W  Front: wennw  Back: neenesene}</v>
       </c>
       <c r="I196" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A196,"} {%0 %1- ",G196, "}")</f>
+        <f t="shared" si="27"/>
         <v>#sub {%0 %1- Vigilent Forest} {%0 %1- Vigilent Forest -  Room Exits: N E W  Front: wennw  Back: neenesene}</v>
       </c>
     </row>
@@ -7557,19 +7561,19 @@
         <v>384</v>
       </c>
       <c r="F197" t="str">
-        <f>CONCATENATE(A197,"%0Exits are: ",C197)</f>
+        <f t="shared" si="25"/>
         <v>Weaving Mists%0Exits are: E S W</v>
       </c>
       <c r="G197" t="str">
-        <f>CONCATENATE(A197, " -  Room Exits: ", C197, "  Front: ", IF(D197="", "None", D197), "  Back: ", IF(E197="", "None", E197))</f>
+        <f t="shared" si="26"/>
         <v>Weaving Mists -  Room Exits: E S W  Front: nsssnesw  Back: None</v>
       </c>
       <c r="H197" t="str">
-        <f>CONCATENATE("#sub {", F197, "} {", G197, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {Weaving Mists%0Exits are: E S W} {Weaving Mists -  Room Exits: E S W  Front: nsssnesw  Back: None}</v>
       </c>
       <c r="I197" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A197,"} {%0 %1- ",G197, "}")</f>
+        <f t="shared" si="27"/>
         <v>#sub {%0 %1- Weaving Mists} {%0 %1- Weaving Mists -  Room Exits: E S W  Front: nsssnesw  Back: None}</v>
       </c>
     </row>
@@ -7587,19 +7591,19 @@
         <v>360</v>
       </c>
       <c r="F198" t="str">
-        <f>CONCATENATE(A198,"%0Exits are: ",C198)</f>
+        <f t="shared" si="25"/>
         <v>West of the Thicket%0Exits are: N W</v>
       </c>
       <c r="G198" t="str">
-        <f>CONCATENATE(A198, " -  Room Exits: ", C198, "  Front: ", IF(D198="", "None", D198), "  Back: ", IF(E198="", "None", E198))</f>
+        <f t="shared" si="26"/>
         <v>West of the Thicket -  Room Exits: N W  Front: nswesew  Back: None</v>
       </c>
       <c r="H198" t="str">
-        <f>CONCATENATE("#sub {", F198, "} {", G198, "}")</f>
+        <f t="shared" si="24"/>
         <v>#sub {West of the Thicket%0Exits are: N W} {West of the Thicket -  Room Exits: N W  Front: nswesew  Back: None}</v>
       </c>
       <c r="I198" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A198,"} {%0 %1- ",G198, "}")</f>
+        <f t="shared" si="27"/>
         <v>#sub {%0 %1- West of the Thicket} {%0 %1- West of the Thicket -  Room Exits: N W  Front: nswesew  Back: None}</v>
       </c>
     </row>
@@ -7617,19 +7621,19 @@
         <v>203</v>
       </c>
       <c r="F199" t="str">
-        <f>CONCATENATE(A199,"%0Exits are: ",C199)</f>
+        <f t="shared" si="25"/>
         <v>Whispering Pines%0Exits are: S W</v>
       </c>
       <c r="G199" t="str">
-        <f>CONCATENATE(A199, " -  Room Exits: ", C199, "  Front: ", IF(D199="", "None", D199), "  Back: ", IF(E199="", "None", E199))</f>
+        <f t="shared" si="26"/>
         <v>Whispering Pines -  Room Exits: S W  Front: wewnesew  Back: None</v>
       </c>
       <c r="H199" t="str">
-        <f>CONCATENATE("#sub {", F199, "} {", G199, "}")</f>
+        <f t="shared" ref="H199:H230" si="28">CONCATENATE("#sub {", F199, "} {", G199, "}")</f>
         <v>#sub {Whispering Pines%0Exits are: S W} {Whispering Pines -  Room Exits: S W  Front: wewnesew  Back: None}</v>
       </c>
       <c r="I199" t="str">
-        <f>CONCATENATE("#sub {%0 %1- ",A199,"} {%0 %1- ",G199, "}")</f>
+        <f t="shared" si="27"/>
         <v>#sub {%0 %1- Whispering Pines} {%0 %1- Whispering Pines -  Room Exits: S W  Front: wewnesew  Back: None}</v>
       </c>
     </row>

</xml_diff>